<commit_message>
Change checker_framework_data from xlsx to csv
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -446,10 +446,10 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>-0.2288200781137409</v>
+        <v>-0.21548035538398</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
Data change after updating parser.py
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -441,7 +441,7 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -470,10 +470,10 @@
         <v>52</v>
       </c>
       <c r="F3">
-        <v>-0.21548035538398</v>
+        <v>-0.03063026539342525</v>
       </c>
       <c r="G3">
-        <v>-0.2722013988321133</v>
+        <v>-0.03818805867014237</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Add more identifier comments to snippets
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -470,10 +470,10 @@
         <v>52</v>
       </c>
       <c r="F3">
-        <v>-0.03063026539342525</v>
+        <v>-0.04665772984347336</v>
       </c>
       <c r="G3">
-        <v>-0.03818805867014237</v>
+        <v>-0.05733362687092258</v>
       </c>
     </row>
     <row r="4" spans="1:7">

</xml_diff>

<commit_message>
Add p-values to correlation analysis
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Complexity Metric</t>
   </si>
@@ -34,7 +34,13 @@
     <t>Kendall's Tau (τ)</t>
   </si>
   <si>
+    <t>Kendall's p-Value</t>
+  </si>
+  <si>
     <t>Spearman's Rho (ρ)</t>
+  </si>
+  <si>
+    <t>Spearman's p-Value</t>
   </si>
   <si>
     <t>Something - COG Dataset 1</t>
@@ -404,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,10 +438,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -450,15 +462,21 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -473,12 +491,18 @@
         <v>-0.2163280190361007</v>
       </c>
       <c r="G3">
+        <v>0.00681274956405711</v>
+      </c>
+      <c r="H3">
         <v>-0.2723771706469902</v>
       </c>
+      <c r="I3">
+        <v>0.00611470670329826</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -490,10 +514,16 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Infer to correlation
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -10,13 +10,14 @@
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
     <sheet name="checker_framework" sheetId="2" r:id="rId2"/>
     <sheet name="typestate_checker" sheetId="3" r:id="rId3"/>
+    <sheet name="infer" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="15">
   <si>
     <t>Complexity Metric</t>
   </si>
@@ -493,22 +494,22 @@
         <v>86</v>
       </c>
       <c r="D3">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
-        <v>-0.1443638401868161</v>
+        <v>-0.03275384325686242</v>
       </c>
       <c r="G3">
-        <v>0.04452351453632922</v>
+        <v>0.6458960401104946</v>
       </c>
       <c r="H3">
-        <v>-0.1962254995564965</v>
+        <v>-0.04216656825659747</v>
       </c>
       <c r="I3">
-        <v>0.05038845563471506</v>
+        <v>0.6770078435983685</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -686,16 +687,16 @@
         <v>100</v>
       </c>
       <c r="F3">
-        <v>-0.2163280190361007</v>
+        <v>-0.1855044244235976</v>
       </c>
       <c r="G3">
-        <v>0.00681274956405711</v>
+        <v>0.02021255303764821</v>
       </c>
       <c r="H3">
-        <v>-0.2723771706469902</v>
+        <v>-0.2319964250630901</v>
       </c>
       <c r="I3">
-        <v>0.00611470670329826</v>
+        <v>0.02020171421364228</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -867,22 +868,22 @@
         <v>84</v>
       </c>
       <c r="D3">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
-        <v>-0.08139940496774911</v>
+        <v>0.002808180844581953</v>
       </c>
       <c r="G3">
-        <v>0.2583817555585647</v>
+        <v>0.9687827959561681</v>
       </c>
       <c r="H3">
-        <v>-0.1103050781934682</v>
+        <v>0.006327541624453262</v>
       </c>
       <c r="I3">
-        <v>0.2746043898034243</v>
+        <v>0.9501801871045381</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -970,6 +971,157 @@
       </c>
       <c r="I6">
         <v>0.1217337691688223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>-0.139855453798248</v>
+      </c>
+      <c r="G3">
+        <v>0.09054763551591515</v>
+      </c>
+      <c r="H3">
+        <v>-0.1701042564652381</v>
+      </c>
+      <c r="I3">
+        <v>0.09064383040289893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganized java src structure
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -491,25 +491,25 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
-        <v>-0.03275384325686242</v>
+        <v>-0.1781295403599469</v>
       </c>
       <c r="G3">
-        <v>0.6458960401104946</v>
+        <v>0.01301652681931669</v>
       </c>
       <c r="H3">
-        <v>-0.04216656825659747</v>
+        <v>-0.2506050579036035</v>
       </c>
       <c r="I3">
-        <v>0.6770078435983685</v>
+        <v>0.01190964758677489</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -687,16 +687,16 @@
         <v>100</v>
       </c>
       <c r="F3">
-        <v>-0.1855044244235976</v>
+        <v>-0.2163280190361007</v>
       </c>
       <c r="G3">
-        <v>0.02021255303764821</v>
+        <v>0.00681274956405711</v>
       </c>
       <c r="H3">
-        <v>-0.2319964250630901</v>
+        <v>-0.2723771706469902</v>
       </c>
       <c r="I3">
-        <v>0.02020171421364228</v>
+        <v>0.00611470670329826</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -865,25 +865,25 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
-        <v>0.002808180844581953</v>
+        <v>-0.1064800639782623</v>
       </c>
       <c r="G3">
-        <v>0.9687827959561681</v>
+        <v>0.1390306358667875</v>
       </c>
       <c r="H3">
-        <v>0.006327541624453262</v>
+        <v>-0.1473585047345789</v>
       </c>
       <c r="I3">
-        <v>0.9501801871045381</v>
+        <v>0.1434514157012983</v>
       </c>
     </row>
     <row r="4" spans="1:9">

</xml_diff>

<commit_message>
Add COG Dataset 2 to pipeline
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FA240E-1006-43C3-8AEE-91AD9E228BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -18,12 +12,12 @@
     <sheet name="typestate_checker" sheetId="3" r:id="rId3"/>
     <sheet name="infer" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
   <si>
     <t>Complexity Metric</t>
   </si>
@@ -59,6 +53,18 @@
   </si>
   <si>
     <t>Rating (4 through 0)  - COG Dataset 1</t>
+  </si>
+  <si>
+    <t>Time - COG Dataset 2</t>
+  </si>
+  <si>
+    <t>Physiological (BA32) - COG Dataset 2</t>
+  </si>
+  <si>
+    <t>Physiological (BA31post) - COG Dataset 2</t>
+  </si>
+  <si>
+    <t>Physiological (BA31ant) - COG Dataset 2</t>
   </si>
   <si>
     <t>Rating (5 through 1) - COG Dataset 3</t>
@@ -76,8 +82,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,14 +146,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -194,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,27 +224,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,24 +258,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,19 +433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -529,19 +486,19 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>9.7198787839491582E-2</v>
+        <v>0.09719878783949158</v>
       </c>
       <c r="G2">
-        <v>0.57290993164184068</v>
+        <v>0.5729099316418407</v>
       </c>
       <c r="H2">
-        <v>0.13606298717832269</v>
+        <v>0.1360629871783227</v>
       </c>
       <c r="I2">
-        <v>0.53589313847232645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.5358931384723264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -558,19 +515,19 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>-9.2668216633232658E-2</v>
+        <v>-0.09266821663323266</v>
       </c>
       <c r="G3">
-        <v>0.59847216676328707</v>
+        <v>0.5984721667632871</v>
       </c>
       <c r="H3">
-        <v>-0.12631636075141109</v>
+        <v>-0.1263163607514111</v>
       </c>
       <c r="I3">
-        <v>0.56575289921057181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.5657528992105718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -587,132 +544,248 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <v>-0.12596964497290161</v>
+        <v>-0.1259696449729016</v>
       </c>
       <c r="G4">
-        <v>0.46796767746816181</v>
+        <v>0.4679676774681618</v>
       </c>
       <c r="H4">
-        <v>-0.17216051139458019</v>
+        <v>-0.1721605113945802</v>
       </c>
       <c r="I4">
-        <v>0.43215989634328322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.4321598963432832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>385</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>-0.17812954035994691</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="G5">
-        <v>1.301652681931669E-2</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="H5">
-        <v>-0.25060505790360349</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="I5">
-        <v>1.190964758677489E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>-0.34953103682127779</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="G6">
-        <v>0.1036923833375111</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="H6">
-        <v>-0.40899089824532692</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="I6">
-        <v>0.11572409682995791</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>-6.3913749070614201E-2</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="G7">
-        <v>0.76385613579207756</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="H7">
-        <v>-8.738275920531946E-2</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="I7">
-        <v>0.74760879513821366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>-0.1113404428537808</v>
+      </c>
+      <c r="G8">
+        <v>0.6639079018776488</v>
+      </c>
+      <c r="H8">
+        <v>-0.131013944022344</v>
+      </c>
+      <c r="I8">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>88</v>
+      </c>
+      <c r="D9">
+        <v>388</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>-0.1939581840402086</v>
+      </c>
+      <c r="G9">
+        <v>0.006863249574703261</v>
+      </c>
+      <c r="H9">
+        <v>-0.2761573958744979</v>
+      </c>
+      <c r="I9">
+        <v>0.005416589176637902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>0.33374500859622358</v>
-      </c>
-      <c r="G8">
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>-0.3495310368212778</v>
+      </c>
+      <c r="G10">
+        <v>0.1036923833375111</v>
+      </c>
+      <c r="H10">
+        <v>-0.4089908982453269</v>
+      </c>
+      <c r="I10">
+        <v>0.1157240968299579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>-0.0639137490706142</v>
+      </c>
+      <c r="G11">
+        <v>0.7638561357920776</v>
+      </c>
+      <c r="H11">
+        <v>-0.08738275920531946</v>
+      </c>
+      <c r="I11">
+        <v>0.7476087951382137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>0.3337450085962236</v>
+      </c>
+      <c r="G12">
         <v>0.117961265079868</v>
       </c>
-      <c r="H8">
-        <v>0.39351186984290798</v>
-      </c>
-      <c r="I8">
-        <v>0.13155914944413771</v>
+      <c r="H12">
+        <v>0.393511869842908</v>
+      </c>
+      <c r="I12">
+        <v>0.1315591494441377</v>
       </c>
     </row>
   </sheetData>
@@ -721,19 +794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,7 +830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -782,16 +850,16 @@
         <v>0.2297034206521828</v>
       </c>
       <c r="G2">
-        <v>0.18729084163390899</v>
+        <v>0.187290841633909</v>
       </c>
       <c r="H2">
-        <v>0.28096954242303013</v>
+        <v>0.2809695424230301</v>
       </c>
       <c r="I2">
-        <v>0.19405167261558409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1940516726155841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -811,16 +879,16 @@
         <v>-0.2277100170213244</v>
       </c>
       <c r="G3">
-        <v>0.20032802218695259</v>
+        <v>0.2003280221869526</v>
       </c>
       <c r="H3">
-        <v>-0.27197235029387162</v>
+        <v>-0.2719723502938716</v>
       </c>
       <c r="I3">
-        <v>0.20932509565963231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.2093250956596323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -837,132 +905,200 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <v>-0.26347777762091701</v>
+        <v>-0.263477777620917</v>
       </c>
       <c r="G4">
         <v>0.1329850671160174</v>
       </c>
       <c r="H4">
-        <v>-0.32017787305285961</v>
+        <v>-0.3201778730528596</v>
       </c>
       <c r="I4">
-        <v>0.13637641008504059</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1363764100850406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>-0.21632801903610069</v>
-      </c>
-      <c r="G5">
-        <v>6.8127495640571099E-3</v>
-      </c>
-      <c r="H5">
-        <v>-0.27237717064699019</v>
-      </c>
-      <c r="I5">
-        <v>6.11470670329826E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>-0.16284238361758671</v>
-      </c>
-      <c r="G6">
-        <v>0.45801098838521898</v>
-      </c>
-      <c r="H6">
-        <v>-0.19161611347062391</v>
-      </c>
-      <c r="I6">
-        <v>0.4771333722542902</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>-0.24849977213699159</v>
-      </c>
-      <c r="G7">
-        <v>0.25281290101640808</v>
-      </c>
-      <c r="H7">
-        <v>-0.29526172657404681</v>
-      </c>
-      <c r="I7">
-        <v>0.26690125229506823</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>0.27889955205754868</v>
-      </c>
-      <c r="G8">
-        <v>0.20089032653971309</v>
-      </c>
-      <c r="H8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>51</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>-0.2163280190361007</v>
+      </c>
+      <c r="G9">
+        <v>0.00681274956405711</v>
+      </c>
+      <c r="H9">
+        <v>-0.2723771706469902</v>
+      </c>
+      <c r="I9">
+        <v>0.00611470670329826</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>-0.1628423836175867</v>
+      </c>
+      <c r="G10">
+        <v>0.458010988385219</v>
+      </c>
+      <c r="H10">
+        <v>-0.1916161134706239</v>
+      </c>
+      <c r="I10">
+        <v>0.4771333722542902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>-0.2484997721369916</v>
+      </c>
+      <c r="G11">
+        <v>0.2528129010164081</v>
+      </c>
+      <c r="H11">
+        <v>-0.2952617265740468</v>
+      </c>
+      <c r="I11">
+        <v>0.2669012522950682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>0.2788995520575487</v>
+      </c>
+      <c r="G12">
+        <v>0.2008903265397131</v>
+      </c>
+      <c r="H12">
         <v>0.3302413141237342</v>
       </c>
-      <c r="I8">
-        <v>0.21158246186830859</v>
+      <c r="I12">
+        <v>0.2115824618683086</v>
       </c>
     </row>
   </sheetData>
@@ -971,16 +1107,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1029,16 +1163,16 @@
         <v>0.182178575000007</v>
       </c>
       <c r="G2">
-        <v>0.29564657602090749</v>
+        <v>0.2956465760209075</v>
       </c>
       <c r="H2">
-        <v>0.24046942819989059</v>
+        <v>0.2404694281998906</v>
       </c>
       <c r="I2">
-        <v>0.26904897632032188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.2690489763203219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1055,19 +1189,19 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>-0.17078251276599329</v>
+        <v>-0.1707825127659933</v>
       </c>
       <c r="G3">
         <v>0.3368221511559395</v>
       </c>
       <c r="H3">
-        <v>-0.22063279587022341</v>
+        <v>-0.2206327958702234</v>
       </c>
       <c r="I3">
-        <v>0.31170668319455619</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3117066831945562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1084,131 +1218,247 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <v>-0.21557272714438661</v>
+        <v>-0.2155727271443866</v>
       </c>
       <c r="G4">
         <v>0.2189727791934982</v>
       </c>
       <c r="H4">
-        <v>-0.28300682710477038</v>
+        <v>-0.2830068271047704</v>
       </c>
       <c r="I4">
-        <v>0.19070138371258061</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1907013837125806</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>318</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>-0.1064800639782623</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="G5">
-        <v>0.13903063586678749</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="H5">
-        <v>-0.1473585047345789</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="I5">
-        <v>0.1434514157012983</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>-0.49785866253711791</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="G6">
-        <v>2.1337320545634531E-2</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="H6">
-        <v>-0.57692307692307687</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="I6">
-        <v>1.929785020805572E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>-1.6951587590520258E-2</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="G7">
-        <v>0.93692172809769891</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="H7">
-        <v>-3.8348249442368518E-2</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="I7">
-        <v>0.88786930283188992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>-0.1113404428537808</v>
+      </c>
+      <c r="G8">
+        <v>0.6639079018776488</v>
+      </c>
+      <c r="H8">
+        <v>-0.131013944022344</v>
+      </c>
+      <c r="I8">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>86</v>
+      </c>
+      <c r="D9">
+        <v>321</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>-0.1247544764623047</v>
+      </c>
+      <c r="G9">
+        <v>0.08311989853557726</v>
+      </c>
+      <c r="H9">
+        <v>-0.1750549250837969</v>
+      </c>
+      <c r="I9">
+        <v>0.08150516687294729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>0.34045327482409782</v>
-      </c>
-      <c r="G8">
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>-0.4978586625371179</v>
+      </c>
+      <c r="G10">
+        <v>0.02133732054563453</v>
+      </c>
+      <c r="H10">
+        <v>-0.5769230769230769</v>
+      </c>
+      <c r="I10">
+        <v>0.01929785020805572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>-0.01695158759052026</v>
+      </c>
+      <c r="G11">
+        <v>0.9369217280976989</v>
+      </c>
+      <c r="H11">
+        <v>-0.03834824944236852</v>
+      </c>
+      <c r="I11">
+        <v>0.8878693028318899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>0.3404532748240978</v>
+      </c>
+      <c r="G12">
         <v>0.1131965364706231</v>
       </c>
-      <c r="H8">
-        <v>0.40295301713800152</v>
-      </c>
-      <c r="I8">
+      <c r="H12">
+        <v>0.4029530171380015</v>
+      </c>
+      <c r="I12">
         <v>0.1217337691688223</v>
       </c>
     </row>
@@ -1218,16 +1468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1290,7 +1538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1307,41 +1555,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>-0.13985545379824799</v>
-      </c>
-      <c r="G5">
-        <v>9.0547635515915145E-2</v>
-      </c>
-      <c r="H5">
-        <v>-0.17010425646523811</v>
-      </c>
-      <c r="I5">
-        <v>9.0643830402898931E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1350,15 +1586,15 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1367,15 +1603,15 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1384,6 +1620,86 @@
         <v>0</v>
       </c>
       <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>-0.139855453798248</v>
+      </c>
+      <c r="G9">
+        <v>0.09054763551591515</v>
+      </c>
+      <c r="H9">
+        <v>-0.1701042564652381</v>
+      </c>
+      <c r="I9">
+        <v>0.09064383040289893</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create bash script for JBMC.
Note: Doesn't work on all snippets yet. Some need an entry point.
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -718,7 +718,7 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>192</v>
@@ -747,7 +747,7 @@
         <v>50</v>
       </c>
       <c r="C11">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>192</v>
@@ -776,7 +776,7 @@
         <v>50</v>
       </c>
       <c r="C12">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>192</v>
@@ -1939,16 +1939,16 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>-0.2513580286171832</v>
+        <v>-0.2465459984594313</v>
       </c>
       <c r="G10">
-        <v>0.03054279092665989</v>
+        <v>0.03317524973370743</v>
       </c>
       <c r="H10">
-        <v>-0.3106508608887624</v>
+        <v>-0.3098303775675377</v>
       </c>
       <c r="I10">
-        <v>0.02811234624135277</v>
+        <v>0.02855238451552488</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1968,16 +1968,16 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>-0.02644542653481615</v>
+        <v>-0.02257043088830945</v>
       </c>
       <c r="G11">
-        <v>0.8211283092369018</v>
+        <v>0.8463887047098356</v>
       </c>
       <c r="H11">
-        <v>-0.02889232075369115</v>
+        <v>-0.02588543710805493</v>
       </c>
       <c r="I11">
-        <v>0.8421268384730887</v>
+        <v>0.8583790451496913</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1997,16 +1997,16 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>-0.008002176888210664</v>
+        <v>-0.007967906165899995</v>
       </c>
       <c r="G12">
-        <v>0.9479027969797296</v>
+        <v>0.9479195406770614</v>
       </c>
       <c r="H12">
-        <v>-0.008309173651488432</v>
+        <v>-0.007746944922644224</v>
       </c>
       <c r="I12">
-        <v>0.9543304334608099</v>
+        <v>0.9574176555277638</v>
       </c>
     </row>
     <row r="13" spans="1:9">

</xml_diff>

<commit_message>
Fix CF Memory Issue
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -498,25 +498,25 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>23</v>
       </c>
       <c r="F2">
-        <v>0.182178575000007</v>
+        <v>0.09719878783949158</v>
       </c>
       <c r="G2">
-        <v>0.2956465760209075</v>
+        <v>0.5729099316418407</v>
       </c>
       <c r="H2">
-        <v>0.2404694281998906</v>
+        <v>0.1360629871783227</v>
       </c>
       <c r="I2">
-        <v>0.2690489763203219</v>
+        <v>0.5358931384723264</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -527,25 +527,25 @@
         <v>23</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>23</v>
       </c>
       <c r="F3">
-        <v>-0.1707825127659933</v>
+        <v>-0.09266821663323266</v>
       </c>
       <c r="G3">
-        <v>0.3368221511559395</v>
+        <v>0.5984721667632871</v>
       </c>
       <c r="H3">
-        <v>-0.2206327958702234</v>
+        <v>-0.1263163607514111</v>
       </c>
       <c r="I3">
-        <v>0.3117066831945562</v>
+        <v>0.5657528992105718</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -556,25 +556,25 @@
         <v>23</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>23</v>
       </c>
       <c r="F4">
-        <v>-0.2155727271443866</v>
+        <v>-0.1259696449729016</v>
       </c>
       <c r="G4">
-        <v>0.2189727791934982</v>
+        <v>0.4679676774681618</v>
       </c>
       <c r="H4">
-        <v>-0.2830068271047704</v>
+        <v>-0.1721605113945802</v>
       </c>
       <c r="I4">
-        <v>0.1907013837125806</v>
+        <v>0.4321598963432832</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -704,22 +704,22 @@
         <v>90</v>
       </c>
       <c r="D9">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>-0.2247660100928766</v>
+        <v>-0.2278622001693345</v>
       </c>
       <c r="G9">
-        <v>0.001764582967150859</v>
+        <v>0.001503036931867509</v>
       </c>
       <c r="H9">
-        <v>-0.3198917635397611</v>
+        <v>-0.3234568550885335</v>
       </c>
       <c r="I9">
-        <v>0.001177004266505542</v>
+        <v>0.0010284898212685</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -820,22 +820,22 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>30</v>
       </c>
       <c r="F13">
-        <v>-0.08428239551583107</v>
+        <v>-0.1130105839368017</v>
       </c>
       <c r="G13">
-        <v>0.5573926619420599</v>
+        <v>0.4404006981390032</v>
       </c>
       <c r="H13">
-        <v>-0.1042936484359613</v>
+        <v>-0.1377826417184593</v>
       </c>
       <c r="I13">
-        <v>0.5833716951885439</v>
+        <v>0.4677936200616143</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -849,22 +849,22 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>30</v>
       </c>
       <c r="F14">
-        <v>0.02177533914355364</v>
+        <v>-0.1668825406867738</v>
       </c>
       <c r="G14">
-        <v>0.8796360025154407</v>
+        <v>0.2550672974746294</v>
       </c>
       <c r="H14">
-        <v>0.01538737380554546</v>
+        <v>-0.2023907691537807</v>
       </c>
       <c r="I14">
-        <v>0.9356777338988833</v>
+        <v>0.2834571786891915</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -878,22 +878,22 @@
         <v>18</v>
       </c>
       <c r="D15">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>30</v>
       </c>
       <c r="F15">
-        <v>0.5138507339513572</v>
+        <v>0.5876550364713691</v>
       </c>
       <c r="G15">
-        <v>0.0003474388616958172</v>
+        <v>6.023530742288514E-05</v>
       </c>
       <c r="H15">
-        <v>0.6847206873667281</v>
+        <v>0.7491931143441224</v>
       </c>
       <c r="I15">
-        <v>2.998737859074545E-05</v>
+        <v>1.904021591222836E-06</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -907,22 +907,22 @@
         <v>18</v>
       </c>
       <c r="D16">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
       <c r="F16">
-        <v>0.5138507339513572</v>
+        <v>0.5876550364713691</v>
       </c>
       <c r="G16">
-        <v>0.0003474388616958172</v>
+        <v>6.023530742288514E-05</v>
       </c>
       <c r="H16">
-        <v>0.6847206873667281</v>
+        <v>0.7491931143441224</v>
       </c>
       <c r="I16">
-        <v>2.998737859074545E-05</v>
+        <v>1.904021591222836E-06</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1062,13 +1062,25 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>23</v>
+      </c>
+      <c r="F2">
+        <v>0.2297034206521828</v>
+      </c>
+      <c r="G2">
+        <v>0.187290841633909</v>
+      </c>
+      <c r="H2">
+        <v>0.2809695424230301</v>
+      </c>
+      <c r="I2">
+        <v>0.1940516726155841</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1079,13 +1091,25 @@
         <v>23</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>23</v>
+      </c>
+      <c r="F3">
+        <v>-0.2277100170213244</v>
+      </c>
+      <c r="G3">
+        <v>0.2003280221869526</v>
+      </c>
+      <c r="H3">
+        <v>-0.2719723502938716</v>
+      </c>
+      <c r="I3">
+        <v>0.2093250956596323</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1096,13 +1120,25 @@
         <v>23</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>23</v>
+      </c>
+      <c r="F4">
+        <v>-0.263477777620917</v>
+      </c>
+      <c r="G4">
+        <v>0.1329850671160174</v>
+      </c>
+      <c r="H4">
+        <v>-0.3201778730528596</v>
+      </c>
+      <c r="I4">
+        <v>0.1363764100850406</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1181,25 +1217,25 @@
         <v>100</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>-0.2077746871466997</v>
+        <v>-0.2289041597670328</v>
       </c>
       <c r="G9">
-        <v>0.009352982100299357</v>
+        <v>0.004154062204876697</v>
       </c>
       <c r="H9">
-        <v>-0.2604109502335396</v>
+        <v>-0.2872671746617843</v>
       </c>
       <c r="I9">
-        <v>0.008878948824661271</v>
+        <v>0.003756720549751365</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1297,25 +1333,25 @@
         <v>30</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <v>30</v>
       </c>
       <c r="F13">
-        <v>0.009546929107576048</v>
+        <v>-0.06524669105718928</v>
       </c>
       <c r="G13">
-        <v>0.9493645325968086</v>
+        <v>0.6720517686591893</v>
       </c>
       <c r="H13">
-        <v>0.004196479702249133</v>
+        <v>-0.07861110510609637</v>
       </c>
       <c r="I13">
-        <v>0.982441223262396</v>
+        <v>0.679668768010645</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1326,25 +1362,25 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>30</v>
       </c>
       <c r="F14">
-        <v>-0.01274389539389715</v>
+        <v>-0.153506269493634</v>
       </c>
       <c r="G14">
-        <v>0.9325134307836964</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="H14">
-        <v>-0.02583745234823027</v>
+        <v>-0.1847566494939108</v>
       </c>
       <c r="I14">
-        <v>0.8921955158667667</v>
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1355,25 +1391,25 @@
         <v>30</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>30</v>
       </c>
       <c r="F15">
-        <v>0.3723302351954658</v>
+        <v>0.443677499188887</v>
       </c>
       <c r="G15">
-        <v>0.01326079811977314</v>
+        <v>0.003993565524162987</v>
       </c>
       <c r="H15">
-        <v>0.4450891284197987</v>
+        <v>0.5345555147214552</v>
       </c>
       <c r="I15">
-        <v>0.0137155505697057</v>
+        <v>0.002341385142708154</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1384,25 +1420,25 @@
         <v>30</v>
       </c>
       <c r="C16">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
       <c r="F16">
-        <v>0.3723302351954658</v>
+        <v>0.443677499188887</v>
       </c>
       <c r="G16">
-        <v>0.01326079811977314</v>
+        <v>0.003993565524162987</v>
       </c>
       <c r="H16">
-        <v>0.4450891284197987</v>
+        <v>0.5345555147214552</v>
       </c>
       <c r="I16">
-        <v>0.0137155505697057</v>
+        <v>0.002341385142708154</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2293,7 +2329,7 @@
         <v>30</v>
       </c>
       <c r="C13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>18</v>
@@ -2302,16 +2338,16 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>-0.06040669802439581</v>
+        <v>-0.1435427203258164</v>
       </c>
       <c r="G13">
-        <v>0.6875732300778175</v>
+        <v>0.3516806827985527</v>
       </c>
       <c r="H13">
-        <v>-0.0876988331331129</v>
+        <v>-0.172944431233412</v>
       </c>
       <c r="I13">
-        <v>0.6449239596498875</v>
+        <v>0.360759748541673</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2322,7 +2358,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>18</v>
@@ -2331,16 +2367,16 @@
         <v>30</v>
       </c>
       <c r="F14">
-        <v>0.01209525019049433</v>
+        <v>-0.153506269493634</v>
       </c>
       <c r="G14">
-        <v>0.9358876871208994</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="H14">
-        <v>0.01096357373936683</v>
+        <v>-0.1847566494939108</v>
       </c>
       <c r="I14">
-        <v>0.9541469485685775</v>
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2351,7 +2387,7 @@
         <v>30</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15">
         <v>18</v>
@@ -2360,16 +2396,16 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <v>0.5255382728122435</v>
+        <v>0.6916149252062063</v>
       </c>
       <c r="G15">
-        <v>0.0004675150984229676</v>
+        <v>7.211867226751588E-06</v>
       </c>
       <c r="H15">
-        <v>0.6398028508120283</v>
+        <v>0.8332777141246215</v>
       </c>
       <c r="I15">
-        <v>0.0001406507422922937</v>
+        <v>1.098076308139691E-08</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2380,7 +2416,7 @@
         <v>30</v>
       </c>
       <c r="C16">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>18</v>
@@ -2389,16 +2425,16 @@
         <v>30</v>
       </c>
       <c r="F16">
-        <v>0.5255382728122435</v>
+        <v>0.6916149252062063</v>
       </c>
       <c r="G16">
-        <v>0.0004675150984229676</v>
+        <v>7.211867226751588E-06</v>
       </c>
       <c r="H16">
-        <v>0.6398028508120283</v>
+        <v>0.8332777141246215</v>
       </c>
       <c r="I16">
-        <v>0.0001406507422922937</v>
+        <v>1.098076308139691E-08</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>

<commit_message>
Updates to datasets 3 for JPF
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="30">
   <si>
     <t>Complexity Metric</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Spearman's p-Value</t>
   </si>
   <si>
+    <t>Higher/Lower</t>
+  </si>
+  <si>
     <t>Time (in sec.) - COG Dataset 1</t>
   </si>
   <si>
@@ -98,6 +101,12 @@
   </si>
   <si>
     <t>Rating (readability low, med, high) - fMRI Dataset</t>
+  </si>
+  <si>
+    <t>Higher</t>
+  </si>
+  <si>
+    <t>Lower</t>
   </si>
 </sst>
 </file>
@@ -455,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +498,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -518,10 +530,13 @@
       <c r="I2">
         <v>0.5358931384723264</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -547,10 +562,13 @@
       <c r="I3">
         <v>0.5657528992105718</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -576,10 +594,13 @@
       <c r="I4">
         <v>0.4321598963432832</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -605,10 +626,13 @@
       <c r="I5">
         <v>0.3338931364506602</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -635,9 +659,9 @@
         <v>0.6848487144273757</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -664,9 +688,9 @@
         <v>0.3338931364506602</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -693,9 +717,9 @@
         <v>0.6848487144273757</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -704,27 +728,30 @@
         <v>90</v>
       </c>
       <c r="D9">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>-0.2278622001693345</v>
+        <v>-0.2296446241402438</v>
       </c>
       <c r="G9">
-        <v>0.001503036931867509</v>
+        <v>0.001381085952098848</v>
       </c>
       <c r="H9">
-        <v>-0.3234568550885335</v>
+        <v>-0.3250508508876161</v>
       </c>
       <c r="I9">
-        <v>0.0010284898212685</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.0009677863595653327</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -750,10 +777,13 @@
       <c r="I10">
         <v>0.02797470554846711</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -779,10 +809,13 @@
       <c r="I11">
         <v>0.8406889719449382</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -808,10 +841,13 @@
       <c r="I12">
         <v>0.8701989009134035</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -837,10 +873,13 @@
       <c r="I13">
         <v>0.4677936200616143</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -866,10 +905,13 @@
       <c r="I14">
         <v>0.2834571786891915</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -895,10 +937,13 @@
       <c r="I15">
         <v>1.904021591222836E-06</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -924,10 +969,13 @@
       <c r="I16">
         <v>1.904021591222836E-06</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -953,10 +1001,13 @@
       <c r="I17">
         <v>0.1157240968299579</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -982,10 +1033,13 @@
       <c r="I18">
         <v>0.7476087951382137</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -1010,6 +1064,9 @@
       </c>
       <c r="I19">
         <v>0.1315591494441377</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1019,13 +1076,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,10 +1110,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -1082,10 +1142,13 @@
       <c r="I2">
         <v>0.1940516726155841</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -1111,10 +1174,13 @@
       <c r="I3">
         <v>0.2093250956596323</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -1140,10 +1206,13 @@
       <c r="I4">
         <v>0.1363764100850406</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1157,10 +1226,13 @@
       <c r="E5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1175,9 +1247,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -1192,9 +1264,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1209,9 +1281,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -1237,10 +1309,13 @@
       <c r="I9">
         <v>0.003756720549751365</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -1266,10 +1341,13 @@
       <c r="I10">
         <v>0.02748882596687927</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -1295,10 +1373,13 @@
       <c r="I11">
         <v>0.8466646412386398</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -1324,10 +1405,13 @@
       <c r="I12">
         <v>0.8808493755591094</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -1353,10 +1437,13 @@
       <c r="I13">
         <v>0.679668768010645</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1382,10 +1469,13 @@
       <c r="I14">
         <v>0.328369658424491</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -1411,10 +1501,13 @@
       <c r="I15">
         <v>0.002341385142708154</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -1440,10 +1533,13 @@
       <c r="I16">
         <v>0.002341385142708154</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1469,10 +1565,13 @@
       <c r="I17">
         <v>0.4771333722542902</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -1498,10 +1597,13 @@
       <c r="I18">
         <v>0.2669012522950682</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -1526,6 +1628,9 @@
       </c>
       <c r="I19">
         <v>0.2115824618683086</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1535,13 +1640,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,10 +1674,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -1598,10 +1706,13 @@
       <c r="I2">
         <v>0.2690489763203219</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -1627,10 +1738,13 @@
       <c r="I3">
         <v>0.3117066831945562</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -1656,10 +1770,13 @@
       <c r="I4">
         <v>0.1907013837125806</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1685,10 +1802,13 @@
       <c r="I5">
         <v>0.3338931364506602</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1715,9 +1835,9 @@
         <v>0.6848487144273757</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -1744,9 +1864,9 @@
         <v>0.3338931364506602</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1773,9 +1893,9 @@
         <v>0.6848487144273757</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -1801,10 +1921,13 @@
       <c r="I9">
         <v>0.0276105659239954</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -1830,10 +1953,13 @@
       <c r="I10">
         <v>0.4725395318267059</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -1859,10 +1985,13 @@
       <c r="I11">
         <v>0.5381698827874621</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -1888,10 +2017,13 @@
       <c r="I12">
         <v>0.3313563853369854</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -1905,10 +2037,13 @@
       <c r="E13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1922,10 +2057,13 @@
       <c r="E14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -1939,10 +2077,13 @@
       <c r="E15">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -1956,10 +2097,13 @@
       <c r="E16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1985,10 +2129,13 @@
       <c r="I17">
         <v>0.01929785020805572</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -2014,10 +2161,13 @@
       <c r="I18">
         <v>0.8878693028318899</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -2042,6 +2192,9 @@
       </c>
       <c r="I19">
         <v>0.1217337691688223</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2051,13 +2204,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2085,10 +2238,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -2102,10 +2258,13 @@
       <c r="E2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -2119,10 +2278,13 @@
       <c r="E3">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -2136,10 +2298,13 @@
       <c r="E4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -2153,10 +2318,13 @@
       <c r="E5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -2171,9 +2339,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -2188,9 +2356,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -2205,38 +2373,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>-0.139855453798248</v>
+        <v>-0.1325530043077417</v>
       </c>
       <c r="G9">
-        <v>0.09054763551591515</v>
+        <v>0.1086826442074059</v>
       </c>
       <c r="H9">
-        <v>-0.1701042564652381</v>
+        <v>-0.1612223880273475</v>
       </c>
       <c r="I9">
-        <v>0.09064383040289893</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.1090548020620709</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -2262,10 +2433,13 @@
       <c r="I10">
         <v>0.02804344582260457</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -2291,10 +2465,13 @@
       <c r="I11">
         <v>0.8718796181740638</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -2320,10 +2497,13 @@
       <c r="I12">
         <v>0.8935368700981905</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -2349,10 +2529,13 @@
       <c r="I13">
         <v>0.360759748541673</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -2378,10 +2561,13 @@
       <c r="I14">
         <v>0.328369658424491</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -2407,10 +2593,13 @@
       <c r="I15">
         <v>1.098076308139691E-08</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -2436,10 +2625,13 @@
       <c r="I16">
         <v>1.098076308139691E-08</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -2453,10 +2645,13 @@
       <c r="E17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -2470,10 +2665,13 @@
       <c r="E18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -2486,6 +2684,9 @@
       </c>
       <c r="E19">
         <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed column widths on results sheet
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -484,6 +484,20 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -1219,6 +1233,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -1906,6 +1934,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -2593,6 +2635,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Fixed order of rows in results sheet
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -563,16 +563,16 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>0.09719878783949158</v>
+        <v>-0.09266821663323266</v>
       </c>
       <c r="J2">
-        <v>0.5729099316418407</v>
+        <v>0.5984721667632871</v>
       </c>
       <c r="K2">
-        <v>0.1360629871783227</v>
+        <v>-0.1263163607514111</v>
       </c>
       <c r="L2">
-        <v>0.5358931384723264</v>
+        <v>0.5657528992105718</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -601,16 +601,16 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.09266821663323266</v>
+        <v>-0.1259696449729016</v>
       </c>
       <c r="J3">
-        <v>0.5984721667632871</v>
+        <v>0.4679676774681618</v>
       </c>
       <c r="K3">
-        <v>-0.1263163607514111</v>
+        <v>-0.1721605113945802</v>
       </c>
       <c r="L3">
-        <v>0.5657528992105718</v>
+        <v>0.4321598963432832</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -639,16 +639,16 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>-0.1259696449729016</v>
+        <v>0.09719878783949158</v>
       </c>
       <c r="J4">
-        <v>0.4679676774681618</v>
+        <v>0.5729099316418407</v>
       </c>
       <c r="K4">
-        <v>-0.1721605113945802</v>
+        <v>0.1360629871783227</v>
       </c>
       <c r="L4">
-        <v>0.4321598963432832</v>
+        <v>0.5358931384723264</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -677,16 +677,16 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.2597943666588219</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J5">
-        <v>0.3106354563374008</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.3056992027188027</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L5">
-        <v>0.3338931364506602</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -715,16 +715,16 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>0.1113404428537808</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J6">
-        <v>0.6639079018776488</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K6">
-        <v>0.131013944022344</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L6">
-        <v>0.6848487144273757</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -753,16 +753,16 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.2597943666588219</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J7">
-        <v>0.3106354563374008</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K7">
-        <v>-0.3056992027188027</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L7">
-        <v>0.3338931364506602</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -791,16 +791,16 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.1113404428537808</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J8">
-        <v>0.6639079018776488</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K8">
-        <v>-0.131013944022344</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L8">
-        <v>0.6848487144273757</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -867,16 +867,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.247884667760308</v>
+        <v>-0.02815294687312959</v>
       </c>
       <c r="J10">
-        <v>0.03188792894690582</v>
+        <v>0.8086800956106934</v>
       </c>
       <c r="K10">
-        <v>-0.3109097018922294</v>
+        <v>-0.02915890758270907</v>
       </c>
       <c r="L10">
-        <v>0.02797470554846711</v>
+        <v>0.8406889719449382</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -905,16 +905,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-0.02186507152633387</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.8574604535784878</v>
       </c>
       <c r="K11">
-        <v>-0.02915890758270907</v>
+        <v>-0.0237054182352517</v>
       </c>
       <c r="L11">
-        <v>0.8406889719449382</v>
+        <v>0.8701989009134035</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -943,16 +943,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.02186507152633387</v>
+        <v>-0.247884667760308</v>
       </c>
       <c r="J12">
-        <v>0.8574604535784878</v>
+        <v>0.03188792894690582</v>
       </c>
       <c r="K12">
-        <v>-0.0237054182352517</v>
+        <v>-0.3109097018922294</v>
       </c>
       <c r="L12">
-        <v>0.8701989009134035</v>
+        <v>0.02797470554846711</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -981,16 +981,16 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.1130105839368017</v>
+        <v>-0.1668825406867738</v>
       </c>
       <c r="J13">
-        <v>0.4404006981390032</v>
+        <v>0.2550672974746294</v>
       </c>
       <c r="K13">
-        <v>-0.1377826417184593</v>
+        <v>-0.2023907691537807</v>
       </c>
       <c r="L13">
-        <v>0.4677936200616143</v>
+        <v>0.2834571786891915</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1019,16 +1019,16 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>-0.1668825406867738</v>
+        <v>0.5876550364713691</v>
       </c>
       <c r="J14">
-        <v>0.2550672974746294</v>
+        <v>6.023530742288514E-05</v>
       </c>
       <c r="K14">
-        <v>-0.2023907691537807</v>
+        <v>0.7491931143441224</v>
       </c>
       <c r="L14">
-        <v>0.2834571786891915</v>
+        <v>1.904021591222836E-06</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1095,16 +1095,16 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>0.5876550364713691</v>
+        <v>-0.1130105839368017</v>
       </c>
       <c r="J16">
-        <v>6.023530742288514E-05</v>
+        <v>0.4404006981390032</v>
       </c>
       <c r="K16">
-        <v>0.7491931143441224</v>
+        <v>-0.1377826417184593</v>
       </c>
       <c r="L16">
-        <v>1.904021591222836E-06</v>
+        <v>0.4677936200616143</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1171,16 +1171,16 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.0639137490706142</v>
+        <v>0.3337450085962236</v>
       </c>
       <c r="J18">
-        <v>0.7638561357920776</v>
+        <v>0.117961265079868</v>
       </c>
       <c r="K18">
-        <v>-0.08738275920531946</v>
+        <v>0.393511869842908</v>
       </c>
       <c r="L18">
-        <v>0.7476087951382137</v>
+        <v>0.1315591494441377</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1209,16 +1209,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.3337450085962236</v>
+        <v>-0.0639137490706142</v>
       </c>
       <c r="J19">
-        <v>0.117961265079868</v>
+        <v>0.7638561357920776</v>
       </c>
       <c r="K19">
-        <v>0.393511869842908</v>
+        <v>-0.08738275920531946</v>
       </c>
       <c r="L19">
-        <v>0.1315591494441377</v>
+        <v>0.7476087951382137</v>
       </c>
     </row>
   </sheetData>
@@ -1312,16 +1312,16 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>0.2297034206521828</v>
+        <v>-0.2277100170213244</v>
       </c>
       <c r="J2">
-        <v>0.187290841633909</v>
+        <v>0.2003280221869526</v>
       </c>
       <c r="K2">
-        <v>0.2809695424230301</v>
+        <v>-0.2719723502938716</v>
       </c>
       <c r="L2">
-        <v>0.1940516726155841</v>
+        <v>0.2093250956596323</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1350,16 +1350,16 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.2277100170213244</v>
+        <v>-0.263477777620917</v>
       </c>
       <c r="J3">
-        <v>0.2003280221869526</v>
+        <v>0.1329850671160174</v>
       </c>
       <c r="K3">
-        <v>-0.2719723502938716</v>
+        <v>-0.3201778730528596</v>
       </c>
       <c r="L3">
-        <v>0.2093250956596323</v>
+        <v>0.1363764100850406</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1388,16 +1388,16 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>-0.263477777620917</v>
+        <v>0.2297034206521828</v>
       </c>
       <c r="J4">
-        <v>0.1329850671160174</v>
+        <v>0.187290841633909</v>
       </c>
       <c r="K4">
-        <v>-0.3201778730528596</v>
+        <v>0.2809695424230301</v>
       </c>
       <c r="L4">
-        <v>0.1363764100850406</v>
+        <v>0.1940516726155841</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1568,16 +1568,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.2516122567491849</v>
+        <v>-0.02439922062337898</v>
       </c>
       <c r="J10">
-        <v>0.02940004335865699</v>
+        <v>0.8337884478927275</v>
       </c>
       <c r="K10">
-        <v>-0.3118320089283974</v>
+        <v>-0.02805160729475809</v>
       </c>
       <c r="L10">
-        <v>0.02748882596687927</v>
+        <v>0.8466646412386398</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1606,16 +1606,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K11">
-        <v>-0.02805160729475809</v>
+        <v>-0.02174552145202223</v>
       </c>
       <c r="L11">
-        <v>0.8466646412386398</v>
+        <v>0.8808493755591094</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1644,16 +1644,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.01788960397609135</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J12">
-        <v>0.8831700141519032</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K12">
-        <v>-0.02174552145202223</v>
+        <v>-0.3118320089283974</v>
       </c>
       <c r="L12">
-        <v>0.8808493755591094</v>
+        <v>0.02748882596687927</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1682,16 +1682,16 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.06524669105718928</v>
+        <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.6720517686591893</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
-        <v>-0.07861110510609637</v>
+        <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.679668768010645</v>
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1720,16 +1720,16 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>-0.153506269493634</v>
+        <v>0.443677499188887</v>
       </c>
       <c r="J14">
-        <v>0.3197630116677985</v>
+        <v>0.003993565524162987</v>
       </c>
       <c r="K14">
-        <v>-0.1847566494939108</v>
+        <v>0.5345555147214552</v>
       </c>
       <c r="L14">
-        <v>0.328369658424491</v>
+        <v>0.002341385142708154</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1796,16 +1796,16 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>0.443677499188887</v>
+        <v>-0.06524669105718928</v>
       </c>
       <c r="J16">
-        <v>0.003993565524162987</v>
+        <v>0.6720517686591893</v>
       </c>
       <c r="K16">
-        <v>0.5345555147214552</v>
+        <v>-0.07861110510609637</v>
       </c>
       <c r="L16">
-        <v>0.002341385142708154</v>
+        <v>0.679668768010645</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1872,16 +1872,16 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.2484997721369916</v>
+        <v>0.2788995520575487</v>
       </c>
       <c r="J18">
-        <v>0.2528129010164081</v>
+        <v>0.2008903265397131</v>
       </c>
       <c r="K18">
-        <v>-0.2952617265740468</v>
+        <v>0.3302413141237342</v>
       </c>
       <c r="L18">
-        <v>0.2669012522950682</v>
+        <v>0.2115824618683086</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1910,16 +1910,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.2788995520575487</v>
+        <v>-0.2484997721369916</v>
       </c>
       <c r="J19">
-        <v>0.2008903265397131</v>
+        <v>0.2528129010164081</v>
       </c>
       <c r="K19">
-        <v>0.3302413141237342</v>
+        <v>-0.2952617265740468</v>
       </c>
       <c r="L19">
-        <v>0.2115824618683086</v>
+        <v>0.2669012522950682</v>
       </c>
     </row>
   </sheetData>
@@ -2013,16 +2013,16 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>0.182178575000007</v>
+        <v>-0.1707825127659933</v>
       </c>
       <c r="J2">
-        <v>0.2956465760209075</v>
+        <v>0.3368221511559395</v>
       </c>
       <c r="K2">
-        <v>0.2404694281998906</v>
+        <v>-0.2206327958702234</v>
       </c>
       <c r="L2">
-        <v>0.2690489763203219</v>
+        <v>0.3117066831945562</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2051,16 +2051,16 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.1707825127659933</v>
+        <v>-0.2155727271443866</v>
       </c>
       <c r="J3">
-        <v>0.3368221511559395</v>
+        <v>0.2189727791934982</v>
       </c>
       <c r="K3">
-        <v>-0.2206327958702234</v>
+        <v>-0.2830068271047704</v>
       </c>
       <c r="L3">
-        <v>0.3117066831945562</v>
+        <v>0.1907013837125806</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2089,16 +2089,16 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>-0.2155727271443866</v>
+        <v>0.182178575000007</v>
       </c>
       <c r="J4">
-        <v>0.2189727791934982</v>
+        <v>0.2956465760209075</v>
       </c>
       <c r="K4">
-        <v>-0.2830068271047704</v>
+        <v>0.2404694281998906</v>
       </c>
       <c r="L4">
-        <v>0.1907013837125806</v>
+        <v>0.2690489763203219</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2127,16 +2127,16 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.2597943666588219</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J5">
-        <v>0.3106354563374008</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.3056992027188027</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L5">
-        <v>0.3338931364506602</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2165,16 +2165,16 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>0.1113404428537808</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J6">
-        <v>0.6639079018776488</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K6">
-        <v>0.131013944022344</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L6">
-        <v>0.6848487144273757</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2203,16 +2203,16 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.2597943666588219</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J7">
-        <v>0.3106354563374008</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K7">
-        <v>-0.3056992027188027</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L7">
-        <v>0.3338931364506602</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2241,16 +2241,16 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.1113404428537808</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J8">
-        <v>0.6639079018776488</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K8">
-        <v>-0.131013944022344</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L8">
-        <v>0.6848487144273757</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2317,16 +2317,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.08571428571428572</v>
+        <v>-0.07398454341194179</v>
       </c>
       <c r="J10">
-        <v>0.4668542708227255</v>
+        <v>0.5326520619235142</v>
       </c>
       <c r="K10">
-        <v>-0.1039438393012856</v>
+        <v>-0.08913753281991174</v>
       </c>
       <c r="L10">
-        <v>0.4725395318267059</v>
+        <v>0.5381698827874621</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2355,16 +2355,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.07398454341194179</v>
+        <v>-0.121885527067201</v>
       </c>
       <c r="J11">
-        <v>0.5326520619235142</v>
+        <v>0.3262530979002883</v>
       </c>
       <c r="K11">
-        <v>-0.08913753281991174</v>
+        <v>-0.1402412823250271</v>
       </c>
       <c r="L11">
-        <v>0.5381698827874621</v>
+        <v>0.3313563853369854</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2393,16 +2393,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.121885527067201</v>
+        <v>-0.08571428571428572</v>
       </c>
       <c r="J12">
-        <v>0.3262530979002883</v>
+        <v>0.4668542708227255</v>
       </c>
       <c r="K12">
-        <v>-0.1402412823250271</v>
+        <v>-0.1039438393012856</v>
       </c>
       <c r="L12">
-        <v>0.3313563853369854</v>
+        <v>0.4725395318267059</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2573,16 +2573,16 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.01695158759052026</v>
+        <v>0.3404532748240978</v>
       </c>
       <c r="J18">
-        <v>0.9369217280976989</v>
+        <v>0.1131965364706231</v>
       </c>
       <c r="K18">
-        <v>-0.03834824944236852</v>
+        <v>0.4029530171380015</v>
       </c>
       <c r="L18">
-        <v>0.8878693028318899</v>
+        <v>0.1217337691688223</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2611,16 +2611,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.3404532748240978</v>
+        <v>-0.01695158759052026</v>
       </c>
       <c r="J19">
-        <v>0.1131965364706231</v>
+        <v>0.9369217280976989</v>
       </c>
       <c r="K19">
-        <v>0.4029530171380015</v>
+        <v>-0.03834824944236852</v>
       </c>
       <c r="L19">
-        <v>0.1217337691688223</v>
+        <v>0.8878693028318899</v>
       </c>
     </row>
   </sheetData>
@@ -2934,16 +2934,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.248946277190559</v>
+        <v>-0.02073391231297599</v>
       </c>
       <c r="J10">
-        <v>0.03184335671615308</v>
+        <v>0.8590316155348903</v>
       </c>
       <c r="K10">
-        <v>-0.3107802994453792</v>
+        <v>-0.02339586347864377</v>
       </c>
       <c r="L10">
-        <v>0.02804344582260457</v>
+        <v>0.8718796181740638</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2972,16 +2972,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02073391231297599</v>
+        <v>-0.01796621933296706</v>
       </c>
       <c r="J11">
-        <v>0.8590316155348903</v>
+        <v>0.8831428170689836</v>
       </c>
       <c r="K11">
-        <v>-0.02339586347864377</v>
+        <v>-0.01941575076033076</v>
       </c>
       <c r="L11">
-        <v>0.8718796181740638</v>
+        <v>0.8935368700981905</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3010,16 +3010,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.01796621933296706</v>
+        <v>-0.248946277190559</v>
       </c>
       <c r="J12">
-        <v>0.8831428170689836</v>
+        <v>0.03184335671615308</v>
       </c>
       <c r="K12">
-        <v>-0.01941575076033076</v>
+        <v>-0.3107802994453792</v>
       </c>
       <c r="L12">
-        <v>0.8935368700981905</v>
+        <v>0.02804344582260457</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3048,16 +3048,16 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.1435427203258164</v>
+        <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.3516806827985527</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
-        <v>-0.172944431233412</v>
+        <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.360759748541673</v>
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3086,16 +3086,16 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>-0.153506269493634</v>
+        <v>0.6916149252062063</v>
       </c>
       <c r="J14">
-        <v>0.3197630116677985</v>
+        <v>7.211867226751588E-06</v>
       </c>
       <c r="K14">
-        <v>-0.1847566494939108</v>
+        <v>0.8332777141246215</v>
       </c>
       <c r="L14">
-        <v>0.328369658424491</v>
+        <v>1.098076308139691E-08</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3162,16 +3162,16 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>0.6916149252062063</v>
+        <v>-0.1435427203258164</v>
       </c>
       <c r="J16">
-        <v>7.211867226751588E-06</v>
+        <v>0.3516806827985527</v>
       </c>
       <c r="K16">
-        <v>0.8332777141246215</v>
+        <v>-0.172944431233412</v>
       </c>
       <c r="L16">
-        <v>1.098076308139691E-08</v>
+        <v>0.360759748541673</v>
       </c>
     </row>
     <row r="17" spans="1:8">

</xml_diff>

<commit_message>
Fix ordering in correlation.py
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -55,42 +55,42 @@
     <t>spearmans_p_value</t>
   </si>
   <si>
+    <t>output_difficulty</t>
+  </si>
+  <si>
+    <t>time_to_give_output</t>
+  </si>
+  <si>
+    <t>brain_act_31ant</t>
+  </si>
+  <si>
+    <t>brain_act_32</t>
+  </si>
+  <si>
+    <t>time_to_understand</t>
+  </si>
+  <si>
+    <t>readability_level_before</t>
+  </si>
+  <si>
+    <t>correct_verif_questions</t>
+  </si>
+  <si>
+    <t>readability_level</t>
+  </si>
+  <si>
+    <t>binary_understandability</t>
+  </si>
+  <si>
     <t>correct_output_rating</t>
   </si>
   <si>
-    <t>output_difficulty</t>
-  </si>
-  <si>
-    <t>time_to_give_output</t>
-  </si>
-  <si>
-    <t>brain_act_31ant</t>
+    <t>gap_accuracy</t>
   </si>
   <si>
     <t>brain_act_31post</t>
   </si>
   <si>
-    <t>brain_act_32</t>
-  </si>
-  <si>
-    <t>time_to_understand</t>
-  </si>
-  <si>
-    <t>readability_level</t>
-  </si>
-  <si>
-    <t>correct_verif_questions</t>
-  </si>
-  <si>
-    <t>binary_understandability</t>
-  </si>
-  <si>
-    <t>gap_accuracy</t>
-  </si>
-  <si>
-    <t>readability_level_before</t>
-  </si>
-  <si>
     <t>readability_level_ba</t>
   </si>
   <si>
@@ -106,16 +106,16 @@
     <t>f</t>
   </si>
   <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>physiological</t>
+  </si>
+  <si>
     <t>correctness</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>physiological</t>
   </si>
   <si>
     <t>lower</t>
@@ -563,16 +563,16 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.09266821663323266</v>
+        <v>-0.1259696449729016</v>
       </c>
       <c r="J2">
-        <v>0.5984721667632871</v>
+        <v>0.4679676774681618</v>
       </c>
       <c r="K2">
-        <v>-0.1263163607514111</v>
+        <v>-0.1721605113945802</v>
       </c>
       <c r="L2">
-        <v>0.5657528992105718</v>
+        <v>0.4321598963432832</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -586,7 +586,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -601,16 +601,16 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.1259696449729016</v>
+        <v>0.09719878783949158</v>
       </c>
       <c r="J3">
-        <v>0.4679676774681618</v>
+        <v>0.5729099316418407</v>
       </c>
       <c r="K3">
-        <v>-0.1721605113945802</v>
+        <v>0.1360629871783227</v>
       </c>
       <c r="L3">
-        <v>0.4321598963432832</v>
+        <v>0.5358931384723264</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -618,7 +618,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -627,28 +627,28 @@
         <v>34</v>
       </c>
       <c r="E4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="I4">
-        <v>0.09719878783949158</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J4">
-        <v>0.5729099316418407</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K4">
-        <v>0.1360629871783227</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L4">
-        <v>0.5358931384723264</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -677,13 +677,13 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.1113404428537808</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J5">
         <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.131013944022344</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L5">
         <v>0.6848487144273757</v>
@@ -694,37 +694,37 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I6">
-        <v>-0.2597943666588219</v>
+        <v>-0.247884667760308</v>
       </c>
       <c r="J6">
-        <v>0.3106354563374008</v>
+        <v>0.03188792894690582</v>
       </c>
       <c r="K6">
-        <v>-0.3056992027188027</v>
+        <v>-0.3109097018922294</v>
       </c>
       <c r="L6">
-        <v>0.3338931364506602</v>
+        <v>0.02797470554846711</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -732,37 +732,37 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I7">
-        <v>0.1113404428537808</v>
+        <v>0.5876550364713691</v>
       </c>
       <c r="J7">
-        <v>0.6639079018776488</v>
+        <v>6.023530742288514E-05</v>
       </c>
       <c r="K7">
-        <v>0.131013944022344</v>
+        <v>0.7491931143441224</v>
       </c>
       <c r="L7">
-        <v>0.6848487144273757</v>
+        <v>1.904021591222836E-06</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -770,83 +770,83 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I8">
-        <v>-0.2597943666588219</v>
+        <v>-0.02815294687312959</v>
       </c>
       <c r="J8">
-        <v>0.3106354563374008</v>
+        <v>0.8086800956106934</v>
       </c>
       <c r="K8">
-        <v>-0.3056992027188027</v>
+        <v>-0.02915890758270907</v>
       </c>
       <c r="L8">
-        <v>0.3338931364506602</v>
+        <v>0.8406889719449382</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9">
-        <v>90</v>
-      </c>
-      <c r="G9">
-        <v>392</v>
-      </c>
       <c r="H9">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I9">
-        <v>-0.2296446241402438</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J9">
-        <v>0.001381085952098848</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K9">
-        <v>-0.3250508508876161</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L9">
-        <v>0.0009677863595653327</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -855,39 +855,39 @@
         <v>33</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F10">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="G10">
-        <v>156</v>
+        <v>392</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I10">
-        <v>-0.02815294687312959</v>
+        <v>-0.2296446241402438</v>
       </c>
       <c r="J10">
-        <v>0.8086800956106934</v>
+        <v>0.001381085952098848</v>
       </c>
       <c r="K10">
-        <v>-0.02915890758270907</v>
+        <v>-0.3250508508876161</v>
       </c>
       <c r="L10">
-        <v>0.8406889719449382</v>
+        <v>0.0009677863595653327</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -919,40 +919,40 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F12">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.09266821663323266</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>0.5984721667632871</v>
       </c>
       <c r="K12">
-        <v>-0.3109097018922294</v>
+        <v>-0.1263163607514111</v>
       </c>
       <c r="L12">
-        <v>0.02797470554846711</v>
+        <v>0.5657528992105718</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -963,7 +963,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -995,92 +995,92 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-      <c r="F14">
-        <v>18</v>
-      </c>
-      <c r="G14">
-        <v>30</v>
-      </c>
       <c r="H14">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I14">
-        <v>0.5876550364713691</v>
+        <v>-0.0639137490706142</v>
       </c>
       <c r="J14">
-        <v>6.023530742288514E-05</v>
+        <v>0.7638561357920776</v>
       </c>
       <c r="K14">
-        <v>0.7491931143441224</v>
+        <v>-0.08738275920531946</v>
       </c>
       <c r="L14">
-        <v>1.904021591222836E-06</v>
+        <v>0.7476087951382137</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="I15">
-        <v>0.5876550364713691</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J15">
-        <v>6.023530742288514E-05</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K15">
-        <v>0.7491931143441224</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L15">
-        <v>1.904021591222836E-06</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -1095,65 +1095,65 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.1130105839368017</v>
+        <v>0.5876550364713691</v>
       </c>
       <c r="J16">
-        <v>0.4404006981390032</v>
+        <v>6.023530742288514E-05</v>
       </c>
       <c r="K16">
-        <v>-0.1377826417184593</v>
+        <v>0.7491931143441224</v>
       </c>
       <c r="L16">
-        <v>0.4677936200616143</v>
+        <v>1.904021591222836E-06</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G17">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I17">
-        <v>-0.3495310368212778</v>
+        <v>-0.1130105839368017</v>
       </c>
       <c r="J17">
-        <v>0.1036923833375111</v>
+        <v>0.4404006981390032</v>
       </c>
       <c r="K17">
-        <v>-0.4089908982453269</v>
+        <v>-0.1377826417184593</v>
       </c>
       <c r="L17">
-        <v>0.1157240968299579</v>
+        <v>0.4677936200616143</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -1171,30 +1171,30 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.3337450085962236</v>
+        <v>-0.3495310368212778</v>
       </c>
       <c r="J18">
-        <v>0.117961265079868</v>
+        <v>0.1036923833375111</v>
       </c>
       <c r="K18">
-        <v>0.393511869842908</v>
+        <v>-0.4089908982453269</v>
       </c>
       <c r="L18">
-        <v>0.1315591494441377</v>
+        <v>0.1157240968299579</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1209,16 +1209,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-0.0639137490706142</v>
+        <v>0.3337450085962236</v>
       </c>
       <c r="J19">
-        <v>0.7638561357920776</v>
+        <v>0.117961265079868</v>
       </c>
       <c r="K19">
-        <v>-0.08738275920531946</v>
+        <v>0.393511869842908</v>
       </c>
       <c r="L19">
-        <v>0.7476087951382137</v>
+        <v>0.1315591494441377</v>
       </c>
     </row>
   </sheetData>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1300,74 +1300,62 @@
         <v>33</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="I2">
-        <v>-0.2277100170213244</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J2">
-        <v>0.2003280221869526</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K2">
-        <v>-0.2719723502938716</v>
+        <v>-0.02174552145202223</v>
       </c>
       <c r="L2">
-        <v>0.2093250956596323</v>
+        <v>0.8808493755591094</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>-0.263477777620917</v>
-      </c>
-      <c r="J3">
-        <v>0.1329850671160174</v>
-      </c>
-      <c r="K3">
-        <v>-0.3201778730528596</v>
-      </c>
-      <c r="L3">
-        <v>0.1363764100850406</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1376,28 +1364,16 @@
         <v>34</v>
       </c>
       <c r="E4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>23</v>
-      </c>
-      <c r="I4">
-        <v>0.2297034206521828</v>
-      </c>
-      <c r="J4">
-        <v>0.187290841633909</v>
-      </c>
-      <c r="K4">
-        <v>0.2809695424230301</v>
-      </c>
-      <c r="L4">
-        <v>0.1940516726155841</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1408,7 +1384,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -1428,54 +1404,78 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>0.2788995520575487</v>
+      </c>
+      <c r="J6">
+        <v>0.2008903265397131</v>
+      </c>
+      <c r="K6">
+        <v>0.3302413141237342</v>
+      </c>
+      <c r="L6">
+        <v>0.2115824618683086</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>-0.2277100170213244</v>
+      </c>
+      <c r="J7">
+        <v>0.2003280221869526</v>
+      </c>
+      <c r="K7">
+        <v>-0.2719723502938716</v>
+      </c>
+      <c r="L7">
+        <v>0.2093250956596323</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1483,71 +1483,83 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>-0.02439922062337898</v>
+      </c>
+      <c r="J8">
+        <v>0.8337884478927275</v>
+      </c>
+      <c r="K8">
+        <v>-0.02805160729475809</v>
+      </c>
+      <c r="L8">
+        <v>0.8466646412386398</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F9">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I9">
-        <v>-0.2289041597670328</v>
+        <v>-0.153506269493634</v>
       </c>
       <c r="J9">
-        <v>0.004154062204876697</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K9">
-        <v>-0.2872671746617843</v>
+        <v>-0.1847566494939108</v>
       </c>
       <c r="L9">
-        <v>0.003756720549751365</v>
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -1556,109 +1568,109 @@
         <v>33</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="I10">
-        <v>-0.02439922062337898</v>
+        <v>-0.263477777620917</v>
       </c>
       <c r="J10">
-        <v>0.8337884478927275</v>
+        <v>0.1329850671160174</v>
       </c>
       <c r="K10">
-        <v>-0.02805160729475809</v>
+        <v>-0.3201778730528596</v>
       </c>
       <c r="L10">
-        <v>0.8466646412386398</v>
+        <v>0.1363764100850406</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="I11">
-        <v>-0.01788960397609135</v>
+        <v>-0.1628423836175867</v>
       </c>
       <c r="J11">
-        <v>0.8831700141519032</v>
+        <v>0.458010988385219</v>
       </c>
       <c r="K11">
-        <v>-0.02174552145202223</v>
+        <v>-0.1916161134706239</v>
       </c>
       <c r="L11">
-        <v>0.8808493755591094</v>
+        <v>0.4771333722542902</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F12">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G12">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.2289041597670328</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>0.004154062204876697</v>
       </c>
       <c r="K12">
-        <v>-0.3118320089283974</v>
+        <v>-0.2872671746617843</v>
       </c>
       <c r="L12">
-        <v>0.02748882596687927</v>
+        <v>0.003756720549751365</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -1682,27 +1694,27 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.153506269493634</v>
+        <v>0.443677499188887</v>
       </c>
       <c r="J13">
-        <v>0.3197630116677985</v>
+        <v>0.003993565524162987</v>
       </c>
       <c r="K13">
-        <v>-0.1847566494939108</v>
+        <v>0.5345555147214552</v>
       </c>
       <c r="L13">
-        <v>0.328369658424491</v>
+        <v>0.002341385142708154</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -1734,40 +1746,40 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I15">
-        <v>0.443677499188887</v>
+        <v>0.2297034206521828</v>
       </c>
       <c r="J15">
-        <v>0.003993565524162987</v>
+        <v>0.187290841633909</v>
       </c>
       <c r="K15">
-        <v>0.5345555147214552</v>
+        <v>0.2809695424230301</v>
       </c>
       <c r="L15">
-        <v>0.002341385142708154</v>
+        <v>0.1940516726155841</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1778,7 +1790,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -1810,89 +1822,77 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="I17">
-        <v>-0.1628423836175867</v>
-      </c>
-      <c r="J17">
-        <v>0.458010988385219</v>
-      </c>
-      <c r="K17">
-        <v>-0.1916161134706239</v>
-      </c>
-      <c r="L17">
-        <v>0.4771333722542902</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="F18">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18">
-        <v>16</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
       <c r="G18">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="I18">
-        <v>0.2788995520575487</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J18">
-        <v>0.2008903265397131</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K18">
-        <v>0.3302413141237342</v>
+        <v>-0.3118320089283974</v>
       </c>
       <c r="L18">
-        <v>0.2115824618683086</v>
+        <v>0.02748882596687927</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -1989,16 +1989,16 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2013,62 +2013,62 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.1707825127659933</v>
+        <v>0.182178575000007</v>
       </c>
       <c r="J2">
-        <v>0.3368221511559395</v>
+        <v>0.2956465760209075</v>
       </c>
       <c r="K2">
-        <v>-0.2206327958702234</v>
+        <v>0.2404694281998906</v>
       </c>
       <c r="L2">
-        <v>0.3117066831945562</v>
+        <v>0.2690489763203219</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3">
-        <v>23</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>14</v>
-      </c>
       <c r="H3">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="I3">
-        <v>-0.2155727271443866</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J3">
-        <v>0.2189727791934982</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K3">
-        <v>-0.2830068271047704</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L3">
-        <v>0.1907013837125806</v>
+        <v>0.6848487144273757</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -2077,28 +2077,28 @@
         <v>34</v>
       </c>
       <c r="E4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>14</v>
-      </c>
       <c r="H4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="I4">
-        <v>0.182178575000007</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J4">
-        <v>0.2956465760209075</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K4">
-        <v>0.2404694281998906</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L4">
-        <v>0.2690489763203219</v>
+        <v>0.3338931364506602</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2109,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -2127,13 +2127,13 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.1113404428537808</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J5">
         <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.131013944022344</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L5">
         <v>0.6848487144273757</v>
@@ -2147,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2179,293 +2179,305 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I7">
-        <v>0.1113404428537808</v>
+        <v>-0.08571428571428572</v>
       </c>
       <c r="J7">
-        <v>0.6639079018776488</v>
+        <v>0.4668542708227255</v>
       </c>
       <c r="K7">
-        <v>0.131013944022344</v>
+        <v>-0.1039438393012856</v>
       </c>
       <c r="L7">
-        <v>0.6848487144273757</v>
+        <v>0.4725395318267059</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>-0.2597943666588219</v>
-      </c>
-      <c r="J8">
-        <v>0.3106354563374008</v>
-      </c>
-      <c r="K8">
-        <v>-0.3056992027188027</v>
-      </c>
-      <c r="L8">
-        <v>0.3338931364506602</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="F9">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>327</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459341</v>
+        <v>-0.01695158759052026</v>
       </c>
       <c r="J9">
-        <v>0.0301286154880051</v>
+        <v>0.9369217280976989</v>
       </c>
       <c r="K9">
-        <v>-0.2203331090972887</v>
+        <v>-0.03834824944236852</v>
       </c>
       <c r="L9">
-        <v>0.0276105659239954</v>
+        <v>0.8878693028318899</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="I10">
-        <v>-0.07398454341194179</v>
+        <v>-0.1707825127659933</v>
       </c>
       <c r="J10">
-        <v>0.5326520619235142</v>
+        <v>0.3368221511559395</v>
       </c>
       <c r="K10">
-        <v>-0.08913753281991174</v>
+        <v>-0.2206327958702234</v>
       </c>
       <c r="L10">
-        <v>0.5381698827874621</v>
+        <v>0.3117066831945562</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="I11">
-        <v>-0.121885527067201</v>
+        <v>-0.2155727271443866</v>
       </c>
       <c r="J11">
-        <v>0.3262530979002883</v>
+        <v>0.2189727791934982</v>
       </c>
       <c r="K11">
-        <v>-0.1402412823250271</v>
+        <v>-0.2830068271047704</v>
       </c>
       <c r="L11">
-        <v>0.3313563853369854</v>
+        <v>0.1907013837125806</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="G12">
-        <v>52</v>
+        <v>327</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I12">
-        <v>-0.08571428571428572</v>
+        <v>-0.15625137459341</v>
       </c>
       <c r="J12">
-        <v>0.4668542708227255</v>
+        <v>0.0301286154880051</v>
       </c>
       <c r="K12">
-        <v>-0.1039438393012856</v>
+        <v>-0.2203331090972887</v>
       </c>
       <c r="L12">
-        <v>0.4725395318267059</v>
+        <v>0.0276105659239954</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>-0.07398454341194179</v>
+      </c>
+      <c r="J13">
+        <v>0.5326520619235142</v>
+      </c>
+      <c r="K13">
+        <v>-0.08913753281991174</v>
+      </c>
+      <c r="L13">
+        <v>0.5381698827874621</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>-0.121885527067201</v>
+      </c>
+      <c r="J14">
+        <v>0.3262530979002883</v>
+      </c>
+      <c r="K14">
+        <v>-0.1402412823250271</v>
+      </c>
+      <c r="L14">
+        <v>0.3313563853369854</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -2485,16 +2497,16 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -2511,10 +2523,10 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -2523,39 +2535,27 @@
         <v>33</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="I17">
-        <v>-0.4978586625371179</v>
-      </c>
-      <c r="J17">
-        <v>0.02133732054563453</v>
-      </c>
-      <c r="K17">
-        <v>-0.5769230769230769</v>
-      </c>
-      <c r="L17">
-        <v>0.01929785020805572</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2573,30 +2573,30 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.3404532748240978</v>
+        <v>-0.4978586625371179</v>
       </c>
       <c r="J18">
-        <v>0.1131965364706231</v>
+        <v>0.02133732054563453</v>
       </c>
       <c r="K18">
-        <v>0.4029530171380015</v>
+        <v>-0.5769230769230769</v>
       </c>
       <c r="L18">
-        <v>0.1217337691688223</v>
+        <v>0.01929785020805572</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -2611,16 +2611,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-0.01695158759052026</v>
+        <v>0.3404532748240978</v>
       </c>
       <c r="J19">
-        <v>0.9369217280976989</v>
+        <v>0.1131965364706231</v>
       </c>
       <c r="K19">
-        <v>-0.03834824944236852</v>
+        <v>0.4029530171380015</v>
       </c>
       <c r="L19">
-        <v>0.8878693028318899</v>
+        <v>0.1217337691688223</v>
       </c>
     </row>
   </sheetData>
@@ -2690,13 +2690,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -2716,71 +2716,95 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
       <c r="E3">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H3">
-        <v>23</v>
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>-0.02073391231297599</v>
+      </c>
+      <c r="J3">
+        <v>0.8590316155348903</v>
+      </c>
+      <c r="K3">
+        <v>-0.02339586347864377</v>
+      </c>
+      <c r="L3">
+        <v>0.8718796181740638</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>-0.153506269493634</v>
+      </c>
+      <c r="J4">
+        <v>0.3197630116677985</v>
+      </c>
+      <c r="K4">
+        <v>-0.1847566494939108</v>
+      </c>
+      <c r="L4">
+        <v>0.328369658424491</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2789,18 +2813,18 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2820,13 +2844,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2846,7 +2870,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -2872,48 +2896,36 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <v>-0.1325530043077417</v>
-      </c>
-      <c r="J9">
-        <v>0.1086826442074059</v>
-      </c>
-      <c r="K9">
-        <v>-0.1612223880273475</v>
-      </c>
-      <c r="L9">
-        <v>0.1090548020620709</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2922,39 +2934,39 @@
         <v>33</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I10">
-        <v>-0.02073391231297599</v>
+        <v>-0.1325530043077417</v>
       </c>
       <c r="J10">
-        <v>0.8590316155348903</v>
+        <v>0.1086826442074059</v>
       </c>
       <c r="K10">
-        <v>-0.02339586347864377</v>
+        <v>-0.1612223880273475</v>
       </c>
       <c r="L10">
-        <v>0.8718796181740638</v>
+        <v>0.1090548020620709</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -2986,45 +2998,45 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="F12">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12">
-        <v>50</v>
-      </c>
-      <c r="F12">
-        <v>21</v>
-      </c>
       <c r="G12">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>-0.248946277190559</v>
+        <v>0.6916149252062063</v>
       </c>
       <c r="J12">
-        <v>0.03184335671615308</v>
+        <v>7.211867226751588E-06</v>
       </c>
       <c r="K12">
-        <v>-0.3107802994453792</v>
+        <v>0.8332777141246215</v>
       </c>
       <c r="L12">
-        <v>0.02804344582260457</v>
+        <v>1.098076308139691E-08</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -3048,193 +3060,181 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.153506269493634</v>
+        <v>0.6916149252062063</v>
       </c>
       <c r="J13">
-        <v>0.3197630116677985</v>
+        <v>7.211867226751588E-06</v>
       </c>
       <c r="K13">
-        <v>-0.1847566494939108</v>
+        <v>0.8332777141246215</v>
       </c>
       <c r="L13">
-        <v>0.328369658424491</v>
+        <v>1.098076308139691E-08</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F14">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>30</v>
-      </c>
-      <c r="I14">
-        <v>0.6916149252062063</v>
-      </c>
-      <c r="J14">
-        <v>7.211867226751588E-06</v>
-      </c>
-      <c r="K14">
-        <v>0.8332777141246215</v>
-      </c>
-      <c r="L14">
-        <v>1.098076308139691E-08</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>30</v>
-      </c>
-      <c r="I15">
-        <v>0.6916149252062063</v>
-      </c>
-      <c r="J15">
-        <v>7.211867226751588E-06</v>
-      </c>
-      <c r="K15">
-        <v>0.8332777141246215</v>
-      </c>
-      <c r="L15">
-        <v>1.098076308139691E-08</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>21</v>
+      </c>
+      <c r="G17">
+        <v>21</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <v>-0.248946277190559</v>
+      </c>
+      <c r="J17">
+        <v>0.03184335671615308</v>
+      </c>
+      <c r="K17">
+        <v>-0.3107802994453792</v>
+      </c>
+      <c r="L17">
+        <v>0.02804344582260457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
         <v>18</v>
       </c>
-      <c r="G16">
+      <c r="G18">
         <v>18</v>
       </c>
-      <c r="H16">
-        <v>30</v>
-      </c>
-      <c r="I16">
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
         <v>-0.1435427203258164</v>
       </c>
-      <c r="J16">
+      <c r="J18">
         <v>0.3516806827985527</v>
       </c>
-      <c r="K16">
+      <c r="K18">
         <v>-0.172944431233412</v>
       </c>
-      <c r="L16">
+      <c r="L18">
         <v>0.360759748541673</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17">
-        <v>16</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18">
-        <v>16</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Add raw_correlation_data.csv fixed issue reading in dataset 9 metrics
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9567D1F6-8BD4-4E4F-A0E9-21B0BA5B16F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="typestate_checker" sheetId="3" r:id="rId3"/>
     <sheet name="infer" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -61,6 +55,9 @@
     <t>spearmans_p_value</t>
   </si>
   <si>
+    <t>correct_output_rating</t>
+  </si>
+  <si>
     <t>output_difficulty</t>
   </si>
   <si>
@@ -70,33 +67,30 @@
     <t>brain_act_31ant</t>
   </si>
   <si>
+    <t>brain_act_31post</t>
+  </si>
+  <si>
     <t>brain_act_32</t>
   </si>
   <si>
     <t>time_to_understand</t>
   </si>
   <si>
+    <t>readability_level</t>
+  </si>
+  <si>
+    <t>correct_verif_questions</t>
+  </si>
+  <si>
+    <t>binary_understandability</t>
+  </si>
+  <si>
+    <t>gap_accuracy</t>
+  </si>
+  <si>
     <t>readability_level_before</t>
   </si>
   <si>
-    <t>correct_verif_questions</t>
-  </si>
-  <si>
-    <t>readability_level</t>
-  </si>
-  <si>
-    <t>binary_understandability</t>
-  </si>
-  <si>
-    <t>correct_output_rating</t>
-  </si>
-  <si>
-    <t>gap_accuracy</t>
-  </si>
-  <si>
-    <t>brain_act_31post</t>
-  </si>
-  <si>
     <t>readability_level_ba</t>
   </si>
   <si>
@@ -112,6 +106,9 @@
     <t>f</t>
   </si>
   <si>
+    <t>correctness</t>
+  </si>
+  <si>
     <t>rating</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>physiological</t>
-  </si>
-  <si>
-    <t>correctness</t>
   </si>
   <si>
     <t>lower</t>
@@ -133,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,14 +191,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -251,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,27 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,24 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -528,14 +478,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -546,12 +494,12 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,15 +537,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -615,27 +563,27 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-9.2668216633232658E-2</v>
+        <v>-0.09266821663323266</v>
       </c>
       <c r="J2">
-        <v>0.59847216676328707</v>
+        <v>0.5984721667632871</v>
       </c>
       <c r="K2">
-        <v>-0.12631636075141109</v>
+        <v>-0.1263163607514111</v>
       </c>
       <c r="L2">
-        <v>0.56575289921057181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.5657528992105718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -653,27 +601,27 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.12596964497290161</v>
+        <v>-0.1259696449729016</v>
       </c>
       <c r="J3">
-        <v>0.46796767746816181</v>
+        <v>0.4679676774681618</v>
       </c>
       <c r="K3">
-        <v>-0.17216051139458019</v>
+        <v>-0.1721605113945802</v>
       </c>
       <c r="L3">
-        <v>0.43215989634328322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4321598963432832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -691,27 +639,27 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>9.7198787839491582E-2</v>
+        <v>0.09719878783949158</v>
       </c>
       <c r="J4">
-        <v>0.57290993164184068</v>
+        <v>0.5729099316418407</v>
       </c>
       <c r="K4">
-        <v>0.13606298717832269</v>
+        <v>0.1360629871783227</v>
       </c>
       <c r="L4">
-        <v>0.53589313847232645</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.5358931384723264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -729,27 +677,27 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.11134044285378079</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J5">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.13101394402234401</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L5">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -767,27 +715,27 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J6">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K6">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L6">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -805,27 +753,27 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.11134044285378079</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J7">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K7">
-        <v>0.13101394402234401</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L7">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -843,19 +791,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J8">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K8">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L8">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -863,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -881,27 +829,27 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.22964462414024381</v>
+        <v>-0.2296446241402438</v>
       </c>
       <c r="J9">
-        <v>1.3810859520988481E-3</v>
+        <v>0.001381085952098848</v>
       </c>
       <c r="K9">
-        <v>-0.32505085088761609</v>
+        <v>-0.3250508508876161</v>
       </c>
       <c r="L9">
-        <v>9.6778635956533269E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.0009677863595653327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -919,27 +867,27 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-2.8152946873129591E-2</v>
+        <v>-0.02815294687312959</v>
       </c>
       <c r="J10">
-        <v>0.80868009561069343</v>
+        <v>0.8086800956106934</v>
       </c>
       <c r="K10">
-        <v>-2.915890758270907E-2</v>
+        <v>-0.02915890758270907</v>
       </c>
       <c r="L10">
-        <v>0.84068897194493819</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8406889719449382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -957,27 +905,27 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-2.1865071526333869E-2</v>
+        <v>-0.02186507152633387</v>
       </c>
       <c r="J11">
-        <v>0.85746045357848777</v>
+        <v>0.8574604535784878</v>
       </c>
       <c r="K11">
-        <v>-2.3705418235251699E-2</v>
+        <v>-0.0237054182352517</v>
       </c>
       <c r="L11">
-        <v>0.87019890091340346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8701989009134035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -995,19 +943,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.24788466776030799</v>
+        <v>-0.247884667760308</v>
       </c>
       <c r="J12">
-        <v>3.1887928946905821E-2</v>
+        <v>0.03188792894690582</v>
       </c>
       <c r="K12">
-        <v>-0.31090970189222938</v>
+        <v>-0.3109097018922294</v>
       </c>
       <c r="L12">
-        <v>2.7974705548467111E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.02797470554846711</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1015,7 +963,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -1036,24 +984,24 @@
         <v>-0.1668825406867738</v>
       </c>
       <c r="J13">
-        <v>0.25506729747462942</v>
+        <v>0.2550672974746294</v>
       </c>
       <c r="K13">
-        <v>-0.20239076915378071</v>
+        <v>-0.2023907691537807</v>
       </c>
       <c r="L13">
-        <v>0.28345717868919151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2834571786891915</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -1071,19 +1019,19 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.58765503647136907</v>
+        <v>0.2791309202017375</v>
       </c>
       <c r="J14">
-        <v>6.0235307422885138E-5</v>
+        <v>0.05845574211659071</v>
       </c>
       <c r="K14">
-        <v>0.74919311434412239</v>
+        <v>0.3426469504890525</v>
       </c>
       <c r="L14">
-        <v>1.9040215912228359E-6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.06380076796503868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1039,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -1109,19 +1057,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.58765503647136907</v>
+        <v>0.2664954118305773</v>
       </c>
       <c r="J15">
-        <v>6.0235307422885138E-5</v>
+        <v>0.06971859781714017</v>
       </c>
       <c r="K15">
-        <v>0.74919311434412239</v>
+        <v>0.3230358829236744</v>
       </c>
       <c r="L15">
-        <v>1.9040215912228359E-6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.08165110179558877</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1129,7 +1077,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -1150,16 +1098,16 @@
         <v>-0.1130105839368017</v>
       </c>
       <c r="J16">
-        <v>0.44040069813900318</v>
+        <v>0.4404006981390032</v>
       </c>
       <c r="K16">
         <v>-0.1377826417184593</v>
       </c>
       <c r="L16">
-        <v>0.46779362006161429</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4677936200616143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1167,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -1185,19 +1133,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.34953103682127779</v>
+        <v>-0.3495310368212778</v>
       </c>
       <c r="J17">
         <v>0.1036923833375111</v>
       </c>
       <c r="K17">
-        <v>-0.40899089824532692</v>
+        <v>-0.4089908982453269</v>
       </c>
       <c r="L17">
-        <v>0.11572409682995791</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1157240968299579</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1205,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -1223,27 +1171,27 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.33374500859622358</v>
+        <v>0.3337450085962236</v>
       </c>
       <c r="J18">
         <v>0.117961265079868</v>
       </c>
       <c r="K18">
-        <v>0.39351186984290798</v>
+        <v>0.393511869842908</v>
       </c>
       <c r="L18">
-        <v>0.13155914944413771</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1315591494441377</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -1261,16 +1209,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-6.3913749070614201E-2</v>
+        <v>-0.0639137490706142</v>
       </c>
       <c r="J19">
-        <v>0.76385613579207756</v>
+        <v>0.7638561357920776</v>
       </c>
       <c r="K19">
-        <v>-8.738275920531946E-2</v>
+        <v>-0.08738275920531946</v>
       </c>
       <c r="L19">
-        <v>0.74760879513821366</v>
+        <v>0.7476087951382137</v>
       </c>
     </row>
   </sheetData>
@@ -1279,14 +1227,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1296,12 +1242,13 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="10" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1339,15 +1286,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -1368,24 +1315,24 @@
         <v>-0.2277100170213244</v>
       </c>
       <c r="J2">
-        <v>0.20032802218695259</v>
+        <v>0.2003280221869526</v>
       </c>
       <c r="K2">
-        <v>-0.27197235029387162</v>
+        <v>-0.2719723502938716</v>
       </c>
       <c r="L2">
-        <v>0.20932509565963231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2093250956596323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -1403,27 +1350,27 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.26347777762091701</v>
+        <v>-0.263477777620917</v>
       </c>
       <c r="J3">
         <v>0.1329850671160174</v>
       </c>
       <c r="K3">
-        <v>-0.32017787305285961</v>
+        <v>-0.3201778730528596</v>
       </c>
       <c r="L3">
-        <v>0.13637641008504059</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1363764100850406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -1444,24 +1391,24 @@
         <v>0.2297034206521828</v>
       </c>
       <c r="J4">
-        <v>0.18729084163390899</v>
+        <v>0.187290841633909</v>
       </c>
       <c r="K4">
-        <v>0.28096954242303013</v>
+        <v>0.2809695424230301</v>
       </c>
       <c r="L4">
-        <v>0.19405167261558409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1940516726155841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -1479,15 +1426,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -1505,15 +1452,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -1531,15 +1478,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -1557,7 +1504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1565,7 +1512,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -1583,27 +1530,27 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.22890415976703279</v>
+        <v>-0.2289041597670328</v>
       </c>
       <c r="J9">
-        <v>4.1540622048766972E-3</v>
+        <v>0.004154062204876697</v>
       </c>
       <c r="K9">
-        <v>-0.28726717466178431</v>
+        <v>-0.2872671746617843</v>
       </c>
       <c r="L9">
-        <v>3.7567205497513649E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.003756720549751365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1621,27 +1568,27 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-2.439922062337898E-2</v>
+        <v>-0.02439922062337898</v>
       </c>
       <c r="J10">
-        <v>0.83378844789272755</v>
+        <v>0.8337884478927275</v>
       </c>
       <c r="K10">
-        <v>-2.8051607294758089E-2</v>
+        <v>-0.02805160729475809</v>
       </c>
       <c r="L10">
-        <v>0.84666464123863983</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8466646412386398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -1659,27 +1606,27 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-1.7889603976091351E-2</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J11">
-        <v>0.88317001415190322</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K11">
-        <v>-2.1745521452022229E-2</v>
+        <v>-0.02174552145202223</v>
       </c>
       <c r="L11">
-        <v>0.88084937555910936</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8808493755591094</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -1697,19 +1644,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.25161225674918491</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J12">
-        <v>2.940004335865699E-2</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K12">
-        <v>-0.31183200892839741</v>
+        <v>-0.3118320089283974</v>
       </c>
       <c r="L12">
-        <v>2.7488825966879269E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.02748882596687927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1717,7 +1664,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -1738,24 +1685,24 @@
         <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.31976301166779852</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
         <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.32836965842449101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.328369658424491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -1773,19 +1720,19 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.44367749918888699</v>
+        <v>0.2072009724655128</v>
       </c>
       <c r="J14">
-        <v>3.9935655241629866E-3</v>
+        <v>0.1819292666306944</v>
       </c>
       <c r="K14">
-        <v>0.53455551472145524</v>
+        <v>0.2478732543966922</v>
       </c>
       <c r="L14">
-        <v>2.341385142708154E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1866046727680992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1793,7 +1740,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -1811,19 +1758,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.44367749918888699</v>
+        <v>0.2095131203515696</v>
       </c>
       <c r="J15">
-        <v>3.9935655241629866E-3</v>
+        <v>0.1753792300739662</v>
       </c>
       <c r="K15">
-        <v>0.53455551472145524</v>
+        <v>0.2516395234999386</v>
       </c>
       <c r="L15">
-        <v>2.341385142708154E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1797825804394816</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +1778,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -1849,19 +1796,19 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-6.5246691057189277E-2</v>
+        <v>-0.06524669105718928</v>
       </c>
       <c r="J16">
-        <v>0.67205176865918925</v>
+        <v>0.6720517686591893</v>
       </c>
       <c r="K16">
-        <v>-7.8611105106096368E-2</v>
+        <v>-0.07861110510609637</v>
       </c>
       <c r="L16">
-        <v>0.67966876801064502</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.679668768010645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1816,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -1887,19 +1834,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.16284238361758671</v>
+        <v>-0.1628423836175867</v>
       </c>
       <c r="J17">
-        <v>0.45801098838521898</v>
+        <v>0.458010988385219</v>
       </c>
       <c r="K17">
-        <v>-0.19161611347062391</v>
+        <v>-0.1916161134706239</v>
       </c>
       <c r="L17">
         <v>0.4771333722542902</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1907,7 +1854,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -1925,27 +1872,27 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.27889955205754868</v>
+        <v>0.2788995520575487</v>
       </c>
       <c r="J18">
-        <v>0.20089032653971309</v>
+        <v>0.2008903265397131</v>
       </c>
       <c r="K18">
         <v>0.3302413141237342</v>
       </c>
       <c r="L18">
-        <v>0.21158246186830859</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2115824618683086</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -1963,16 +1910,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-0.24849977213699159</v>
+        <v>-0.2484997721369916</v>
       </c>
       <c r="J19">
-        <v>0.25281290101640808</v>
+        <v>0.2528129010164081</v>
       </c>
       <c r="K19">
-        <v>-0.29526172657404681</v>
+        <v>-0.2952617265740468</v>
       </c>
       <c r="L19">
-        <v>0.26690125229506823</v>
+        <v>0.2669012522950682</v>
       </c>
     </row>
   </sheetData>
@@ -1981,14 +1928,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1998,10 +1943,13 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="12" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2039,15 +1987,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -2065,27 +2013,27 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.17078251276599329</v>
+        <v>-0.1707825127659933</v>
       </c>
       <c r="J2">
         <v>0.3368221511559395</v>
       </c>
       <c r="K2">
-        <v>-0.22063279587022341</v>
+        <v>-0.2206327958702234</v>
       </c>
       <c r="L2">
-        <v>0.31170668319455619</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3117066831945562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -2103,27 +2051,27 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.21557272714438661</v>
+        <v>-0.2155727271443866</v>
       </c>
       <c r="J3">
         <v>0.2189727791934982</v>
       </c>
       <c r="K3">
-        <v>-0.28300682710477038</v>
+        <v>-0.2830068271047704</v>
       </c>
       <c r="L3">
-        <v>0.19070138371258061</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1907013837125806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2144,24 +2092,24 @@
         <v>0.182178575000007</v>
       </c>
       <c r="J4">
-        <v>0.29564657602090749</v>
+        <v>0.2956465760209075</v>
       </c>
       <c r="K4">
-        <v>0.24046942819989059</v>
+        <v>0.2404694281998906</v>
       </c>
       <c r="L4">
-        <v>0.26904897632032188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2690489763203219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -2179,27 +2127,27 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.11134044285378079</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J5">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.13101394402234401</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L5">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2217,27 +2165,27 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J6">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K6">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L6">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2255,27 +2203,27 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.11134044285378079</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J7">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K7">
-        <v>0.13101394402234401</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L7">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -2293,19 +2241,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J8">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K8">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L8">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2313,7 +2261,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -2331,27 +2279,27 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459340999</v>
+        <v>-0.15625137459341</v>
       </c>
       <c r="J9">
-        <v>3.0128615488005099E-2</v>
+        <v>0.0301286154880051</v>
       </c>
       <c r="K9">
         <v>-0.2203331090972887</v>
       </c>
       <c r="L9">
-        <v>2.7610565923995401E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.0276105659239954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -2369,27 +2317,27 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-7.3984543411941786E-2</v>
+        <v>-0.07398454341194179</v>
       </c>
       <c r="J10">
-        <v>0.53265206192351422</v>
+        <v>0.5326520619235142</v>
       </c>
       <c r="K10">
-        <v>-8.9137532819911741E-2</v>
+        <v>-0.08913753281991174</v>
       </c>
       <c r="L10">
-        <v>0.53816988278746214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.5381698827874621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -2410,24 +2358,24 @@
         <v>-0.121885527067201</v>
       </c>
       <c r="J11">
-        <v>0.32625309790028828</v>
+        <v>0.3262530979002883</v>
       </c>
       <c r="K11">
-        <v>-0.14024128232502711</v>
+        <v>-0.1402412823250271</v>
       </c>
       <c r="L11">
-        <v>0.33135638533698542</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3313563853369854</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -2445,19 +2393,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-8.5714285714285715E-2</v>
+        <v>-0.08571428571428572</v>
       </c>
       <c r="J12">
-        <v>0.46685427082272551</v>
+        <v>0.4668542708227255</v>
       </c>
       <c r="K12">
         <v>-0.1039438393012856</v>
       </c>
       <c r="L12">
-        <v>0.47253953182670588</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4725395318267059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2465,7 +2413,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -2483,15 +2431,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -2509,7 +2457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2517,7 +2465,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -2535,7 +2483,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2543,7 +2491,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -2561,7 +2509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2569,7 +2517,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -2587,19 +2535,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.49785866253711791</v>
+        <v>-0.4978586625371179</v>
       </c>
       <c r="J17">
-        <v>2.1337320545634531E-2</v>
+        <v>0.02133732054563453</v>
       </c>
       <c r="K17">
-        <v>-0.57692307692307687</v>
+        <v>-0.5769230769230769</v>
       </c>
       <c r="L17">
-        <v>1.929785020805572E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.01929785020805572</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2607,7 +2555,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2625,27 +2573,27 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.34045327482409782</v>
+        <v>0.3404532748240978</v>
       </c>
       <c r="J18">
         <v>0.1131965364706231</v>
       </c>
       <c r="K18">
-        <v>0.40295301713800152</v>
+        <v>0.4029530171380015</v>
       </c>
       <c r="L18">
         <v>0.1217337691688223</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -2663,16 +2611,16 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-1.6951587590520258E-2</v>
+        <v>-0.01695158759052026</v>
       </c>
       <c r="J19">
-        <v>0.93692172809769891</v>
+        <v>0.9369217280976989</v>
       </c>
       <c r="K19">
-        <v>-3.8348249442368518E-2</v>
+        <v>-0.03834824944236852</v>
       </c>
       <c r="L19">
-        <v>0.88786930283188992</v>
+        <v>0.8878693028318899</v>
       </c>
     </row>
   </sheetData>
@@ -2681,14 +2629,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -2698,12 +2644,13 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="10" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2741,15 +2688,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -2767,15 +2714,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -2793,15 +2740,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2819,15 +2766,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -2845,15 +2792,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2871,15 +2818,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2897,15 +2844,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -2923,7 +2870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2931,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -2952,24 +2899,24 @@
         <v>-0.1325530043077417</v>
       </c>
       <c r="J9">
-        <v>0.10868264420740591</v>
+        <v>0.1086826442074059</v>
       </c>
       <c r="K9">
-        <v>-0.16122238802734751</v>
+        <v>-0.1612223880273475</v>
       </c>
       <c r="L9">
         <v>0.1090548020620709</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -2987,27 +2934,27 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-2.0733912312975989E-2</v>
+        <v>-0.02073391231297599</v>
       </c>
       <c r="J10">
-        <v>0.85903161553489027</v>
+        <v>0.8590316155348903</v>
       </c>
       <c r="K10">
-        <v>-2.339586347864377E-2</v>
+        <v>-0.02339586347864377</v>
       </c>
       <c r="L10">
-        <v>0.87187961817406379</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8718796181740638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -3025,27 +2972,27 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-1.7966219332967059E-2</v>
+        <v>-0.01796621933296706</v>
       </c>
       <c r="J11">
-        <v>0.88314281706898357</v>
+        <v>0.8831428170689836</v>
       </c>
       <c r="K11">
-        <v>-1.9415750760330759E-2</v>
+        <v>-0.01941575076033076</v>
       </c>
       <c r="L11">
-        <v>0.89353687009819049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8935368700981905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -3063,19 +3010,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.24894627719055901</v>
+        <v>-0.248946277190559</v>
       </c>
       <c r="J12">
-        <v>3.1843356716153078E-2</v>
+        <v>0.03184335671615308</v>
       </c>
       <c r="K12">
-        <v>-0.31078029944537922</v>
+        <v>-0.3107802994453792</v>
       </c>
       <c r="L12">
-        <v>2.8043445822604571E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.02804344582260457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3083,7 +3030,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -3104,24 +3051,24 @@
         <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.31976301166779852</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
         <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.32836965842449101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.328369658424491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -3139,19 +3086,19 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.69161492520620627</v>
+        <v>0.3157348151855433</v>
       </c>
       <c r="J14">
-        <v>7.2118672267515883E-6</v>
+        <v>0.04194762772357558</v>
       </c>
       <c r="K14">
-        <v>0.83327771412462148</v>
+        <v>0.3777116257473406</v>
       </c>
       <c r="L14">
-        <v>1.098076308139691E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.03960563400379821</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3159,7 +3106,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -3177,19 +3124,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.69161492520620627</v>
+        <v>0.2815332554724217</v>
       </c>
       <c r="J15">
-        <v>7.2118672267515883E-6</v>
+        <v>0.0686155353555807</v>
       </c>
       <c r="K15">
-        <v>0.83327771412462148</v>
+        <v>0.3381406097030425</v>
       </c>
       <c r="L15">
-        <v>1.098076308139691E-8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.06760452162982369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3197,7 +3144,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -3215,19 +3162,19 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.14354272032581639</v>
+        <v>-0.1435427203258164</v>
       </c>
       <c r="J16">
-        <v>0.35168068279855269</v>
+        <v>0.3516806827985527</v>
       </c>
       <c r="K16">
-        <v>-0.17294443123341199</v>
+        <v>-0.172944431233412</v>
       </c>
       <c r="L16">
-        <v>0.36075974854167298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.360759748541673</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -3235,7 +3182,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -3253,7 +3200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3261,7 +3208,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -3279,15 +3226,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Add physiological metrics from fmri dataset
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="37">
   <si>
     <t>metric</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>perc_correct_output</t>
+  </si>
+  <si>
+    <t>something_ba31</t>
+  </si>
+  <si>
+    <t>something_ba32</t>
   </si>
   <si>
     <t>complexity_level</t>
@@ -479,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -545,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -583,10 +589,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -621,10 +627,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -659,10 +665,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -697,10 +703,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -735,10 +741,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -773,10 +779,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -811,10 +817,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -849,10 +855,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -887,10 +893,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -925,10 +931,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -963,10 +969,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -1001,10 +1007,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1039,10 +1045,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -1077,10 +1083,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -1112,13 +1118,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -1150,13 +1156,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -1171,30 +1177,30 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.3337450085962236</v>
+        <v>-0.1661757475835969</v>
       </c>
       <c r="J18">
-        <v>0.117961265079868</v>
+        <v>0.4347470349719929</v>
       </c>
       <c r="K18">
-        <v>0.393511869842908</v>
+        <v>-0.1825328747844451</v>
       </c>
       <c r="L18">
-        <v>0.1315591494441377</v>
+        <v>0.4986441746860601</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1209,15 +1215,91 @@
         <v>16</v>
       </c>
       <c r="I19">
+        <v>-0.08947924869885987</v>
+      </c>
+      <c r="J19">
+        <v>0.6740550539155759</v>
+      </c>
+      <c r="K19">
+        <v>-0.09515011557912563</v>
+      </c>
+      <c r="L19">
+        <v>0.7259456900683131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>0.3337450085962236</v>
+      </c>
+      <c r="J20">
+        <v>0.117961265079868</v>
+      </c>
+      <c r="K20">
+        <v>0.393511869842908</v>
+      </c>
+      <c r="L20">
+        <v>0.1315591494441377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
         <v>-0.0639137490706142</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>0.7638561357920776</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>-0.08738275920531946</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>0.7476087951382137</v>
       </c>
     </row>
@@ -1228,7 +1310,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1294,10 +1376,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -1332,10 +1414,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -1370,10 +1452,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -1408,10 +1490,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -1434,10 +1516,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -1460,10 +1542,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -1486,10 +1568,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1512,10 +1594,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1550,10 +1632,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -1588,10 +1670,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -1626,10 +1708,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -1664,10 +1746,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -1702,10 +1784,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1740,10 +1822,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -1778,10 +1860,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -1813,13 +1895,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -1851,13 +1933,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -1872,30 +1954,30 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.2788995520575487</v>
+        <v>-0.1023234355858201</v>
       </c>
       <c r="J18">
-        <v>0.2008903265397131</v>
+        <v>0.6377328900501884</v>
       </c>
       <c r="K18">
-        <v>0.3302413141237342</v>
+        <v>-0.1215783580010781</v>
       </c>
       <c r="L18">
-        <v>0.2115824618683086</v>
+        <v>0.6537671093538482</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1910,15 +1992,91 @@
         <v>16</v>
       </c>
       <c r="I19">
+        <v>-0.01461763365511715</v>
+      </c>
+      <c r="J19">
+        <v>0.94636892512424</v>
+      </c>
+      <c r="K19">
+        <v>-0.01736833685729687</v>
+      </c>
+      <c r="L19">
+        <v>0.949096032737041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>0.2788995520575487</v>
+      </c>
+      <c r="J20">
+        <v>0.2008903265397131</v>
+      </c>
+      <c r="K20">
+        <v>0.3302413141237342</v>
+      </c>
+      <c r="L20">
+        <v>0.2115824618683086</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
         <v>-0.2484997721369916</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>0.2528129010164081</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>-0.2952617265740468</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>0.2669012522950682</v>
       </c>
     </row>
@@ -1929,7 +2087,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1995,10 +2153,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2033,10 +2191,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -2071,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -2109,10 +2267,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -2147,10 +2305,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -2185,10 +2343,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -2223,10 +2381,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -2261,10 +2419,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2299,10 +2457,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -2337,10 +2495,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -2375,10 +2533,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -2413,10 +2571,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -2439,10 +2597,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -2465,10 +2623,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -2491,10 +2649,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -2514,13 +2672,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -2552,13 +2710,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -2573,30 +2731,30 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.3404532748240978</v>
+        <v>0.08475793795260131</v>
       </c>
       <c r="J18">
-        <v>0.1131965364706231</v>
+        <v>0.6923284900281212</v>
       </c>
       <c r="K18">
-        <v>0.4029530171380015</v>
+        <v>0.1099316484014564</v>
       </c>
       <c r="L18">
-        <v>0.1217337691688223</v>
+        <v>0.685265005536689</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -2611,15 +2769,91 @@
         <v>16</v>
       </c>
       <c r="I19">
+        <v>0.08475793795260131</v>
+      </c>
+      <c r="J19">
+        <v>0.6923284900281212</v>
+      </c>
+      <c r="K19">
+        <v>0.1099316484014564</v>
+      </c>
+      <c r="L19">
+        <v>0.685265005536689</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>0.3404532748240978</v>
+      </c>
+      <c r="J20">
+        <v>0.1131965364706231</v>
+      </c>
+      <c r="K20">
+        <v>0.4029530171380015</v>
+      </c>
+      <c r="L20">
+        <v>0.1217337691688223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
         <v>-0.01695158759052026</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>0.9369217280976989</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>-0.03834824944236852</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>0.8878693028318899</v>
       </c>
     </row>
@@ -2630,7 +2864,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2696,10 +2930,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2722,10 +2956,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -2748,10 +2982,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -2774,10 +3008,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -2800,10 +3034,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -2826,10 +3060,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -2852,10 +3086,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -2878,10 +3112,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2916,10 +3150,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -2954,10 +3188,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -2992,10 +3226,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -3030,10 +3264,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -3068,10 +3302,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -3106,10 +3340,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -3144,10 +3378,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -3179,13 +3413,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -3205,13 +3439,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -3228,27 +3462,79 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19">
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
metric name changes and generating the plots again
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="36">
   <si>
     <t>metric</t>
   </si>
@@ -28,7 +28,7 @@
     <t>metric_type</t>
   </si>
   <si>
-    <t>higher_warnings</t>
+    <t>expected_cor</t>
   </si>
   <si>
     <t>num_snippets_judged</t>
@@ -64,13 +64,13 @@
     <t>time_to_give_output</t>
   </si>
   <si>
-    <t>brain_act_31ant</t>
+    <t>brain_deact_31ant</t>
   </si>
   <si>
-    <t>brain_act_31post</t>
+    <t>brain_deact_31post</t>
   </si>
   <si>
-    <t>brain_act_32</t>
+    <t>brain_deact_32</t>
   </si>
   <si>
     <t>time_to_understand</t>
@@ -100,10 +100,7 @@
     <t>perc_correct_output</t>
   </si>
   <si>
-    <t>something_ba31</t>
-  </si>
-  <si>
-    <t>something_ba32</t>
+    <t>brain_deact_31</t>
   </si>
   <si>
     <t>complexity_level</t>
@@ -124,10 +121,10 @@
     <t>physiological</t>
   </si>
   <si>
-    <t>lower</t>
+    <t>negative</t>
   </si>
   <si>
-    <t>higher</t>
+    <t>positive</t>
   </si>
 </sst>
 </file>
@@ -494,7 +491,7 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
@@ -551,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -589,10 +586,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -627,10 +624,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -665,10 +662,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -703,10 +700,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -741,10 +738,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -779,10 +776,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -817,10 +814,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -844,7 +841,7 @@
         <v>-0.3250508508876161</v>
       </c>
       <c r="L9">
-        <v>0.0009677863595653327</v>
+        <v>0.0009677863595653331</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -855,10 +852,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -893,10 +890,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -931,10 +928,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -958,7 +955,7 @@
         <v>-0.3109097018922294</v>
       </c>
       <c r="L12">
-        <v>0.02797470554846711</v>
+        <v>0.0279747055484671</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -969,10 +966,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -1007,10 +1004,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1034,7 +1031,7 @@
         <v>0.3426469504890525</v>
       </c>
       <c r="L14">
-        <v>0.06380076796503868</v>
+        <v>0.06380076796503871</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1045,10 +1042,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -1072,7 +1069,7 @@
         <v>0.3230358829236744</v>
       </c>
       <c r="L15">
-        <v>0.08165110179558877</v>
+        <v>0.08165110179558879</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1083,10 +1080,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -1118,13 +1115,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -1156,13 +1153,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -1191,16 +1188,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1229,16 +1226,16 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20">
         <v>16</v>
@@ -1270,13 +1267,13 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -1319,7 +1316,7 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
@@ -1376,10 +1373,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -1414,10 +1411,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -1452,10 +1449,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -1490,10 +1487,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -1516,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -1542,10 +1539,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -1568,10 +1565,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1594,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1632,10 +1629,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -1670,10 +1667,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -1708,10 +1705,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -1746,10 +1743,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -1784,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1811,7 +1808,7 @@
         <v>0.2478732543966922</v>
       </c>
       <c r="L14">
-        <v>0.1866046727680992</v>
+        <v>0.1866046727680993</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1822,10 +1819,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -1849,7 +1846,7 @@
         <v>0.2516395234999386</v>
       </c>
       <c r="L15">
-        <v>0.1797825804394816</v>
+        <v>0.1797825804394817</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1860,10 +1857,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -1895,13 +1892,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -1933,13 +1930,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -1968,16 +1965,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -2006,16 +2003,16 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20">
         <v>16</v>
@@ -2047,13 +2044,13 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -2096,7 +2093,7 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
@@ -2153,10 +2150,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2191,10 +2188,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -2229,10 +2226,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -2267,10 +2264,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -2305,10 +2302,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -2343,10 +2340,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -2381,10 +2378,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -2419,10 +2416,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2457,10 +2454,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -2495,10 +2492,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -2533,10 +2530,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -2571,10 +2568,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -2597,10 +2594,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -2623,10 +2620,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -2649,10 +2646,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -2672,13 +2669,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -2710,13 +2707,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -2745,16 +2742,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -2783,16 +2780,16 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20">
         <v>16</v>
@@ -2824,13 +2821,13 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -2873,7 +2870,7 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
@@ -2930,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2956,10 +2953,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -2982,10 +2979,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -3008,10 +3005,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -3034,10 +3031,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -3060,10 +3057,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -3086,10 +3083,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -3112,10 +3109,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -3150,10 +3147,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -3188,10 +3185,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -3226,10 +3223,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -3264,10 +3261,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -3302,10 +3299,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -3340,10 +3337,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -3367,7 +3364,7 @@
         <v>0.3381406097030425</v>
       </c>
       <c r="L15">
-        <v>0.06760452162982369</v>
+        <v>0.06760452162982368</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3378,10 +3375,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -3413,13 +3410,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -3439,13 +3436,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -3462,16 +3459,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -3488,16 +3485,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20">
         <v>16</v>
@@ -3517,13 +3514,13 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>16</v>

</xml_diff>

<commit_message>
Add openjml to pipeline
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -11,13 +11,14 @@
     <sheet name="checker_framework" sheetId="2" r:id="rId2"/>
     <sheet name="typestate_checker" sheetId="3" r:id="rId3"/>
     <sheet name="infer" sheetId="4" r:id="rId4"/>
+    <sheet name="openjml" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="36">
   <si>
     <t>metric</t>
   </si>
@@ -557,25 +558,25 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G2">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.09266821663323266</v>
+        <v>-0.3377277477430254</v>
       </c>
       <c r="J2">
-        <v>0.5984721667632871</v>
+        <v>0.03761941401427579</v>
       </c>
       <c r="K2">
-        <v>-0.1263163607514111</v>
+        <v>-0.3976802252851466</v>
       </c>
       <c r="L2">
-        <v>0.5657528992105718</v>
+        <v>0.06021635626528627</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -595,25 +596,25 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.1259696449729016</v>
+        <v>-0.4275482906928738</v>
       </c>
       <c r="J3">
-        <v>0.4679676774681618</v>
+        <v>0.007641040482277836</v>
       </c>
       <c r="K3">
-        <v>-0.1721605113945802</v>
+        <v>-0.5452867412432369</v>
       </c>
       <c r="L3">
-        <v>0.4321598963432832</v>
+        <v>0.007124393687845218</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -633,25 +634,25 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G4">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.09719878783949158</v>
+        <v>0.4111706600105638</v>
       </c>
       <c r="J4">
-        <v>0.5729099316418407</v>
+        <v>0.00982101261512518</v>
       </c>
       <c r="K4">
-        <v>0.1360629871783227</v>
+        <v>0.5360003171861121</v>
       </c>
       <c r="L4">
-        <v>0.5358931384723264</v>
+        <v>0.008382091244079634</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -671,25 +672,25 @@
         <v>12</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.1113404428537808</v>
+        <v>-0.3133397807202561</v>
       </c>
       <c r="J5">
-        <v>0.6639079018776488</v>
+        <v>0.1884699909010059</v>
       </c>
       <c r="K5">
-        <v>-0.131013944022344</v>
+        <v>-0.3178304128441319</v>
       </c>
       <c r="L5">
-        <v>0.6848487144273757</v>
+        <v>0.3140610795011266</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -709,25 +710,25 @@
         <v>12</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.2597943666588219</v>
+        <v>-0.4526019054848143</v>
       </c>
       <c r="J6">
-        <v>0.3106354563374008</v>
+        <v>0.05748353173133636</v>
       </c>
       <c r="K6">
-        <v>-0.3056992027188027</v>
+        <v>-0.4693542143163343</v>
       </c>
       <c r="L6">
-        <v>0.3338931364506602</v>
+        <v>0.1237049815910057</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -747,25 +748,25 @@
         <v>12</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.1113404428537808</v>
+        <v>-0.3829708431025352</v>
       </c>
       <c r="J7">
-        <v>0.6639079018776488</v>
+        <v>0.1079738014574666</v>
       </c>
       <c r="K7">
-        <v>0.131013944022344</v>
+        <v>-0.458267106891539</v>
       </c>
       <c r="L7">
-        <v>0.6848487144273757</v>
+        <v>0.1340598783554668</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -785,25 +786,25 @@
         <v>12</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H8">
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.2597943666588219</v>
+        <v>0.1392621247645583</v>
       </c>
       <c r="J8">
-        <v>0.3106354563374008</v>
+        <v>0.5588858290416201</v>
       </c>
       <c r="K8">
-        <v>-0.3056992027188027</v>
+        <v>0.2032636361212471</v>
       </c>
       <c r="L8">
-        <v>0.3338931364506602</v>
+        <v>0.5263323724525723</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -841,7 +842,7 @@
         <v>-0.3250508508876161</v>
       </c>
       <c r="L9">
-        <v>0.0009677863595653331</v>
+        <v>0.0009677863595653327</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -955,7 +956,7 @@
         <v>-0.3109097018922294</v>
       </c>
       <c r="L12">
-        <v>0.0279747055484671</v>
+        <v>0.02797470554846711</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1031,7 +1032,7 @@
         <v>0.3426469504890525</v>
       </c>
       <c r="L14">
-        <v>0.06380076796503871</v>
+        <v>0.06380076796503868</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1069,7 +1070,7 @@
         <v>0.3230358829236744</v>
       </c>
       <c r="L15">
-        <v>0.08165110179558879</v>
+        <v>0.08165110179558877</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1127,25 +1128,25 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G17">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H17">
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.3495310368212778</v>
+        <v>-0.2196940145524359</v>
       </c>
       <c r="J17">
-        <v>0.1036923833375111</v>
+        <v>0.2645867247825571</v>
       </c>
       <c r="K17">
-        <v>-0.4089908982453269</v>
+        <v>-0.2568550273540878</v>
       </c>
       <c r="L17">
-        <v>0.1157240968299579</v>
+        <v>0.3368928901528164</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1165,25 +1166,25 @@
         <v>16</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G18">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H18">
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.1661757475835969</v>
+        <v>-0.1265427670608828</v>
       </c>
       <c r="J18">
-        <v>0.4347470349719929</v>
+        <v>0.5166373798159882</v>
       </c>
       <c r="K18">
-        <v>-0.1825328747844451</v>
+        <v>-0.2199433808439152</v>
       </c>
       <c r="L18">
-        <v>0.4986441746860601</v>
+        <v>0.4130696420709956</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1203,25 +1204,25 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G19">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H19">
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-0.08947924869885987</v>
+        <v>-0.1988529196671015</v>
       </c>
       <c r="J19">
-        <v>0.6740550539155759</v>
+        <v>0.3081411014502622</v>
       </c>
       <c r="K19">
-        <v>-0.09515011557912563</v>
+        <v>-0.2711630722733202</v>
       </c>
       <c r="L19">
-        <v>0.7259456900683131</v>
+        <v>0.3096934708383859</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1241,25 +1242,25 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H20">
         <v>16</v>
       </c>
       <c r="I20">
-        <v>0.3337450085962236</v>
+        <v>0.3176833675690128</v>
       </c>
       <c r="J20">
-        <v>0.117961265079868</v>
+        <v>0.1046269459601092</v>
       </c>
       <c r="K20">
-        <v>0.393511869842908</v>
+        <v>0.383676673960822</v>
       </c>
       <c r="L20">
-        <v>0.1315591494441377</v>
+        <v>0.1423607195218297</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1279,25 +1280,25 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G21">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H21">
         <v>16</v>
       </c>
       <c r="I21">
-        <v>-0.0639137490706142</v>
+        <v>-0.1084652289093281</v>
       </c>
       <c r="J21">
-        <v>0.7638561357920776</v>
+        <v>0.5782865569224829</v>
       </c>
       <c r="K21">
-        <v>-0.08738275920531946</v>
+        <v>-0.1340750746240306</v>
       </c>
       <c r="L21">
-        <v>0.7476087951382137</v>
+        <v>0.6205705178760341</v>
       </c>
     </row>
   </sheetData>
@@ -1808,7 +1809,7 @@
         <v>0.2478732543966922</v>
       </c>
       <c r="L14">
-        <v>0.1866046727680993</v>
+        <v>0.1866046727680992</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1846,7 +1847,7 @@
         <v>0.2516395234999386</v>
       </c>
       <c r="L15">
-        <v>0.1797825804394817</v>
+        <v>0.1797825804394816</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3364,7 +3365,7 @@
         <v>0.3381406097030425</v>
       </c>
       <c r="L15">
-        <v>0.06760452162982368</v>
+        <v>0.06760452162982369</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3533,6 +3534,735 @@
       </c>
       <c r="H21">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>-0.2588600915717736</v>
+      </c>
+      <c r="J2">
+        <v>0.1185826134820492</v>
+      </c>
+      <c r="K2">
+        <v>-0.3049516074443383</v>
+      </c>
+      <c r="L2">
+        <v>0.157096814687567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>-0.3630554894720564</v>
+      </c>
+      <c r="J3">
+        <v>0.02649782086730554</v>
+      </c>
+      <c r="K3">
+        <v>-0.4471228632493155</v>
+      </c>
+      <c r="L3">
+        <v>0.03242678547292783</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>0.3826849293392768</v>
+      </c>
+      <c r="J4">
+        <v>0.01856470797931634</v>
+      </c>
+      <c r="K4">
+        <v>0.4532739558663172</v>
+      </c>
+      <c r="L4">
+        <v>0.0298421137496698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>-0.2018433569398328</v>
+      </c>
+      <c r="J5">
+        <v>0.4065712940338708</v>
+      </c>
+      <c r="K5">
+        <v>-0.2056848110006326</v>
+      </c>
+      <c r="L5">
+        <v>0.521309719682044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>-0.2385421491107114</v>
+      </c>
+      <c r="J6">
+        <v>0.326671088638757</v>
+      </c>
+      <c r="K6">
+        <v>-0.2437745908155646</v>
+      </c>
+      <c r="L6">
+        <v>0.4451488240391529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>-0.4954336943068622</v>
+      </c>
+      <c r="J7">
+        <v>0.0416368567827736</v>
+      </c>
+      <c r="K7">
+        <v>-0.5561107852980067</v>
+      </c>
+      <c r="L7">
+        <v>0.06043495620092659</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>0.3486385256233475</v>
+      </c>
+      <c r="J8">
+        <v>0.1517044197305971</v>
+      </c>
+      <c r="K8">
+        <v>0.4037516660382788</v>
+      </c>
+      <c r="L8">
+        <v>0.1930534976448194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>66</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>-0.04742586610203935</v>
+      </c>
+      <c r="J17">
+        <v>0.8133897137921887</v>
+      </c>
+      <c r="K17">
+        <v>-0.05516439735389509</v>
+      </c>
+      <c r="L17">
+        <v>0.8392040637204297</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>66</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18">
+        <v>-0.2341464528954235</v>
+      </c>
+      <c r="J18">
+        <v>0.2394610678736877</v>
+      </c>
+      <c r="K18">
+        <v>-0.3941803537221308</v>
+      </c>
+      <c r="L18">
+        <v>0.1308460784849121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>66</v>
+      </c>
+      <c r="H19">
+        <v>16</v>
+      </c>
+      <c r="I19">
+        <v>-0.3465367502852268</v>
+      </c>
+      <c r="J19">
+        <v>0.08168784200947533</v>
+      </c>
+      <c r="K19">
+        <v>-0.4659884026560074</v>
+      </c>
+      <c r="L19">
+        <v>0.06887392462117192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>0.2069128189347872</v>
+      </c>
+      <c r="J20">
+        <v>0.3001633609183921</v>
+      </c>
+      <c r="K20">
+        <v>0.2324012320436338</v>
+      </c>
+      <c r="L20">
+        <v>0.386409849065194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <v>66</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
+        <v>0.009365858115816941</v>
+      </c>
+      <c r="J21">
+        <v>0.9624706702182941</v>
+      </c>
+      <c r="K21">
+        <v>0.02597312408246599</v>
+      </c>
+      <c r="L21">
+        <v>0.9239334339869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue parsing openjml
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -1128,25 +1128,25 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H17">
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.2196940145524359</v>
+        <v>-0.1647705109143269</v>
       </c>
       <c r="J17">
-        <v>0.2645867247825571</v>
+        <v>0.4027546538976249</v>
       </c>
       <c r="K17">
-        <v>-0.2568550273540878</v>
+        <v>-0.2341913484699036</v>
       </c>
       <c r="L17">
-        <v>0.3368928901528164</v>
+        <v>0.3826574736700414</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1166,25 +1166,25 @@
         <v>16</v>
       </c>
       <c r="F18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H18">
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.1265427670608828</v>
+        <v>-0.1626978433639921</v>
       </c>
       <c r="J18">
-        <v>0.5166373798159882</v>
+        <v>0.4043745903773081</v>
       </c>
       <c r="K18">
-        <v>-0.2199433808439152</v>
+        <v>-0.2500726110965064</v>
       </c>
       <c r="L18">
-        <v>0.4130696420709956</v>
+        <v>0.3502469232913418</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1204,10 +1204,10 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H19">
         <v>16</v>
@@ -1219,10 +1219,10 @@
         <v>0.3081411014502622</v>
       </c>
       <c r="K19">
-        <v>-0.2711630722733202</v>
+        <v>-0.2741759952985793</v>
       </c>
       <c r="L19">
-        <v>0.3096934708383859</v>
+        <v>0.3041353554760347</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1242,25 +1242,25 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H20">
         <v>16</v>
       </c>
       <c r="I20">
-        <v>0.3176833675690128</v>
+        <v>0.3721433734379864</v>
       </c>
       <c r="J20">
-        <v>0.1046269459601092</v>
+        <v>0.05729901570416417</v>
       </c>
       <c r="K20">
-        <v>0.383676673960822</v>
+        <v>0.443979491086295</v>
       </c>
       <c r="L20">
-        <v>0.1423607195218297</v>
+        <v>0.08493122100226924</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1280,25 +1280,25 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H21">
         <v>16</v>
       </c>
       <c r="I21">
-        <v>-0.1084652289093281</v>
+        <v>-0.1265427670608828</v>
       </c>
       <c r="J21">
-        <v>0.5782865569224829</v>
+        <v>0.5166373798159882</v>
       </c>
       <c r="K21">
-        <v>-0.1340750746240306</v>
+        <v>-0.159684920338733</v>
       </c>
       <c r="L21">
-        <v>0.6205705178760341</v>
+        <v>0.554695992273345</v>
       </c>
     </row>
   </sheetData>
@@ -3557,7 +3557,7 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
@@ -4092,25 +4092,25 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G17">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="H17">
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.04742586610203935</v>
+        <v>0.03774256780481986</v>
       </c>
       <c r="J17">
-        <v>0.8133897137921887</v>
+        <v>0.8508111952177798</v>
       </c>
       <c r="K17">
-        <v>-0.05516439735389509</v>
+        <v>0.06715718224198458</v>
       </c>
       <c r="L17">
-        <v>0.8392040637204297</v>
+        <v>0.8048182163992386</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -4130,25 +4130,25 @@
         <v>16</v>
       </c>
       <c r="F18">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G18">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="H18">
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-0.2341464528954235</v>
+        <v>-0.2608745973749755</v>
       </c>
       <c r="J18">
-        <v>0.2394610678736877</v>
+        <v>0.189459515366179</v>
       </c>
       <c r="K18">
-        <v>-0.3941803537221308</v>
+        <v>-0.3941471994340144</v>
       </c>
       <c r="L18">
-        <v>0.1308460784849121</v>
+        <v>0.1308813812945024</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -4168,25 +4168,25 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G19">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="H19">
         <v>16</v>
       </c>
       <c r="I19">
-        <v>-0.3465367502852268</v>
+        <v>-0.3540440964374667</v>
       </c>
       <c r="J19">
-        <v>0.08168784200947533</v>
+        <v>0.07494263177455186</v>
       </c>
       <c r="K19">
-        <v>-0.4659884026560074</v>
+        <v>-0.4534975499279393</v>
       </c>
       <c r="L19">
-        <v>0.06887392462117192</v>
+        <v>0.07768807638224377</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -4206,25 +4206,25 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G20">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="H20">
         <v>16</v>
       </c>
       <c r="I20">
-        <v>0.2069128189347872</v>
+        <v>0.14034022285596</v>
       </c>
       <c r="J20">
-        <v>0.3001633609183921</v>
+        <v>0.481699512487204</v>
       </c>
       <c r="K20">
-        <v>0.2324012320436338</v>
+        <v>0.1568611789958072</v>
       </c>
       <c r="L20">
-        <v>0.386409849065194</v>
+        <v>0.5618076700772363</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -4244,25 +4244,25 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G21">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="H21">
         <v>16</v>
       </c>
       <c r="I21">
-        <v>0.009365858115816941</v>
+        <v>0.07453559924999299</v>
       </c>
       <c r="J21">
-        <v>0.9624706702182941</v>
+        <v>0.7077285315990198</v>
       </c>
       <c r="K21">
-        <v>0.02597312408246599</v>
+        <v>0.07913380065856659</v>
       </c>
       <c r="L21">
-        <v>0.9239334339869</v>
+        <v>0.770810224273788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add dataset 9 to openjml output
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -976,25 +976,25 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="H13">
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.1668825406867738</v>
+        <v>-0.3546780165447971</v>
       </c>
       <c r="J13">
-        <v>0.2550672974746294</v>
+        <v>0.01262159666689494</v>
       </c>
       <c r="K13">
-        <v>-0.2023907691537807</v>
+        <v>-0.4463770963226328</v>
       </c>
       <c r="L13">
-        <v>0.2834571786891915</v>
+        <v>0.01341282859891604</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1014,25 +1014,25 @@
         <v>30</v>
       </c>
       <c r="F14">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="H14">
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.2791309202017375</v>
+        <v>0.2846501884412231</v>
       </c>
       <c r="J14">
-        <v>0.05845574211659071</v>
+        <v>0.04660031288457147</v>
       </c>
       <c r="K14">
-        <v>0.3426469504890525</v>
+        <v>0.3544834006793617</v>
       </c>
       <c r="L14">
-        <v>0.06380076796503868</v>
+        <v>0.05460272238348809</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1052,25 +1052,25 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="H15">
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.2664954118305773</v>
+        <v>0.2886751345948129</v>
       </c>
       <c r="J15">
-        <v>0.06971859781714017</v>
+        <v>0.04276947240054693</v>
       </c>
       <c r="K15">
-        <v>0.3230358829236744</v>
+        <v>0.3717143584291471</v>
       </c>
       <c r="L15">
-        <v>0.08165110179558877</v>
+        <v>0.04311672358740608</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1090,25 +1090,25 @@
         <v>30</v>
       </c>
       <c r="F16">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G16">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="H16">
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.1130105839368017</v>
+        <v>-0.3462790510727774</v>
       </c>
       <c r="J16">
-        <v>0.4404006981390032</v>
+        <v>0.01478142552429735</v>
       </c>
       <c r="K16">
-        <v>-0.1377826417184593</v>
+        <v>-0.4190867990009841</v>
       </c>
       <c r="L16">
-        <v>0.4677936200616143</v>
+        <v>0.02115728721848806</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3988,13 +3988,25 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H13">
         <v>30</v>
+      </c>
+      <c r="I13">
+        <v>-0.1306708482007147</v>
+      </c>
+      <c r="J13">
+        <v>0.3581258439224645</v>
+      </c>
+      <c r="K13">
+        <v>-0.2011840434130176</v>
+      </c>
+      <c r="L13">
+        <v>0.2863985630278126</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -4014,13 +4026,25 @@
         <v>30</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H14">
         <v>30</v>
+      </c>
+      <c r="I14">
+        <v>0.04028068704356932</v>
+      </c>
+      <c r="J14">
+        <v>0.7782565834710006</v>
+      </c>
+      <c r="K14">
+        <v>0.06082851254261235</v>
+      </c>
+      <c r="L14">
+        <v>0.7494911940114868</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4040,13 +4064,25 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H15">
         <v>30</v>
+      </c>
+      <c r="I15">
+        <v>0.08553337321327789</v>
+      </c>
+      <c r="J15">
+        <v>0.5483178177462631</v>
+      </c>
+      <c r="K15">
+        <v>0.1166847704091495</v>
+      </c>
+      <c r="L15">
+        <v>0.5391786637186142</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4066,13 +4102,25 @@
         <v>30</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H16">
         <v>30</v>
+      </c>
+      <c r="I16">
+        <v>-0.2077674306436665</v>
+      </c>
+      <c r="J16">
+        <v>0.1435729559776537</v>
+      </c>
+      <c r="K16">
+        <v>-0.2975516272906987</v>
+      </c>
+      <c r="L16">
+        <v>0.1102840897457505</v>
       </c>
     </row>
     <row r="17" spans="1:12">

</xml_diff>

<commit_message>
Updated corr results w/ openjml DS6 and DS9
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -988,22 +988,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.09938079899999065</v>
+        <v>0.04969039949999533</v>
       </c>
       <c r="J13">
-        <v>0.7062891119569397</v>
+        <v>0.8509806870320558</v>
       </c>
       <c r="K13">
-        <v>-0.06968868015165987</v>
+        <v>0.1010313640565443</v>
       </c>
       <c r="L13">
-        <v>0.8482942034406975</v>
+        <v>0.7812359924917622</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1026,22 +1026,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>0.298142396999972</v>
+        <v>0.3975231959999626</v>
       </c>
       <c r="J14">
-        <v>0.2582513949765453</v>
+        <v>0.1328549557310538</v>
       </c>
       <c r="K14">
-        <v>0.3357727316398157</v>
+        <v>0.4925278997756535</v>
       </c>
       <c r="L14">
-        <v>0.3428560322348787</v>
+        <v>0.148112135570859</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1064,22 +1064,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.3768891807222046</v>
+        <v>0.4773929622481257</v>
       </c>
       <c r="J15">
-        <v>0.1561291134052561</v>
+        <v>0.07328176503287165</v>
       </c>
       <c r="K15">
-        <v>0.4543553478314664</v>
+        <v>0.5890324631280877</v>
       </c>
       <c r="L15">
-        <v>0.1871125622408251</v>
+        <v>0.07317267760755417</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1102,22 +1102,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.4472135954999579</v>
+        <v>-0.4969039949999532</v>
       </c>
       <c r="J16">
-        <v>0.08992365050871301</v>
+        <v>0.06028917399060209</v>
       </c>
       <c r="K16">
-        <v>-0.5511741066540372</v>
+        <v>-0.5304146612968577</v>
       </c>
       <c r="L16">
-        <v>0.0986527259376493</v>
+        <v>0.1147392659290222</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1140,22 +1140,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.661693159884427</v>
+        <v>-0.6956655929999345</v>
       </c>
       <c r="J17">
-        <v>0.01156677640268989</v>
+        <v>0.008534920414227074</v>
       </c>
       <c r="K17">
-        <v>-0.8244866123205524</v>
+        <v>-0.8335087534664906</v>
       </c>
       <c r="L17">
-        <v>0.00333957523903813</v>
+        <v>0.002735455303093727</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1178,22 +1178,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.1715500784885551</v>
+        <v>0.04969039949999533</v>
       </c>
       <c r="J18">
-        <v>0.5126907602619233</v>
+        <v>0.8509806870320558</v>
       </c>
       <c r="K18">
-        <v>0.2328702645485529</v>
+        <v>0.02525784101413608</v>
       </c>
       <c r="L18">
-        <v>0.5173333174409258</v>
+        <v>0.9447837074747326</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1216,22 +1216,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.1487044791289829</v>
+        <v>0.07537783614444091</v>
       </c>
       <c r="J19">
-        <v>0.5733257059222834</v>
+        <v>0.7773295263554205</v>
       </c>
       <c r="K19">
-        <v>0.1830755546106544</v>
+        <v>0.04433577679458724</v>
       </c>
       <c r="L19">
-        <v>0.612677125327764</v>
+        <v>0.9032059022108545</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1254,22 +1254,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.122535770348968</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>0.6400636806234301</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>-0.1132882368074041</v>
+        <v>0.01262892050706804</v>
       </c>
       <c r="L20">
-        <v>0.7553381169763804</v>
+        <v>0.9723786419920799</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1292,22 +1292,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.5185449728701348</v>
+        <v>-0.4969039949999532</v>
       </c>
       <c r="J21">
-        <v>0.04460971802493961</v>
+        <v>0.06028917399060209</v>
       </c>
       <c r="K21">
-        <v>-0.6646940512883968</v>
+        <v>-0.631446025353402</v>
       </c>
       <c r="L21">
-        <v>0.0360103690823689</v>
+        <v>0.05021407909522695</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1330,22 +1330,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.4714045207910317</v>
+        <v>0.5962847939999439</v>
       </c>
       <c r="J22">
-        <v>0.06788915486182899</v>
+        <v>0.02417054717454525</v>
       </c>
       <c r="K22">
-        <v>0.6893123494842632</v>
+        <v>0.7198484689028782</v>
       </c>
       <c r="L22">
-        <v>0.02744606731217235</v>
+        <v>0.01890477781850608</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1368,22 +1368,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.4714045207910317</v>
+        <v>0.5465943944999486</v>
       </c>
       <c r="J23">
-        <v>0.06788915486182899</v>
+        <v>0.03877750439230662</v>
       </c>
       <c r="K23">
-        <v>0.6646940512883968</v>
+        <v>0.6945906278887423</v>
       </c>
       <c r="L23">
-        <v>0.0360103690823689</v>
+        <v>0.0258112209674474</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1406,22 +1406,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.7071067811865475</v>
+        <v>-0.6956655929999345</v>
       </c>
       <c r="J24">
-        <v>0.00616989932054416</v>
+        <v>0.008534920414227074</v>
       </c>
       <c r="K24">
-        <v>-0.8370221386594626</v>
+        <v>-0.8208798329594226</v>
       </c>
       <c r="L24">
-        <v>0.002523052086935284</v>
+        <v>0.003605943791192453</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5117,25 +5117,25 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.0967301666813349</v>
+        <v>0.04969039949999533</v>
       </c>
       <c r="J13">
-        <v>0.7095485176052034</v>
+        <v>0.8509806870320558</v>
       </c>
       <c r="K13">
-        <v>-0.1442864351352195</v>
+        <v>0.01262892050706804</v>
       </c>
       <c r="L13">
-        <v>0.6908626476513942</v>
+        <v>0.9723786419920799</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -5155,25 +5155,25 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.1450952500220024</v>
+        <v>-0.149071198499986</v>
       </c>
       <c r="J14">
-        <v>0.5763707320629909</v>
+        <v>0.5730251193553904</v>
       </c>
       <c r="K14">
-        <v>-0.1944730212692089</v>
+        <v>-0.1894338076060206</v>
       </c>
       <c r="L14">
-        <v>0.5903173590239674</v>
+        <v>0.6001664342511973</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -5193,25 +5193,25 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.1222789970111296</v>
+        <v>-0.1256297269074015</v>
       </c>
       <c r="J15">
-        <v>0.6402909885089358</v>
+        <v>0.6374017405958849</v>
       </c>
       <c r="K15">
-        <v>-0.1289946138007723</v>
+        <v>-0.152008377581442</v>
       </c>
       <c r="L15">
-        <v>0.7224728853135778</v>
+        <v>0.6750590889374006</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -5231,25 +5231,25 @@
         <v>10</v>
       </c>
       <c r="F16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.2901905000440047</v>
+        <v>-0.298142396999972</v>
       </c>
       <c r="J16">
-        <v>0.2638286605798634</v>
+        <v>0.2596563563704499</v>
       </c>
       <c r="K16">
-        <v>-0.4140393356054125</v>
+        <v>-0.3788676152120412</v>
       </c>
       <c r="L16">
-        <v>0.2342354559095551</v>
+        <v>0.2802942824523375</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -5269,25 +5269,25 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.2205643866281423</v>
+        <v>-0.1987615979999813</v>
       </c>
       <c r="J17">
-        <v>0.399957255078591</v>
+        <v>0.4523703606773608</v>
       </c>
       <c r="K17">
-        <v>-0.4028026197596592</v>
+        <v>-0.3409808536908371</v>
       </c>
       <c r="L17">
-        <v>0.2484528477817244</v>
+        <v>0.3349456951179903</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -5307,25 +5307,25 @@
         <v>10</v>
       </c>
       <c r="F18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.2695786947677295</v>
+        <v>0.149071198499986</v>
       </c>
       <c r="J18">
-        <v>0.3036011712333525</v>
+        <v>0.5730251193553904</v>
       </c>
       <c r="K18">
-        <v>0.3650398741571911</v>
+        <v>0.1641759665918845</v>
       </c>
       <c r="L18">
-        <v>0.2996444166144334</v>
+        <v>0.6503895621649565</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -5345,25 +5345,25 @@
         <v>10</v>
       </c>
       <c r="F19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.1982726388386439</v>
+        <v>0.07537783614444091</v>
       </c>
       <c r="J19">
-        <v>0.4527246044153628</v>
+        <v>0.7773295263554205</v>
       </c>
       <c r="K19">
-        <v>0.2588309565185115</v>
+        <v>0.1076726007868547</v>
       </c>
       <c r="L19">
-        <v>0.4702381281221487</v>
+        <v>0.7671778789420547</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5383,25 +5383,25 @@
         <v>10</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.1715500784885551</v>
+        <v>-0.09938079899999065</v>
       </c>
       <c r="J20">
-        <v>0.5126907602619233</v>
+        <v>0.7071142312899612</v>
       </c>
       <c r="K20">
-        <v>-0.2328702645485529</v>
+        <v>-0.1262892050706804</v>
       </c>
       <c r="L20">
-        <v>0.5173333174409258</v>
+        <v>0.7281063840216824</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5421,25 +5421,25 @@
         <v>10</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2771739468734333</v>
+        <v>-0.149071198499986</v>
       </c>
       <c r="J21">
-        <v>0.2978975979923409</v>
+        <v>0.5730251193553904</v>
       </c>
       <c r="K21">
-        <v>-0.3432465321284133</v>
+        <v>-0.2399494896342928</v>
       </c>
       <c r="L21">
-        <v>0.3315340291730248</v>
+        <v>0.5043017190353258</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -5459,25 +5459,25 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G22">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.5291502622129181</v>
+        <v>0.3975231959999626</v>
       </c>
       <c r="J22">
-        <v>0.0468921588647849</v>
+        <v>0.1328549557310538</v>
       </c>
       <c r="K22">
-        <v>0.6864930642568265</v>
+        <v>0.5304146612968577</v>
       </c>
       <c r="L22">
-        <v>0.02834764584094183</v>
+        <v>0.1147392659290222</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -5497,25 +5497,25 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G23">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.4787549991450212</v>
+        <v>0.298142396999972</v>
       </c>
       <c r="J23">
-        <v>0.07217560549492458</v>
+        <v>0.2596563563704499</v>
       </c>
       <c r="K23">
-        <v>0.5975032225939045</v>
+        <v>0.4041254562261773</v>
       </c>
       <c r="L23">
-        <v>0.06812982343660752</v>
+        <v>0.2467547295422347</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5535,25 +5535,25 @@
         <v>10</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G24">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.4283597360771242</v>
+        <v>-0.2484519974999766</v>
       </c>
       <c r="J24">
-        <v>0.1076721642577082</v>
+        <v>0.347558036741169</v>
       </c>
       <c r="K24">
-        <v>-0.5975032225939045</v>
+        <v>-0.4293832972403134</v>
       </c>
       <c r="L24">
-        <v>0.06812982343660752</v>
+        <v>0.2155824117700313</v>
       </c>
     </row>
     <row r="25" spans="1:12">

</xml_diff>

<commit_message>
updated corr results with DS6 in openjml
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1562DC7-0C5A-0F47-9D29-3CAAC5A3D591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -19,26 +13,7 @@
     <sheet name="infer" sheetId="4" r:id="rId4"/>
     <sheet name="openjml" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_tools!$A$1:$L$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">checker_framework!$A$1:$L$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">infer!$A$1:$L$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">openjml!$A$1:$L$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">typestate_checker!$A$1:$L$21</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -105,31 +80,31 @@
     <t>readability_level</t>
   </si>
   <si>
-    <t>correct_verif_questions</t>
+    <t>binary_understandability</t>
   </si>
   <si>
-    <t>binary_understandability</t>
+    <t>correct_verif_questions</t>
   </si>
   <si>
     <t>gap_accuracy</t>
   </si>
   <si>
+    <t>readability_level_ba</t>
+  </si>
+  <si>
     <t>readability_level_before</t>
   </si>
   <si>
-    <t>readability_level_ba</t>
-  </si>
-  <si>
     <t>time_to_read_complete</t>
-  </si>
-  <si>
-    <t>perc_correct_output</t>
   </si>
   <si>
     <t>brain_deact_31</t>
   </si>
   <si>
     <t>complexity_level</t>
+  </si>
+  <si>
+    <t>perc_correct_output</t>
   </si>
   <si>
     <t>f</t>
@@ -156,8 +131,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,14 +195,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -274,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,27 +273,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,24 +307,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -551,27 +482,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="12" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -635,19 +567,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.33772774774302539</v>
+        <v>-0.3377277477430254</v>
       </c>
       <c r="J2">
-        <v>3.7619414014275793E-2</v>
+        <v>0.03761941401427579</v>
       </c>
       <c r="K2">
-        <v>-0.39768022528514663</v>
+        <v>-0.3976802252851466</v>
       </c>
       <c r="L2">
-        <v>6.0216356265286271E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.06021635626528627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -673,19 +605,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.42754829069287381</v>
+        <v>-0.4275482906928738</v>
       </c>
       <c r="J3">
-        <v>7.6410404822778357E-3</v>
+        <v>0.007641040482277836</v>
       </c>
       <c r="K3">
-        <v>-0.54528674124323695</v>
+        <v>-0.5452867412432369</v>
       </c>
       <c r="L3">
-        <v>7.124393687845218E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.007124393687845218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -711,19 +643,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.41117066001056379</v>
+        <v>0.4111706600105638</v>
       </c>
       <c r="J4">
-        <v>9.8210126151251805E-3</v>
+        <v>0.00982101261512518</v>
       </c>
       <c r="K4">
-        <v>0.53600031718611207</v>
+        <v>0.5360003171861121</v>
       </c>
       <c r="L4">
-        <v>8.3820912440796345E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.008382091244079634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -749,19 +681,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.31333978072025609</v>
+        <v>-0.3133397807202561</v>
       </c>
       <c r="J5">
-        <v>0.18846999090100591</v>
+        <v>0.1884699909010059</v>
       </c>
       <c r="K5">
-        <v>-0.31783041284413188</v>
+        <v>-0.3178304128441319</v>
       </c>
       <c r="L5">
-        <v>0.31406107950112661</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3140610795011266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -787,19 +719,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.45260190548481433</v>
+        <v>-0.4526019054848143</v>
       </c>
       <c r="J6">
-        <v>5.7483531731336357E-2</v>
+        <v>0.05748353173133636</v>
       </c>
       <c r="K6">
-        <v>-0.46935421431633428</v>
+        <v>-0.4693542143163343</v>
       </c>
       <c r="L6">
-        <v>0.12370498159100569</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1237049815910057</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -825,19 +757,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.38297084310253521</v>
+        <v>-0.3829708431025352</v>
       </c>
       <c r="J7">
         <v>0.1079738014574666</v>
       </c>
       <c r="K7">
-        <v>-0.45826710689153899</v>
+        <v>-0.458267106891539</v>
       </c>
       <c r="L7">
-        <v>0.13405987835546679</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1340598783554668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -863,19 +795,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.13926212476455829</v>
+        <v>0.1392621247645583</v>
       </c>
       <c r="J8">
         <v>0.5588858290416201</v>
       </c>
       <c r="K8">
-        <v>0.20326363612124709</v>
+        <v>0.2032636361212471</v>
       </c>
       <c r="L8">
-        <v>0.52633237245257225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.5263323724525723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -901,21 +833,21 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.22964462414024381</v>
+        <v>-0.2296446241402438</v>
       </c>
       <c r="J9">
-        <v>1.3810859520988481E-3</v>
+        <v>0.001381085952098848</v>
       </c>
       <c r="K9">
-        <v>-0.32505085088761609</v>
+        <v>-0.3250508508876161</v>
       </c>
       <c r="L9">
-        <v>9.6778635956533269E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.0009677863595653327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -930,30 +862,30 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G10">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-2.1865071526333869E-2</v>
+        <v>-0.02584053907657639</v>
       </c>
       <c r="J10">
-        <v>0.85746045357848777</v>
+        <v>0.8319012317886401</v>
       </c>
       <c r="K10">
-        <v>-2.3705418235251699E-2</v>
+        <v>-0.02491868767248899</v>
       </c>
       <c r="L10">
-        <v>0.87019890091340346</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8636170341288709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -968,28 +900,28 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G11">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-2.8152946873129591E-2</v>
+        <v>-0.02439922062337898</v>
       </c>
       <c r="J11">
-        <v>0.80868009561069343</v>
+        <v>0.8337884478927275</v>
       </c>
       <c r="K11">
-        <v>-2.915890758270907E-2</v>
+        <v>-0.02888208251072132</v>
       </c>
       <c r="L11">
-        <v>0.84068897194493819</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8421820698041393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1006,28 +938,28 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G12">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.24788466776030799</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J12">
-        <v>3.1887928946905821E-2</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K12">
-        <v>-0.31090970189222938</v>
+        <v>-0.311094163299463</v>
       </c>
       <c r="L12">
-        <v>2.7974705548467111E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.02787696039183273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1053,21 +985,21 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.35467801654479708</v>
+        <v>-0.3546780165447971</v>
       </c>
       <c r="J13">
-        <v>1.2621596666894941E-2</v>
+        <v>0.01262159666689494</v>
       </c>
       <c r="K13">
-        <v>-0.44637709632263278</v>
+        <v>-0.4463770963226328</v>
       </c>
       <c r="L13">
-        <v>1.341282859891604E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.01341282859891604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -1091,21 +1023,21 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.28867513459481292</v>
+        <v>0.2886751345948129</v>
       </c>
       <c r="J14">
-        <v>4.2769472400546932E-2</v>
+        <v>0.04276947240054693</v>
       </c>
       <c r="K14">
-        <v>0.37171435842914707</v>
+        <v>0.3717143584291471</v>
       </c>
       <c r="L14">
-        <v>4.3116723587406078E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.04311672358740608</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1129,19 +1061,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.28465018844122308</v>
+        <v>0.2846501884412231</v>
       </c>
       <c r="J15">
-        <v>4.660031288457147E-2</v>
+        <v>0.04660031288457147</v>
       </c>
       <c r="K15">
-        <v>0.35448340067936168</v>
+        <v>0.3544834006793617</v>
       </c>
       <c r="L15">
-        <v>5.4602722383488088E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.05460272238348809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1170,18 +1102,18 @@
         <v>-0.3462790510727774</v>
       </c>
       <c r="J16">
-        <v>1.4781425524297349E-2</v>
+        <v>0.01478142552429735</v>
       </c>
       <c r="K16">
-        <v>-0.41908679900098411</v>
+        <v>-0.4190867990009841</v>
       </c>
       <c r="L16">
-        <v>2.1157287218488061E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.02115728721848806</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1208,16 +1140,16 @@
         <v>-0.1626978433639921</v>
       </c>
       <c r="J17">
-        <v>0.40437459037730811</v>
+        <v>0.4043745903773081</v>
       </c>
       <c r="K17">
-        <v>-0.25007261109650641</v>
+        <v>-0.2500726110965064</v>
       </c>
       <c r="L17">
-        <v>0.35024692329134183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3502469232913418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1246,18 +1178,18 @@
         <v>-0.1988529196671015</v>
       </c>
       <c r="J18">
-        <v>0.30814110145026219</v>
+        <v>0.3081411014502622</v>
       </c>
       <c r="K18">
-        <v>-0.27417599529857928</v>
+        <v>-0.2741759952985793</v>
       </c>
       <c r="L18">
-        <v>0.30413535547603471</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3041353554760347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -1281,21 +1213,21 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.37214337343798642</v>
+        <v>0.3721433734379864</v>
       </c>
       <c r="J19">
-        <v>5.7299015704164173E-2</v>
+        <v>0.05729901570416417</v>
       </c>
       <c r="K19">
-        <v>0.44397949108629498</v>
+        <v>0.443979491086295</v>
       </c>
       <c r="L19">
-        <v>8.4931221002269242E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.08493122100226924</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1322,16 +1254,16 @@
         <v>-0.1647705109143269</v>
       </c>
       <c r="J20">
-        <v>0.40275465389762488</v>
+        <v>0.4027546538976249</v>
       </c>
       <c r="K20">
-        <v>-0.23419134846990361</v>
+        <v>-0.2341913484699036</v>
       </c>
       <c r="L20">
-        <v>0.38265747367004138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3826574736700414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1360,49 +1292,43 @@
         <v>-0.1265427670608828</v>
       </c>
       <c r="J21">
-        <v>0.51663737981598823</v>
+        <v>0.5166373798159882</v>
       </c>
       <c r="K21">
-        <v>-0.15968492033873299</v>
+        <v>-0.159684920338733</v>
       </c>
       <c r="L21">
-        <v>0.55469599227334498</v>
+        <v>0.554695992273345</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L21" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1440,7 +1366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1469,16 +1395,16 @@
         <v>-0.2277100170213244</v>
       </c>
       <c r="J2">
-        <v>0.20032802218695259</v>
+        <v>0.2003280221869526</v>
       </c>
       <c r="K2">
-        <v>-0.27197235029387162</v>
+        <v>-0.2719723502938716</v>
       </c>
       <c r="L2">
-        <v>0.20932509565963231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.2093250956596323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1504,19 +1430,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.26347777762091701</v>
+        <v>-0.263477777620917</v>
       </c>
       <c r="J3">
         <v>0.1329850671160174</v>
       </c>
       <c r="K3">
-        <v>-0.32017787305285961</v>
+        <v>-0.3201778730528596</v>
       </c>
       <c r="L3">
-        <v>0.13637641008504059</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1363764100850406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1545,16 +1471,16 @@
         <v>0.2297034206521828</v>
       </c>
       <c r="J4">
-        <v>0.18729084163390899</v>
+        <v>0.187290841633909</v>
       </c>
       <c r="K4">
-        <v>0.28096954242303013</v>
+        <v>0.2809695424230301</v>
       </c>
       <c r="L4">
-        <v>0.19405167261558409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1940516726155841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1580,7 +1506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1606,7 +1532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1632,7 +1558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1658,7 +1584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1684,21 +1610,21 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.22890415976703279</v>
+        <v>-0.2289041597670328</v>
       </c>
       <c r="J9">
-        <v>4.1540622048766972E-3</v>
+        <v>0.004154062204876697</v>
       </c>
       <c r="K9">
-        <v>-0.28726717466178431</v>
+        <v>-0.2872671746617843</v>
       </c>
       <c r="L9">
-        <v>3.7567205497513649E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.003756720549751365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1722,21 +1648,21 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-1.7889603976091351E-2</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J10">
-        <v>0.88317001415190322</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K10">
-        <v>-2.1745521452022229E-2</v>
+        <v>-0.02174552145202223</v>
       </c>
       <c r="L10">
-        <v>0.88084937555910936</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8808493755591094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1760,19 +1686,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-2.439922062337898E-2</v>
+        <v>-0.02439922062337898</v>
       </c>
       <c r="J11">
-        <v>0.83378844789272755</v>
+        <v>0.8337884478927275</v>
       </c>
       <c r="K11">
-        <v>-2.8051607294758089E-2</v>
+        <v>-0.02805160729475809</v>
       </c>
       <c r="L11">
-        <v>0.84666464123863983</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8466646412386398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1798,19 +1724,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.25161225674918491</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J12">
-        <v>2.940004335865699E-2</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K12">
-        <v>-0.31183200892839741</v>
+        <v>-0.3118320089283974</v>
       </c>
       <c r="L12">
-        <v>2.7488825966879269E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.02748882596687927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1839,18 +1765,18 @@
         <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.31976301166779852</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
         <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.32836965842449101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.328369658424491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -1877,18 +1803,18 @@
         <v>0.2095131203515696</v>
       </c>
       <c r="J14">
-        <v>0.17537923007396619</v>
+        <v>0.1753792300739662</v>
       </c>
       <c r="K14">
-        <v>0.25163952349993862</v>
+        <v>0.2516395234999386</v>
       </c>
       <c r="L14">
-        <v>0.17978258043948159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1797825804394816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1912,19 +1838,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.20720097246551281</v>
+        <v>0.2072009724655128</v>
       </c>
       <c r="J15">
-        <v>0.18192926663069439</v>
+        <v>0.1819292666306944</v>
       </c>
       <c r="K15">
-        <v>0.24787325439669219</v>
+        <v>0.2478732543966922</v>
       </c>
       <c r="L15">
-        <v>0.18660467276809919</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1866046727680992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1950,21 +1876,21 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-6.5246691057189277E-2</v>
+        <v>-0.06524669105718928</v>
       </c>
       <c r="J16">
-        <v>0.67205176865918925</v>
+        <v>0.6720517686591893</v>
       </c>
       <c r="K16">
-        <v>-7.8611105106096368E-2</v>
+        <v>-0.07861110510609637</v>
       </c>
       <c r="L16">
-        <v>0.67966876801064502</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.679668768010645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1988,19 +1914,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.10232343558582011</v>
+        <v>-0.1023234355858201</v>
       </c>
       <c r="J17">
-        <v>0.63773289005018841</v>
+        <v>0.6377328900501884</v>
       </c>
       <c r="K17">
-        <v>-0.12157835800107809</v>
+        <v>-0.1215783580010781</v>
       </c>
       <c r="L17">
-        <v>0.65376710935384819</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.6537671093538482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2026,21 +1952,21 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>-1.4617633655117149E-2</v>
+        <v>-0.01461763365511715</v>
       </c>
       <c r="J18">
-        <v>0.94636892512423998</v>
+        <v>0.94636892512424</v>
       </c>
       <c r="K18">
-        <v>-1.736833685729687E-2</v>
+        <v>-0.01736833685729687</v>
       </c>
       <c r="L18">
-        <v>0.94909603273704102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.949096032737041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -2064,21 +1990,21 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.27889955205754868</v>
+        <v>0.2788995520575487</v>
       </c>
       <c r="J19">
-        <v>0.20089032653971309</v>
+        <v>0.2008903265397131</v>
       </c>
       <c r="K19">
         <v>0.3302413141237342</v>
       </c>
       <c r="L19">
-        <v>0.21158246186830859</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.2115824618683086</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -2102,19 +2028,19 @@
         <v>16</v>
       </c>
       <c r="I20">
-        <v>-0.16284238361758671</v>
+        <v>-0.1628423836175867</v>
       </c>
       <c r="J20">
-        <v>0.45801098838521898</v>
+        <v>0.458010988385219</v>
       </c>
       <c r="K20">
-        <v>-0.19161611347062391</v>
+        <v>-0.1916161134706239</v>
       </c>
       <c r="L20">
         <v>0.4771333722542902</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2140,50 +2066,46 @@
         <v>16</v>
       </c>
       <c r="I21">
-        <v>-0.24849977213699159</v>
+        <v>-0.2484997721369916</v>
       </c>
       <c r="J21">
-        <v>0.25281290101640808</v>
+        <v>0.2528129010164081</v>
       </c>
       <c r="K21">
-        <v>-0.29526172657404681</v>
+        <v>-0.2952617265740468</v>
       </c>
       <c r="L21">
-        <v>0.26690125229506823</v>
+        <v>0.2669012522950682</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L21" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="12" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2247,19 +2169,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.17078251276599329</v>
+        <v>-0.1707825127659933</v>
       </c>
       <c r="J2">
         <v>0.3368221511559395</v>
       </c>
       <c r="K2">
-        <v>-0.22063279587022341</v>
+        <v>-0.2206327958702234</v>
       </c>
       <c r="L2">
-        <v>0.31170668319455619</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3117066831945562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2285,19 +2207,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.21557272714438661</v>
+        <v>-0.2155727271443866</v>
       </c>
       <c r="J3">
         <v>0.2189727791934982</v>
       </c>
       <c r="K3">
-        <v>-0.28300682710477038</v>
+        <v>-0.2830068271047704</v>
       </c>
       <c r="L3">
-        <v>0.19070138371258061</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1907013837125806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2326,16 +2248,16 @@
         <v>0.182178575000007</v>
       </c>
       <c r="J4">
-        <v>0.29564657602090749</v>
+        <v>0.2956465760209075</v>
       </c>
       <c r="K4">
-        <v>0.24046942819989059</v>
+        <v>0.2404694281998906</v>
       </c>
       <c r="L4">
-        <v>0.26904897632032188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.2690489763203219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2361,19 +2283,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.11134044285378079</v>
+        <v>-0.1113404428537808</v>
       </c>
       <c r="J5">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K5">
-        <v>-0.13101394402234401</v>
+        <v>-0.131013944022344</v>
       </c>
       <c r="L5">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2399,19 +2321,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J6">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K6">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L6">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2437,19 +2359,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.11134044285378079</v>
+        <v>0.1113404428537808</v>
       </c>
       <c r="J7">
-        <v>0.66390790187764881</v>
+        <v>0.6639079018776488</v>
       </c>
       <c r="K7">
-        <v>0.13101394402234401</v>
+        <v>0.131013944022344</v>
       </c>
       <c r="L7">
-        <v>0.68484871442737572</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.6848487144273757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2475,19 +2397,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.25979436665882188</v>
+        <v>-0.2597943666588219</v>
       </c>
       <c r="J8">
-        <v>0.31063545633740081</v>
+        <v>0.3106354563374008</v>
       </c>
       <c r="K8">
-        <v>-0.30569920271880269</v>
+        <v>-0.3056992027188027</v>
       </c>
       <c r="L8">
-        <v>0.33389313645066021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3338931364506602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2513,21 +2435,21 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459340999</v>
+        <v>-0.15625137459341</v>
       </c>
       <c r="J9">
-        <v>3.0128615488005099E-2</v>
+        <v>0.0301286154880051</v>
       </c>
       <c r="K9">
         <v>-0.2203331090972887</v>
       </c>
       <c r="L9">
-        <v>2.7610565923995401E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.0276105659239954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -2554,18 +2476,18 @@
         <v>-0.121885527067201</v>
       </c>
       <c r="J10">
-        <v>0.32625309790028828</v>
+        <v>0.3262530979002883</v>
       </c>
       <c r="K10">
-        <v>-0.14024128232502711</v>
+        <v>-0.1402412823250271</v>
       </c>
       <c r="L10">
-        <v>0.33135638533698542</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.3313563853369854</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -2589,19 +2511,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-7.3984543411941786E-2</v>
+        <v>-0.07398454341194179</v>
       </c>
       <c r="J11">
-        <v>0.53265206192351422</v>
+        <v>0.5326520619235142</v>
       </c>
       <c r="K11">
-        <v>-8.9137532819911741E-2</v>
+        <v>-0.08913753281991174</v>
       </c>
       <c r="L11">
-        <v>0.53816988278746214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.5381698827874621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2627,19 +2549,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-8.5714285714285715E-2</v>
+        <v>-0.08571428571428572</v>
       </c>
       <c r="J12">
-        <v>0.46685427082272551</v>
+        <v>0.4668542708227255</v>
       </c>
       <c r="K12">
         <v>-0.1039438393012856</v>
       </c>
       <c r="L12">
-        <v>0.47253953182670588</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.4725395318267059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2665,9 +2587,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -2691,9 +2613,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -2717,7 +2639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2743,9 +2665,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -2769,19 +2691,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>8.4757937952601309E-2</v>
+        <v>0.08475793795260131</v>
       </c>
       <c r="J17">
-        <v>0.69232849002812125</v>
+        <v>0.6923284900281212</v>
       </c>
       <c r="K17">
         <v>0.1099316484014564</v>
       </c>
       <c r="L17">
-        <v>0.68526500553668901</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.685265005536689</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2807,21 +2729,21 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>8.4757937952601309E-2</v>
+        <v>0.08475793795260131</v>
       </c>
       <c r="J18">
-        <v>0.69232849002812125</v>
+        <v>0.6923284900281212</v>
       </c>
       <c r="K18">
         <v>0.1099316484014564</v>
       </c>
       <c r="L18">
-        <v>0.68526500553668901</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.685265005536689</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -2845,21 +2767,21 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.34045327482409782</v>
+        <v>0.3404532748240978</v>
       </c>
       <c r="J19">
         <v>0.1131965364706231</v>
       </c>
       <c r="K19">
-        <v>0.40295301713800152</v>
+        <v>0.4029530171380015</v>
       </c>
       <c r="L19">
         <v>0.1217337691688223</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -2883,19 +2805,19 @@
         <v>16</v>
       </c>
       <c r="I20">
-        <v>-0.49785866253711791</v>
+        <v>-0.4978586625371179</v>
       </c>
       <c r="J20">
-        <v>2.1337320545634531E-2</v>
+        <v>0.02133732054563453</v>
       </c>
       <c r="K20">
-        <v>-0.57692307692307687</v>
+        <v>-0.5769230769230769</v>
       </c>
       <c r="L20">
-        <v>1.929785020805572E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.01929785020805572</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2921,51 +2843,46 @@
         <v>16</v>
       </c>
       <c r="I21">
-        <v>-1.6951587590520258E-2</v>
+        <v>-0.01695158759052026</v>
       </c>
       <c r="J21">
-        <v>0.93692172809769891</v>
+        <v>0.9369217280976989</v>
       </c>
       <c r="K21">
-        <v>-3.8348249442368518E-2</v>
+        <v>-0.03834824944236852</v>
       </c>
       <c r="L21">
-        <v>0.88786930283188992</v>
+        <v>0.8878693028318899</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L21" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="12" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3003,7 +2920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3029,7 +2946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3055,7 +2972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3081,7 +2998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3107,7 +3024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3133,7 +3050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3159,7 +3076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3185,7 +3102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3214,18 +3131,18 @@
         <v>-0.1325530043077417</v>
       </c>
       <c r="J9">
-        <v>0.10868264420740591</v>
+        <v>0.1086826442074059</v>
       </c>
       <c r="K9">
-        <v>-0.16122238802734751</v>
+        <v>-0.1612223880273475</v>
       </c>
       <c r="L9">
         <v>0.1090548020620709</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -3249,21 +3166,21 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-1.7966219332967059E-2</v>
+        <v>-0.01796621933296706</v>
       </c>
       <c r="J10">
-        <v>0.88314281706898357</v>
+        <v>0.8831428170689836</v>
       </c>
       <c r="K10">
-        <v>-1.9415750760330759E-2</v>
+        <v>-0.01941575076033076</v>
       </c>
       <c r="L10">
-        <v>0.89353687009819049</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8935368700981905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -3287,19 +3204,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-2.0733912312975989E-2</v>
+        <v>-0.02073391231297599</v>
       </c>
       <c r="J11">
-        <v>0.85903161553489027</v>
+        <v>0.8590316155348903</v>
       </c>
       <c r="K11">
-        <v>-2.339586347864377E-2</v>
+        <v>-0.02339586347864377</v>
       </c>
       <c r="L11">
-        <v>0.87187961817406379</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8718796181740638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3325,19 +3242,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.24894627719055901</v>
+        <v>-0.248946277190559</v>
       </c>
       <c r="J12">
-        <v>3.1843356716153078E-2</v>
+        <v>0.03184335671615308</v>
       </c>
       <c r="K12">
-        <v>-0.31078029944537922</v>
+        <v>-0.3107802994453792</v>
       </c>
       <c r="L12">
-        <v>2.8043445822604571E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.02804344582260457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3366,18 +3283,18 @@
         <v>-0.153506269493634</v>
       </c>
       <c r="J13">
-        <v>0.31976301166779852</v>
+        <v>0.3197630116677985</v>
       </c>
       <c r="K13">
         <v>-0.1847566494939108</v>
       </c>
       <c r="L13">
-        <v>0.32836965842449101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.328369658424491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -3404,18 +3321,18 @@
         <v>0.2815332554724217</v>
       </c>
       <c r="J14">
-        <v>6.8615535355580695E-2</v>
+        <v>0.0686155353555807</v>
       </c>
       <c r="K14">
-        <v>0.33814060970304249</v>
+        <v>0.3381406097030425</v>
       </c>
       <c r="L14">
-        <v>6.7604521629823694E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.06760452162982369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -3442,16 +3359,16 @@
         <v>0.3157348151855433</v>
       </c>
       <c r="J15">
-        <v>4.1947627723575583E-2</v>
+        <v>0.04194762772357558</v>
       </c>
       <c r="K15">
-        <v>0.37771162574734057</v>
+        <v>0.3777116257473406</v>
       </c>
       <c r="L15">
-        <v>3.9605634003798212E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.03960563400379821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3477,21 +3394,21 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.14354272032581639</v>
+        <v>-0.1435427203258164</v>
       </c>
       <c r="J16">
-        <v>0.35168068279855269</v>
+        <v>0.3516806827985527</v>
       </c>
       <c r="K16">
-        <v>-0.17294443123341199</v>
+        <v>-0.172944431233412</v>
       </c>
       <c r="L16">
-        <v>0.36075974854167298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.360759748541673</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -3515,7 +3432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3541,9 +3458,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -3567,9 +3484,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -3593,7 +3510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3620,39 +3537,33 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L21" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3690,7 +3601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3716,7 +3627,7 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.25886009157177359</v>
+        <v>-0.2588600915717736</v>
       </c>
       <c r="J2">
         <v>0.1185826134820492</v>
@@ -3728,7 +3639,7 @@
         <v>0.157096814687567</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3757,16 +3668,16 @@
         <v>-0.3630554894720564</v>
       </c>
       <c r="J3">
-        <v>2.6497820867305542E-2</v>
+        <v>0.02649782086730554</v>
       </c>
       <c r="K3">
-        <v>-0.44712286324931549</v>
+        <v>-0.4471228632493155</v>
       </c>
       <c r="L3">
-        <v>3.2426785472927828E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.03242678547292783</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3792,19 +3703,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.38268492933927678</v>
+        <v>0.3826849293392768</v>
       </c>
       <c r="J4">
-        <v>1.856470797931634E-2</v>
+        <v>0.01856470797931634</v>
       </c>
       <c r="K4">
-        <v>0.45327395586631719</v>
+        <v>0.4532739558663172</v>
       </c>
       <c r="L4">
-        <v>2.9842113749669798E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.0298421137496698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3833,16 +3744,16 @@
         <v>-0.2018433569398328</v>
       </c>
       <c r="J5">
-        <v>0.40657129403387082</v>
+        <v>0.4065712940338708</v>
       </c>
       <c r="K5">
         <v>-0.2056848110006326</v>
       </c>
       <c r="L5">
-        <v>0.52130971968204398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.521309719682044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3868,10 +3779,10 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.23854214911071139</v>
+        <v>-0.2385421491107114</v>
       </c>
       <c r="J6">
-        <v>0.32667108863875699</v>
+        <v>0.326671088638757</v>
       </c>
       <c r="K6">
         <v>-0.2437745908155646</v>
@@ -3880,7 +3791,7 @@
         <v>0.4451488240391529</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3906,19 +3817,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.49543369430686218</v>
+        <v>-0.4954336943068622</v>
       </c>
       <c r="J7">
-        <v>4.1636856782773603E-2</v>
+        <v>0.0416368567827736</v>
       </c>
       <c r="K7">
-        <v>-0.55611078529800673</v>
+        <v>-0.5561107852980067</v>
       </c>
       <c r="L7">
-        <v>6.0434956200926593E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.06043495620092659</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3944,19 +3855,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.34863852562334752</v>
+        <v>0.3486385256233475</v>
       </c>
       <c r="J8">
-        <v>0.15170441973059709</v>
+        <v>0.1517044197305971</v>
       </c>
       <c r="K8">
-        <v>0.40375166603827878</v>
+        <v>0.4037516660382788</v>
       </c>
       <c r="L8">
-        <v>0.19305349764481941</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1930534976448194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3982,9 +3893,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -3999,18 +3910,30 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>-0.02584053907657639</v>
+      </c>
+      <c r="J10">
+        <v>0.8319012317886401</v>
+      </c>
+      <c r="K10">
+        <v>-0.02491868767248899</v>
+      </c>
+      <c r="L10">
+        <v>0.8636170341288709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -4025,16 +3948,28 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>-0.02439922062337898</v>
+      </c>
+      <c r="J11">
+        <v>0.8337884478927275</v>
+      </c>
+      <c r="K11">
+        <v>-0.02888208251072132</v>
+      </c>
+      <c r="L11">
+        <v>0.8421820698041393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4051,16 +3986,28 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>-0.2516122567491849</v>
+      </c>
+      <c r="J12">
+        <v>0.02940004335865699</v>
+      </c>
+      <c r="K12">
+        <v>-0.311094163299463</v>
+      </c>
+      <c r="L12">
+        <v>0.02787696039183273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -4089,18 +4036,18 @@
         <v>-0.1306708482007147</v>
       </c>
       <c r="J13">
-        <v>0.35812584392246449</v>
+        <v>0.3581258439224645</v>
       </c>
       <c r="K13">
         <v>-0.2011840434130176</v>
       </c>
       <c r="L13">
-        <v>0.28639856302781258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.2863985630278126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -4124,21 +4071,21 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <v>8.5533373213277891E-2</v>
+        <v>0.08553337321327789</v>
       </c>
       <c r="J14">
-        <v>0.54831781774626309</v>
+        <v>0.5483178177462631</v>
       </c>
       <c r="K14">
         <v>0.1166847704091495</v>
       </c>
       <c r="L14">
-        <v>0.53917866371861423</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.5391786637186142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -4162,19 +4109,19 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <v>4.0280687043569317E-2</v>
+        <v>0.04028068704356932</v>
       </c>
       <c r="J15">
-        <v>0.77825658347100057</v>
+        <v>0.7782565834710006</v>
       </c>
       <c r="K15">
-        <v>6.0828512542612352E-2</v>
+        <v>0.06082851254261235</v>
       </c>
       <c r="L15">
-        <v>0.74949119401148678</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.7494911940114868</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -4200,21 +4147,21 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.20776743064366651</v>
+        <v>-0.2077674306436665</v>
       </c>
       <c r="J16">
-        <v>0.14357295597765371</v>
+        <v>0.1435729559776537</v>
       </c>
       <c r="K16">
-        <v>-0.29755162729069867</v>
+        <v>-0.2975516272906987</v>
       </c>
       <c r="L16">
         <v>0.1102840897457505</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -4238,19 +4185,19 @@
         <v>16</v>
       </c>
       <c r="I17">
-        <v>-0.26087459737497548</v>
+        <v>-0.2608745973749755</v>
       </c>
       <c r="J17">
         <v>0.189459515366179</v>
       </c>
       <c r="K17">
-        <v>-0.39414719943401438</v>
+        <v>-0.3941471994340144</v>
       </c>
       <c r="L17">
-        <v>0.13088138129450241</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.1308813812945024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -4279,18 +4226,18 @@
         <v>-0.3540440964374667</v>
       </c>
       <c r="J18">
-        <v>7.4942631774551863E-2</v>
+        <v>0.07494263177455186</v>
       </c>
       <c r="K18">
-        <v>-0.45349754992793928</v>
+        <v>-0.4534975499279393</v>
       </c>
       <c r="L18">
-        <v>7.7688076382243773E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.07768807638224377</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -4314,7 +4261,7 @@
         <v>16</v>
       </c>
       <c r="I19">
-        <v>0.14034022285596001</v>
+        <v>0.14034022285596</v>
       </c>
       <c r="J19">
         <v>0.481699512487204</v>
@@ -4323,12 +4270,12 @@
         <v>0.1568611789958072</v>
       </c>
       <c r="L19">
-        <v>0.56180767007723631</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.5618076700772363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -4352,19 +4299,19 @@
         <v>16</v>
       </c>
       <c r="I20">
-        <v>3.7742567804819861E-2</v>
+        <v>0.03774256780481986</v>
       </c>
       <c r="J20">
-        <v>0.85081119521777981</v>
+        <v>0.8508111952177798</v>
       </c>
       <c r="K20">
-        <v>6.7157182241984581E-2</v>
+        <v>0.06715718224198458</v>
       </c>
       <c r="L20">
-        <v>0.80481821639923856</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.8048182163992386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -4390,24 +4337,19 @@
         <v>16</v>
       </c>
       <c r="I21">
-        <v>7.4535599249992993E-2</v>
+        <v>0.07453559924999299</v>
       </c>
       <c r="J21">
-        <v>0.70772853159901983</v>
+        <v>0.7077285315990198</v>
       </c>
       <c r="K21">
-        <v>7.9133800658566594E-2</v>
+        <v>0.07913380065856659</v>
       </c>
       <c r="L21">
-        <v>0.77081022427378798</v>
+        <v>0.770810224273788</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L21" xr:uid="{00000000-0001-0000-0400-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated corr results DS6 now actually added
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -871,25 +871,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G10">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.02186507152633387</v>
+        <v>-0.02584053907657639</v>
       </c>
       <c r="J10">
-        <v>0.8574604535784878</v>
+        <v>0.8319012317886401</v>
       </c>
       <c r="K10">
-        <v>-0.0237054182352517</v>
+        <v>-0.02491868767248899</v>
       </c>
       <c r="L10">
-        <v>0.8701989009134035</v>
+        <v>0.8636170341288709</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -909,25 +909,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G11">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-0.02439922062337898</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.8337884478927275</v>
       </c>
       <c r="K11">
-        <v>-0.02915890758270907</v>
+        <v>-0.02888208251072132</v>
       </c>
       <c r="L11">
-        <v>0.8406889719449382</v>
+        <v>0.8421820698041393</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -947,25 +947,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G12">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.2516122567491849</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>0.02940004335865699</v>
       </c>
       <c r="K12">
-        <v>-0.3109097018922294</v>
+        <v>-0.311094163299463</v>
       </c>
       <c r="L12">
-        <v>0.02797470554846711</v>
+        <v>0.02787696039183273</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4686,9 +4686,9 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5039,13 +5039,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H10">
         <v>50</v>
+      </c>
+      <c r="I10">
+        <v>-0.02584053907657639</v>
+      </c>
+      <c r="J10">
+        <v>0.8319012317886401</v>
+      </c>
+      <c r="K10">
+        <v>-0.02491868767248899</v>
+      </c>
+      <c r="L10">
+        <v>0.8636170341288709</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5065,13 +5077,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H11">
         <v>50</v>
+      </c>
+      <c r="I11">
+        <v>-0.02439922062337898</v>
+      </c>
+      <c r="J11">
+        <v>0.8337884478927275</v>
+      </c>
+      <c r="K11">
+        <v>-0.02888208251072132</v>
+      </c>
+      <c r="L11">
+        <v>0.8421820698041393</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5091,13 +5115,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="H12">
         <v>50</v>
+      </c>
+      <c r="I12">
+        <v>-0.2516122567491849</v>
+      </c>
+      <c r="J12">
+        <v>0.02940004335865699</v>
+      </c>
+      <c r="K12">
+        <v>-0.311094163299463</v>
+      </c>
+      <c r="L12">
+        <v>0.02787696039183273</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>

<commit_message>
Add DS 3 5 min timout to corr results
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -507,7 +507,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
@@ -833,25 +833,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G9">
-        <v>392</v>
+        <v>434</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2296446241402438</v>
+        <v>-0.2151139512854704</v>
       </c>
       <c r="J9">
-        <v>0.001381085952098848</v>
+        <v>0.002586148853829074</v>
       </c>
       <c r="K9">
-        <v>-0.3250508508876161</v>
+        <v>-0.3079422632365748</v>
       </c>
       <c r="L9">
-        <v>0.0009677863595653327</v>
+        <v>0.001828155909077151</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5013,13 +5013,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H9">
         <v>100</v>
+      </c>
+      <c r="I9">
+        <v>-0.1099732420898421</v>
+      </c>
+      <c r="J9">
+        <v>0.1687963904269523</v>
+      </c>
+      <c r="K9">
+        <v>-0.1397892658934472</v>
+      </c>
+      <c r="L9">
+        <v>0.1653994232905868</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
Add DS 3 5 min timeout to corr results
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -498,9 +498,9 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -824,25 +824,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G9">
-        <v>392</v>
+        <v>434</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2296446241402438</v>
+        <v>-0.2151139512854704</v>
       </c>
       <c r="J9">
-        <v>0.001381085952098848</v>
+        <v>0.002586148853829074</v>
       </c>
       <c r="K9">
-        <v>-0.3250508508876161</v>
+        <v>-0.3079422632365748</v>
       </c>
       <c r="L9">
-        <v>0.0009677863595653327</v>
+        <v>0.001828155909077151</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3884,13 +3884,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H9">
         <v>100</v>
+      </c>
+      <c r="I9">
+        <v>-0.1099732420898421</v>
+      </c>
+      <c r="J9">
+        <v>0.1687963904269523</v>
+      </c>
+      <c r="K9">
+        <v>-0.1397892658934472</v>
+      </c>
+      <c r="L9">
+        <v>0.1653994232905868</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
Update corr results with JaTyC fixed on DS 6
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -862,25 +862,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10">
-        <v>334</v>
+        <v>819</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.02584053907657639</v>
+        <v>-0.01391413642584883</v>
       </c>
       <c r="J10">
-        <v>0.8319012317886401</v>
+        <v>0.9090032366864784</v>
       </c>
       <c r="K10">
-        <v>-0.02491868767248899</v>
+        <v>-0.01026612600739247</v>
       </c>
       <c r="L10">
-        <v>0.8636170341288709</v>
+        <v>0.9435901857829745</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -900,25 +900,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11">
-        <v>334</v>
+        <v>819</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-0.02815294687312959</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.8086800956106934</v>
       </c>
       <c r="K11">
-        <v>-0.02888208251072132</v>
+        <v>-0.0299893827986723</v>
       </c>
       <c r="L11">
-        <v>0.8421820698041393</v>
+        <v>0.8362130272367809</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -938,25 +938,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12">
-        <v>334</v>
+        <v>819</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.247884667760308</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>0.03188792894690582</v>
       </c>
       <c r="K12">
-        <v>-0.311094163299463</v>
+        <v>-0.3096184720415943</v>
       </c>
       <c r="L12">
-        <v>0.02787696039183273</v>
+        <v>0.02866696147428332</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2099,9 +2099,9 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2464,25 +2464,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G10">
-        <v>52</v>
+        <v>537</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.121885527067201</v>
+        <v>-0.01391413642584883</v>
       </c>
       <c r="J10">
-        <v>0.3262530979002883</v>
+        <v>0.9090032366864784</v>
       </c>
       <c r="K10">
-        <v>-0.1402412823250271</v>
+        <v>-0.01026612600739247</v>
       </c>
       <c r="L10">
-        <v>0.3313563853369854</v>
+        <v>0.9435901857829745</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2502,25 +2502,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>52</v>
+        <v>537</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.07398454341194179</v>
+        <v>-0.02815294687312959</v>
       </c>
       <c r="J11">
-        <v>0.5326520619235142</v>
+        <v>0.8086800956106934</v>
       </c>
       <c r="K11">
-        <v>-0.08913753281991174</v>
+        <v>-0.0299893827986723</v>
       </c>
       <c r="L11">
-        <v>0.5381698827874621</v>
+        <v>0.8362130272367809</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2540,25 +2540,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G12">
-        <v>52</v>
+        <v>537</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.08571428571428572</v>
+        <v>-0.247884667760308</v>
       </c>
       <c r="J12">
-        <v>0.4668542708227255</v>
+        <v>0.03188792894690582</v>
       </c>
       <c r="K12">
-        <v>-0.1039438393012856</v>
+        <v>-0.3096184720415943</v>
       </c>
       <c r="L12">
-        <v>0.4725395318267059</v>
+        <v>0.02866696147428332</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>

<commit_message>
Update corr results with JaTyC fixed for DS9
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -988,22 +988,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.04969039949999533</v>
+        <v>-0.4535394202249742</v>
       </c>
       <c r="J13">
-        <v>0.8509806870320558</v>
+        <v>0.08070214265077501</v>
       </c>
       <c r="K13">
-        <v>0.1010313640565443</v>
+        <v>-0.5512130501182249</v>
       </c>
       <c r="L13">
-        <v>0.7812359924917622</v>
+        <v>0.09862398123473154</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1026,22 +1026,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>0.3975231959999626</v>
+        <v>-0.02387049580131443</v>
       </c>
       <c r="J14">
-        <v>0.1328549557310538</v>
+        <v>0.92675547372309</v>
       </c>
       <c r="K14">
-        <v>0.4925278997756535</v>
+        <v>-0.09290107586262218</v>
       </c>
       <c r="L14">
-        <v>0.148112135570859</v>
+        <v>0.7985237548304135</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1064,22 +1064,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.4773929622481257</v>
+        <v>0.09656090991705352</v>
       </c>
       <c r="J15">
-        <v>0.07328176503287165</v>
+        <v>0.7120793980044939</v>
       </c>
       <c r="K15">
-        <v>0.5890324631280877</v>
+        <v>0.1428819499477476</v>
       </c>
       <c r="L15">
-        <v>0.07317267760755417</v>
+        <v>0.6937488280957302</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1102,22 +1102,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.4969039949999532</v>
+        <v>-0.7399853698407473</v>
       </c>
       <c r="J16">
-        <v>0.06028917399060209</v>
+        <v>0.004375235749920733</v>
       </c>
       <c r="K16">
-        <v>-0.5304146612968577</v>
+        <v>-0.8670767080511405</v>
       </c>
       <c r="L16">
-        <v>0.1147392659290222</v>
+        <v>0.001159768265192443</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1140,22 +1140,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.6956655929999345</v>
+        <v>-0.3103164454170876</v>
       </c>
       <c r="J17">
-        <v>0.008534920414227074</v>
+        <v>0.2320634889020341</v>
       </c>
       <c r="K17">
-        <v>-0.8335087534664906</v>
+        <v>-0.4149581388530457</v>
       </c>
       <c r="L17">
-        <v>0.002735455303093727</v>
+        <v>0.233093730241445</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1178,22 +1178,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.04969039949999533</v>
+        <v>0.4535394202249742</v>
       </c>
       <c r="J18">
-        <v>0.8509806870320558</v>
+        <v>0.08070214265077501</v>
       </c>
       <c r="K18">
-        <v>0.02525784101413608</v>
+        <v>0.5635998602332413</v>
       </c>
       <c r="L18">
-        <v>0.9447837074747326</v>
+        <v>0.08974939558201678</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1216,22 +1216,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.07537783614444091</v>
+        <v>0.4828045495852675</v>
       </c>
       <c r="J19">
-        <v>0.7773295263554205</v>
+        <v>0.06499039472076076</v>
       </c>
       <c r="K19">
-        <v>0.04433577679458724</v>
+        <v>0.5932707052178214</v>
       </c>
       <c r="L19">
-        <v>0.9032059022108545</v>
+        <v>0.0706202179291523</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1254,22 +1254,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>-0.3580574370197164</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0.1679207532945924</v>
       </c>
       <c r="K20">
-        <v>0.01262892050706804</v>
+        <v>-0.4954724046006516</v>
       </c>
       <c r="L20">
-        <v>0.9723786419920799</v>
+        <v>0.1453294522910624</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1292,22 +1292,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.4969039949999532</v>
+        <v>-0.4535394202249742</v>
       </c>
       <c r="J21">
-        <v>0.06028917399060209</v>
+        <v>0.08070214265077501</v>
       </c>
       <c r="K21">
-        <v>-0.631446025353402</v>
+        <v>-0.6007602905782901</v>
       </c>
       <c r="L21">
-        <v>0.05021407909522695</v>
+        <v>0.06625295074379814</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1330,22 +1330,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.5962847939999439</v>
+        <v>0.1193524790065721</v>
       </c>
       <c r="J22">
-        <v>0.02417054717454525</v>
+        <v>0.6457756768370824</v>
       </c>
       <c r="K22">
-        <v>0.7198484689028782</v>
+        <v>0.1486417213801955</v>
       </c>
       <c r="L22">
-        <v>0.01890477781850608</v>
+        <v>0.6819355638686473</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1368,22 +1368,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.5465943944999486</v>
+        <v>0.167093470609201</v>
       </c>
       <c r="J23">
-        <v>0.03877750439230662</v>
+        <v>0.5199036173455835</v>
       </c>
       <c r="K23">
-        <v>0.6945906278887423</v>
+        <v>0.2725098225303584</v>
       </c>
       <c r="L23">
-        <v>0.0258112209674474</v>
+        <v>0.446215643690079</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1406,22 +1406,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.6956655929999345</v>
+        <v>-0.3580574370197164</v>
       </c>
       <c r="J24">
-        <v>0.008534920414227074</v>
+        <v>0.1679207532945924</v>
       </c>
       <c r="K24">
-        <v>-0.8208798329594226</v>
+        <v>-0.4706987843706191</v>
       </c>
       <c r="L24">
-        <v>0.003605943791192453</v>
+        <v>0.1697475039817557</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -3195,13 +3195,25 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H13">
         <v>10</v>
+      </c>
+      <c r="I13">
+        <v>-0.4787549991450212</v>
+      </c>
+      <c r="J13">
+        <v>0.07217560549492458</v>
+      </c>
+      <c r="K13">
+        <v>-0.6292853089020909</v>
+      </c>
+      <c r="L13">
+        <v>0.05124855216842294</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3221,13 +3233,25 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H14">
         <v>10</v>
+      </c>
+      <c r="I14">
+        <v>-0.2267786838055363</v>
+      </c>
+      <c r="J14">
+        <v>0.3943870594034554</v>
+      </c>
+      <c r="K14">
+        <v>-0.2860387767736777</v>
+      </c>
+      <c r="L14">
+        <v>0.4230203924441358</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3247,13 +3271,25 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H15">
         <v>10</v>
+      </c>
+      <c r="I15">
+        <v>-0.1019294382875251</v>
+      </c>
+      <c r="J15">
+        <v>0.7040542681897126</v>
+      </c>
+      <c r="K15">
+        <v>-0.0765092055676006</v>
+      </c>
+      <c r="L15">
+        <v>0.8336123677972922</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3273,13 +3309,25 @@
         <v>10</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H16">
         <v>10</v>
+      </c>
+      <c r="I16">
+        <v>-0.579545525280815</v>
+      </c>
+      <c r="J16">
+        <v>0.02951512807757192</v>
+      </c>
+      <c r="K16">
+        <v>-0.7119187333033755</v>
+      </c>
+      <c r="L16">
+        <v>0.02091481468718881</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3299,13 +3347,25 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H17">
         <v>10</v>
+      </c>
+      <c r="I17">
+        <v>-0.1259881576697424</v>
+      </c>
+      <c r="J17">
+        <v>0.6360988735986226</v>
+      </c>
+      <c r="K17">
+        <v>-0.1906925178491184</v>
+      </c>
+      <c r="L17">
+        <v>0.5977007516614028</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3325,13 +3385,25 @@
         <v>10</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H18">
         <v>10</v>
+      </c>
+      <c r="I18">
+        <v>0.579545525280815</v>
+      </c>
+      <c r="J18">
+        <v>0.02951512807757192</v>
+      </c>
+      <c r="K18">
+        <v>0.7437008196115621</v>
+      </c>
+      <c r="L18">
+        <v>0.01366958411527145</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -3351,13 +3423,25 @@
         <v>10</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H19">
         <v>10</v>
+      </c>
+      <c r="I19">
+        <v>0.560611910581388</v>
+      </c>
+      <c r="J19">
+        <v>0.0366903087793031</v>
+      </c>
+      <c r="K19">
+        <v>0.7172738021962557</v>
+      </c>
+      <c r="L19">
+        <v>0.01954204435368506</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3377,13 +3461,25 @@
         <v>10</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H20">
         <v>10</v>
+      </c>
+      <c r="I20">
+        <v>-0.4787549991450212</v>
+      </c>
+      <c r="J20">
+        <v>0.07217560549492458</v>
+      </c>
+      <c r="K20">
+        <v>-0.6419981434253655</v>
+      </c>
+      <c r="L20">
+        <v>0.04536158917864154</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3403,13 +3499,25 @@
         <v>10</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H21">
         <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.2771739468734333</v>
+      </c>
+      <c r="J21">
+        <v>0.2978975979923409</v>
+      </c>
+      <c r="K21">
+        <v>-0.3750286184365996</v>
+      </c>
+      <c r="L21">
+        <v>0.2855969029688312</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -3429,13 +3537,25 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H22">
         <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.1259881576697424</v>
+      </c>
+      <c r="J22">
+        <v>0.6360988735986226</v>
+      </c>
+      <c r="K22">
+        <v>0.1461975970176575</v>
+      </c>
+      <c r="L22">
+        <v>0.6869410188538527</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3455,13 +3575,25 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H23">
         <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.1259881576697424</v>
+      </c>
+      <c r="J23">
+        <v>0.6360988735986226</v>
+      </c>
+      <c r="K23">
+        <v>0.2161181868956676</v>
+      </c>
+      <c r="L23">
+        <v>0.5487107060733141</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3481,13 +3613,25 @@
         <v>10</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H24">
         <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.2267786838055363</v>
+      </c>
+      <c r="J24">
+        <v>0.3943870594034554</v>
+      </c>
+      <c r="K24">
+        <v>-0.3114644458202268</v>
+      </c>
+      <c r="L24">
+        <v>0.3810089567050594</v>
       </c>
     </row>
     <row r="25" spans="1:12">

</xml_diff>

<commit_message>
Update corr results with JaTyC working on DS9
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -498,9 +498,9 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -979,22 +979,22 @@
         <v>30</v>
       </c>
       <c r="G13">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="H13">
         <v>30</v>
       </c>
       <c r="I13">
-        <v>-0.3546780165447971</v>
+        <v>-0.4048169271682026</v>
       </c>
       <c r="J13">
-        <v>0.01262159666689494</v>
+        <v>0.003684245901134024</v>
       </c>
       <c r="K13">
-        <v>-0.4463770963226328</v>
+        <v>-0.5344276234347691</v>
       </c>
       <c r="L13">
-        <v>0.01341282859891604</v>
+        <v>0.002348131666704992</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1017,22 +1017,22 @@
         <v>30</v>
       </c>
       <c r="G14">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="H14">
         <v>30</v>
       </c>
       <c r="I14">
-        <v>0.2886751345948129</v>
+        <v>0.1515153313763357</v>
       </c>
       <c r="J14">
-        <v>0.04276947240054693</v>
+        <v>0.2780537029565812</v>
       </c>
       <c r="K14">
-        <v>0.3717143584291471</v>
+        <v>0.2312941947390607</v>
       </c>
       <c r="L14">
-        <v>0.04311672358740608</v>
+        <v>0.2187797748162401</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1055,22 +1055,22 @@
         <v>30</v>
       </c>
       <c r="G15">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="H15">
         <v>30</v>
       </c>
       <c r="I15">
-        <v>0.2846501884412231</v>
+        <v>0.2373626514505708</v>
       </c>
       <c r="J15">
-        <v>0.04660031288457147</v>
+        <v>0.09051426625460415</v>
       </c>
       <c r="K15">
-        <v>0.3544834006793617</v>
+        <v>0.3315718656719684</v>
       </c>
       <c r="L15">
-        <v>0.05460272238348809</v>
+        <v>0.07346214270566978</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1093,22 +1093,22 @@
         <v>30</v>
       </c>
       <c r="G16">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="H16">
         <v>30</v>
       </c>
       <c r="I16">
-        <v>-0.3462790510727774</v>
+        <v>-0.3966737953014234</v>
       </c>
       <c r="J16">
-        <v>0.01478142552429735</v>
+        <v>0.004392923006413007</v>
       </c>
       <c r="K16">
-        <v>-0.4190867990009841</v>
+        <v>-0.5638269314967141</v>
       </c>
       <c r="L16">
-        <v>0.02115728721848806</v>
+        <v>0.001175300429566541</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2578,13 +2578,25 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="H13">
         <v>30</v>
+      </c>
+      <c r="I13">
+        <v>-0.3137312989174262</v>
+      </c>
+      <c r="J13">
+        <v>0.02848639994432931</v>
+      </c>
+      <c r="K13">
+        <v>-0.4131284275634866</v>
+      </c>
+      <c r="L13">
+        <v>0.02326314515800765</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2604,13 +2616,25 @@
         <v>30</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="H14">
         <v>30</v>
+      </c>
+      <c r="I14">
+        <v>0.14638501094228</v>
+      </c>
+      <c r="J14">
+        <v>0.3077335885571051</v>
+      </c>
+      <c r="K14">
+        <v>0.2212047859710532</v>
+      </c>
+      <c r="L14">
+        <v>0.2401033542701417</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2630,13 +2654,25 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="H15">
         <v>30</v>
+      </c>
+      <c r="I15">
+        <v>0.2124307787987451</v>
+      </c>
+      <c r="J15">
+        <v>0.1403732278087201</v>
+      </c>
+      <c r="K15">
+        <v>0.2913831605167395</v>
+      </c>
+      <c r="L15">
+        <v>0.1182228233126965</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2656,13 +2692,25 @@
         <v>30</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="H16">
         <v>30</v>
+      </c>
+      <c r="I16">
+        <v>-0.3809072222823607</v>
+      </c>
+      <c r="J16">
+        <v>0.007761477051653751</v>
+      </c>
+      <c r="K16">
+        <v>-0.5322611581053379</v>
+      </c>
+      <c r="L16">
+        <v>0.002464998415486295</v>
       </c>
     </row>
     <row r="17" spans="1:12">

</xml_diff>

<commit_message>
Corr results are same after merge
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="39">
   <si>
     <t>metric</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>perc_correct_output</t>
+  </si>
+  <si>
+    <t>9_gc</t>
+  </si>
+  <si>
+    <t>9_bc</t>
+  </si>
+  <si>
+    <t>9_nc</t>
   </si>
   <si>
     <t>f</t>
@@ -483,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,7 +507,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
@@ -549,10 +558,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -587,10 +596,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -625,10 +634,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -663,10 +672,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -701,10 +710,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -739,10 +748,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -777,10 +786,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -815,10 +824,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -853,10 +862,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -891,10 +900,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -929,10 +938,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -963,341 +972,645 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9</v>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4048169271682026</v>
+        <v>-0.4535394202249742</v>
       </c>
       <c r="J13">
-        <v>0.003684245901134024</v>
+        <v>0.08070214265077501</v>
       </c>
       <c r="K13">
-        <v>-0.5344276234347691</v>
+        <v>-0.5512130501182249</v>
       </c>
       <c r="L13">
-        <v>0.002348131666704992</v>
+        <v>0.09862398123473154</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>0.1515153313763357</v>
+        <v>-0.02387049580131443</v>
       </c>
       <c r="J14">
-        <v>0.2780537029565812</v>
+        <v>0.92675547372309</v>
       </c>
       <c r="K14">
-        <v>0.2312941947390607</v>
+        <v>-0.09290107586262218</v>
       </c>
       <c r="L14">
-        <v>0.2187797748162401</v>
+        <v>0.7985237548304135</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>9</v>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>0.2373626514505708</v>
+        <v>0.09656090991705352</v>
       </c>
       <c r="J15">
-        <v>0.09051426625460415</v>
+        <v>0.7120793980044939</v>
       </c>
       <c r="K15">
-        <v>0.3315718656719684</v>
+        <v>0.1428819499477476</v>
       </c>
       <c r="L15">
-        <v>0.07346214270566978</v>
+        <v>0.6937488280957302</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.3966737953014234</v>
+        <v>-0.7399853698407473</v>
       </c>
       <c r="J16">
-        <v>0.004392923006413007</v>
+        <v>0.004375235749920733</v>
       </c>
       <c r="K16">
-        <v>-0.5638269314967141</v>
+        <v>-0.8670767080511405</v>
       </c>
       <c r="L16">
-        <v>0.001175300429566541</v>
+        <v>0.001159768265192443</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1626978433639921</v>
+        <v>-0.3103164454170876</v>
       </c>
       <c r="J17">
-        <v>0.4043745903773081</v>
+        <v>0.2320634889020341</v>
       </c>
       <c r="K17">
-        <v>-0.2500726110965064</v>
+        <v>-0.4149581388530457</v>
       </c>
       <c r="L17">
-        <v>0.3502469232913418</v>
+        <v>0.233093730241445</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.1988529196671015</v>
+        <v>0.4535394202249742</v>
       </c>
       <c r="J18">
-        <v>0.3081411014502622</v>
+        <v>0.08070214265077501</v>
       </c>
       <c r="K18">
-        <v>-0.2741759952985793</v>
+        <v>0.5635998602332413</v>
       </c>
       <c r="L18">
-        <v>0.3041353554760347</v>
+        <v>0.08974939558201678</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>0.3721433734379864</v>
+        <v>0.4828045495852675</v>
       </c>
       <c r="J19">
-        <v>0.05729901570416417</v>
+        <v>0.06499039472076076</v>
       </c>
       <c r="K19">
-        <v>0.443979491086295</v>
+        <v>0.5932707052178214</v>
       </c>
       <c r="L19">
-        <v>0.08493122100226924</v>
+        <v>0.0706202179291523</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.1647705109143269</v>
+        <v>-0.3580574370197164</v>
       </c>
       <c r="J20">
-        <v>0.4027546538976249</v>
+        <v>0.1679207532945924</v>
       </c>
       <c r="K20">
-        <v>-0.2341913484699036</v>
+        <v>-0.4954724046006516</v>
       </c>
       <c r="L20">
-        <v>0.3826574736700414</v>
+        <v>0.1453294522910624</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>73</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.4535394202249742</v>
+      </c>
+      <c r="J21">
+        <v>0.08070214265077501</v>
+      </c>
+      <c r="K21">
+        <v>-0.6007602905782901</v>
+      </c>
+      <c r="L21">
+        <v>0.06625295074379814</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>73</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.1193524790065721</v>
+      </c>
+      <c r="J22">
+        <v>0.6457756768370824</v>
+      </c>
+      <c r="K22">
+        <v>0.1486417213801955</v>
+      </c>
+      <c r="L22">
+        <v>0.6819355638686473</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>73</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.167093470609201</v>
+      </c>
+      <c r="J23">
+        <v>0.5199036173455835</v>
+      </c>
+      <c r="K23">
+        <v>0.2725098225303584</v>
+      </c>
+      <c r="L23">
+        <v>0.446215643690079</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>73</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.3580574370197164</v>
+      </c>
+      <c r="J24">
+        <v>0.1679207532945924</v>
+      </c>
+      <c r="K24">
+        <v>-0.4706987843706191</v>
+      </c>
+      <c r="L24">
+        <v>0.1697475039817557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>39</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>-0.1626978433639921</v>
+      </c>
+      <c r="J25">
+        <v>0.4043745903773081</v>
+      </c>
+      <c r="K25">
+        <v>-0.2500726110965064</v>
+      </c>
+      <c r="L25">
+        <v>0.3502469232913418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>39</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>-0.1988529196671015</v>
+      </c>
+      <c r="J26">
+        <v>0.3081411014502622</v>
+      </c>
+      <c r="K26">
+        <v>-0.2741759952985793</v>
+      </c>
+      <c r="L26">
+        <v>0.3041353554760347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>39</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.3721433734379864</v>
+      </c>
+      <c r="J27">
+        <v>0.05729901570416417</v>
+      </c>
+      <c r="K27">
+        <v>0.443979491086295</v>
+      </c>
+      <c r="L27">
+        <v>0.08493122100226924</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>15</v>
+      </c>
+      <c r="G28">
+        <v>39</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>-0.1647705109143269</v>
+      </c>
+      <c r="J28">
+        <v>0.4027546538976249</v>
+      </c>
+      <c r="K28">
+        <v>-0.2341913484699036</v>
+      </c>
+      <c r="L28">
+        <v>0.3826574736700414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="E21">
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>15</v>
       </c>
-      <c r="G21">
+      <c r="G29">
         <v>39</v>
       </c>
-      <c r="H21">
+      <c r="H29">
         <v>16</v>
       </c>
-      <c r="I21">
+      <c r="I29">
         <v>-0.1265427670608828</v>
       </c>
-      <c r="J21">
+      <c r="J29">
         <v>0.5166373798159882</v>
       </c>
-      <c r="K21">
+      <c r="K29">
         <v>-0.159684920338733</v>
       </c>
-      <c r="L21">
+      <c r="L29">
         <v>0.554695992273345</v>
       </c>
     </row>
@@ -1308,7 +1621,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1374,10 +1687,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -1412,10 +1725,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -1450,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -1488,10 +1801,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -1514,10 +1827,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -1540,10 +1853,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -1566,10 +1879,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1592,10 +1905,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1630,10 +1943,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -1668,10 +1981,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -1706,10 +2019,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -1740,341 +2053,645 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9</v>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.153506269493634</v>
+        <v>0.3651483716701108</v>
       </c>
       <c r="J13">
-        <v>0.3197630116677985</v>
+        <v>0.2008251226951454</v>
       </c>
       <c r="K13">
-        <v>-0.1847566494939108</v>
+        <v>0.4264014327112208</v>
       </c>
       <c r="L13">
-        <v>0.328369658424491</v>
+        <v>0.2191383605228726</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>0.2095131203515696</v>
+        <v>0.7302967433402215</v>
       </c>
       <c r="J14">
-        <v>0.1753792300739662</v>
+        <v>0.01051524593585891</v>
       </c>
       <c r="K14">
-        <v>0.2516395234999386</v>
+        <v>0.8528028654224417</v>
       </c>
       <c r="L14">
-        <v>0.1797825804394816</v>
+        <v>0.001712874149321468</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>9</v>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>0.2072009724655128</v>
+        <v>0.7385489458759965</v>
       </c>
       <c r="J15">
-        <v>0.1819292666306944</v>
+        <v>0.01028204822194895</v>
       </c>
       <c r="K15">
-        <v>0.2478732543966922</v>
+        <v>0.8553989227683017</v>
       </c>
       <c r="L15">
-        <v>0.1866046727680992</v>
+        <v>0.001600453316805279</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.06524669105718928</v>
+        <v>-0.1217161238900369</v>
       </c>
       <c r="J16">
-        <v>0.6720517686591893</v>
+        <v>0.6698153575994166</v>
       </c>
       <c r="K16">
-        <v>-0.07861110510609637</v>
+        <v>-0.1421338109037403</v>
       </c>
       <c r="L16">
-        <v>0.679668768010645</v>
+        <v>0.6952876854012655</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1023234355858201</v>
+        <v>-0.5477225575051662</v>
       </c>
       <c r="J17">
-        <v>0.6377328900501884</v>
+        <v>0.05500883362926572</v>
       </c>
       <c r="K17">
-        <v>-0.1215783580010781</v>
+        <v>-0.6396021490668313</v>
       </c>
       <c r="L17">
-        <v>0.6537671093538482</v>
+        <v>0.04643461767158175</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.01461763365511715</v>
+        <v>-0.3651483716701108</v>
       </c>
       <c r="J18">
-        <v>0.94636892512424</v>
+        <v>0.2008251226951454</v>
       </c>
       <c r="K18">
-        <v>-0.01736833685729687</v>
+        <v>-0.4264014327112208</v>
       </c>
       <c r="L18">
-        <v>0.949096032737041</v>
+        <v>0.2191383605228726</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>0.2788995520575487</v>
+        <v>-0.3077287274483319</v>
       </c>
       <c r="J19">
-        <v>0.2008903265397131</v>
+        <v>0.2849576406684299</v>
       </c>
       <c r="K19">
-        <v>0.3302413141237342</v>
+        <v>-0.3564162178201257</v>
       </c>
       <c r="L19">
-        <v>0.2115824618683086</v>
+        <v>0.312061132326838</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.1628423836175867</v>
+        <v>0.3042903097250923</v>
       </c>
       <c r="J20">
-        <v>0.458010988385219</v>
+        <v>0.2864220227778588</v>
       </c>
       <c r="K20">
-        <v>-0.1916161134706239</v>
+        <v>0.3553345272593507</v>
       </c>
       <c r="L20">
-        <v>0.4771333722542902</v>
+        <v>0.3136373640754537</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.3651483716701108</v>
+      </c>
+      <c r="J21">
+        <v>0.2008251226951454</v>
+      </c>
+      <c r="K21">
+        <v>-0.4264014327112208</v>
+      </c>
+      <c r="L21">
+        <v>0.2191383605228726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.3042903097250923</v>
+      </c>
+      <c r="J22">
+        <v>0.2864220227778588</v>
+      </c>
+      <c r="K22">
+        <v>0.3553345272593507</v>
+      </c>
+      <c r="L22">
+        <v>0.3136373640754537</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.3651483716701108</v>
+      </c>
+      <c r="J23">
+        <v>0.2008251226951454</v>
+      </c>
+      <c r="K23">
+        <v>0.4264014327112208</v>
+      </c>
+      <c r="L23">
+        <v>0.2191383605228726</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.4260064336151292</v>
+      </c>
+      <c r="J24">
+        <v>0.1355930012663022</v>
+      </c>
+      <c r="K24">
+        <v>-0.497468338163091</v>
+      </c>
+      <c r="L24">
+        <v>0.1434614655950857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>-0.1023234355858201</v>
+      </c>
+      <c r="J25">
+        <v>0.6377328900501884</v>
+      </c>
+      <c r="K25">
+        <v>-0.1215783580010781</v>
+      </c>
+      <c r="L25">
+        <v>0.6537671093538482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>-0.01461763365511715</v>
+      </c>
+      <c r="J26">
+        <v>0.94636892512424</v>
+      </c>
+      <c r="K26">
+        <v>-0.01736833685729687</v>
+      </c>
+      <c r="L26">
+        <v>0.949096032737041</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.2788995520575487</v>
+      </c>
+      <c r="J27">
+        <v>0.2008903265397131</v>
+      </c>
+      <c r="K27">
+        <v>0.3302413141237342</v>
+      </c>
+      <c r="L27">
+        <v>0.2115824618683086</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>-0.1628423836175867</v>
+      </c>
+      <c r="J28">
+        <v>0.458010988385219</v>
+      </c>
+      <c r="K28">
+        <v>-0.1916161134706239</v>
+      </c>
+      <c r="L28">
+        <v>0.4771333722542902</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="E21">
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>3</v>
       </c>
-      <c r="G21">
+      <c r="G29">
         <v>3</v>
       </c>
-      <c r="H21">
+      <c r="H29">
         <v>16</v>
       </c>
-      <c r="I21">
+      <c r="I29">
         <v>-0.2484997721369916</v>
       </c>
-      <c r="J21">
+      <c r="J29">
         <v>0.2528129010164081</v>
       </c>
-      <c r="K21">
+      <c r="K29">
         <v>-0.2952617265740468</v>
       </c>
-      <c r="L21">
+      <c r="L29">
         <v>0.2669012522950682</v>
       </c>
     </row>
@@ -2085,7 +2702,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2151,10 +2768,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -2189,10 +2806,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -2227,10 +2844,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -2265,10 +2882,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -2303,10 +2920,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -2341,10 +2958,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -2379,10 +2996,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -2417,10 +3034,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2455,10 +3072,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -2493,10 +3110,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -2531,10 +3148,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -2565,341 +3182,645 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9</v>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.3137312989174262</v>
+        <v>-0.4787549991450212</v>
       </c>
       <c r="J13">
-        <v>0.02848639994432931</v>
+        <v>0.07217560549492458</v>
       </c>
       <c r="K13">
-        <v>-0.4131284275634866</v>
+        <v>-0.6292853089020909</v>
       </c>
       <c r="L13">
-        <v>0.02326314515800765</v>
+        <v>0.05124855216842294</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>0.14638501094228</v>
+        <v>-0.2267786838055363</v>
       </c>
       <c r="J14">
-        <v>0.3077335885571051</v>
+        <v>0.3943870594034554</v>
       </c>
       <c r="K14">
-        <v>0.2212047859710532</v>
+        <v>-0.2860387767736777</v>
       </c>
       <c r="L14">
-        <v>0.2401033542701417</v>
+        <v>0.4230203924441358</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>9</v>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>0.2124307787987451</v>
+        <v>-0.1019294382875251</v>
       </c>
       <c r="J15">
-        <v>0.1403732278087201</v>
+        <v>0.7040542681897126</v>
       </c>
       <c r="K15">
-        <v>0.2913831605167395</v>
+        <v>-0.0765092055676006</v>
       </c>
       <c r="L15">
-        <v>0.1182228233126965</v>
+        <v>0.8336123677972922</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.3809072222823607</v>
+        <v>-0.579545525280815</v>
       </c>
       <c r="J16">
-        <v>0.007761477051653751</v>
+        <v>0.02951512807757192</v>
       </c>
       <c r="K16">
-        <v>-0.5322611581053379</v>
+        <v>-0.7119187333033755</v>
       </c>
       <c r="L16">
-        <v>0.002464998415486295</v>
+        <v>0.02091481468718881</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <v>0.08475793795260131</v>
+        <v>-0.1259881576697424</v>
       </c>
       <c r="J17">
-        <v>0.6923284900281212</v>
+        <v>0.6360988735986226</v>
       </c>
       <c r="K17">
-        <v>0.1099316484014564</v>
+        <v>-0.1906925178491184</v>
       </c>
       <c r="L17">
-        <v>0.685265005536689</v>
+        <v>0.5977007516614028</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>0.08475793795260131</v>
+        <v>0.579545525280815</v>
       </c>
       <c r="J18">
-        <v>0.6923284900281212</v>
+        <v>0.02951512807757192</v>
       </c>
       <c r="K18">
-        <v>0.1099316484014564</v>
+        <v>0.7437008196115621</v>
       </c>
       <c r="L18">
-        <v>0.685265005536689</v>
+        <v>0.01366958411527145</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>0.3404532748240978</v>
+        <v>0.560611910581388</v>
       </c>
       <c r="J19">
-        <v>0.1131965364706231</v>
+        <v>0.0366903087793031</v>
       </c>
       <c r="K19">
-        <v>0.4029530171380015</v>
+        <v>0.7172738021962557</v>
       </c>
       <c r="L19">
-        <v>0.1217337691688223</v>
+        <v>0.01954204435368506</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.4978586625371179</v>
+        <v>-0.4787549991450212</v>
       </c>
       <c r="J20">
-        <v>0.02133732054563453</v>
+        <v>0.07217560549492458</v>
       </c>
       <c r="K20">
-        <v>-0.5769230769230769</v>
+        <v>-0.6419981434253655</v>
       </c>
       <c r="L20">
-        <v>0.01929785020805572</v>
+        <v>0.04536158917864154</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>37</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.2771739468734333</v>
+      </c>
+      <c r="J21">
+        <v>0.2978975979923409</v>
+      </c>
+      <c r="K21">
+        <v>-0.3750286184365996</v>
+      </c>
+      <c r="L21">
+        <v>0.2855969029688312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>37</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.1259881576697424</v>
+      </c>
+      <c r="J22">
+        <v>0.6360988735986226</v>
+      </c>
+      <c r="K22">
+        <v>0.1461975970176575</v>
+      </c>
+      <c r="L22">
+        <v>0.6869410188538527</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>37</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.1259881576697424</v>
+      </c>
+      <c r="J23">
+        <v>0.6360988735986226</v>
+      </c>
+      <c r="K23">
+        <v>0.2161181868956676</v>
+      </c>
+      <c r="L23">
+        <v>0.5487107060733141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>37</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.2267786838055363</v>
+      </c>
+      <c r="J24">
+        <v>0.3943870594034554</v>
+      </c>
+      <c r="K24">
+        <v>-0.3114644458202268</v>
+      </c>
+      <c r="L24">
+        <v>0.3810089567050594</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>0.08475793795260131</v>
+      </c>
+      <c r="J25">
+        <v>0.6923284900281212</v>
+      </c>
+      <c r="K25">
+        <v>0.1099316484014564</v>
+      </c>
+      <c r="L25">
+        <v>0.685265005536689</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>0.08475793795260131</v>
+      </c>
+      <c r="J26">
+        <v>0.6923284900281212</v>
+      </c>
+      <c r="K26">
+        <v>0.1099316484014564</v>
+      </c>
+      <c r="L26">
+        <v>0.685265005536689</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.3404532748240978</v>
+      </c>
+      <c r="J27">
+        <v>0.1131965364706231</v>
+      </c>
+      <c r="K27">
+        <v>0.4029530171380015</v>
+      </c>
+      <c r="L27">
+        <v>0.1217337691688223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>-0.4978586625371179</v>
+      </c>
+      <c r="J28">
+        <v>0.02133732054563453</v>
+      </c>
+      <c r="K28">
+        <v>-0.5769230769230769</v>
+      </c>
+      <c r="L28">
+        <v>0.01929785020805572</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="E21">
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>2</v>
       </c>
-      <c r="G21">
+      <c r="G29">
         <v>6</v>
       </c>
-      <c r="H21">
+      <c r="H29">
         <v>16</v>
       </c>
-      <c r="I21">
+      <c r="I29">
         <v>-0.01695158759052026</v>
       </c>
-      <c r="J21">
+      <c r="J29">
         <v>0.9369217280976989</v>
       </c>
-      <c r="K21">
+      <c r="K29">
         <v>-0.03834824944236852</v>
       </c>
-      <c r="L21">
+      <c r="L29">
         <v>0.8878693028318899</v>
       </c>
     </row>
@@ -2910,7 +3831,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2976,10 +3897,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -3002,10 +3923,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -3028,10 +3949,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -3054,10 +3975,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -3080,10 +4001,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -3106,10 +4027,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -3132,10 +4053,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -3158,10 +4079,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -3196,10 +4117,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -3234,10 +4155,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -3272,10 +4193,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -3306,281 +4227,585 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9</v>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G13">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.153506269493634</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0.3197630116677985</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>-0.1847566494939108</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>0.328369658424491</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>0.2815332554724217</v>
+        <v>0.6085806194501846</v>
       </c>
       <c r="J14">
-        <v>0.0686155353555807</v>
+        <v>0.03300625766123251</v>
       </c>
       <c r="K14">
-        <v>0.3381406097030425</v>
+        <v>0.7106690545187014</v>
       </c>
       <c r="L14">
-        <v>0.06760452162982369</v>
+        <v>0.02124449212877441</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>9</v>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G15">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>0.3157348151855433</v>
+        <v>0.6770032003863301</v>
       </c>
       <c r="J15">
-        <v>0.04194762772357558</v>
+        <v>0.01865536081150319</v>
       </c>
       <c r="K15">
-        <v>0.3777116257473406</v>
+        <v>0.7841156792042765</v>
       </c>
       <c r="L15">
-        <v>0.03960563400379821</v>
+        <v>0.007255789526699558</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>-0.1217161238900369</v>
+      </c>
+      <c r="J16">
+        <v>0.6698153575994166</v>
+      </c>
+      <c r="K16">
+        <v>-0.1421338109037403</v>
+      </c>
+      <c r="L16">
+        <v>0.6952876854012655</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
         <v>30</v>
-      </c>
-      <c r="F16">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>18</v>
-      </c>
-      <c r="H16">
-        <v>30</v>
-      </c>
-      <c r="I16">
-        <v>-0.1435427203258164</v>
-      </c>
-      <c r="J16">
-        <v>0.3516806827985527</v>
-      </c>
-      <c r="K16">
-        <v>-0.172944431233412</v>
-      </c>
-      <c r="L16">
-        <v>0.360759748541673</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>-0.3042903097250923</v>
+      </c>
+      <c r="J17">
+        <v>0.2864220227778588</v>
+      </c>
+      <c r="K17">
+        <v>-0.3553345272593507</v>
+      </c>
+      <c r="L17">
+        <v>0.3136373640754537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="E17">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>0.06085806194501846</v>
+      </c>
+      <c r="J18">
+        <v>0.8311704095417624</v>
+      </c>
+      <c r="K18">
+        <v>0.07106690545187015</v>
+      </c>
+      <c r="L18">
+        <v>0.8453239136912953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>0.09231861823449956</v>
+      </c>
+      <c r="J19">
+        <v>0.7483812122920345</v>
+      </c>
+      <c r="K19">
+        <v>0.1069248653460377</v>
+      </c>
+      <c r="L19">
+        <v>0.7687577033932652</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>-0.06085806194501846</v>
+      </c>
+      <c r="J20">
+        <v>0.8311704095417624</v>
+      </c>
+      <c r="K20">
+        <v>-0.07106690545187015</v>
+      </c>
+      <c r="L20">
+        <v>0.8453239136912953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.2434322477800739</v>
+      </c>
+      <c r="J21">
+        <v>0.3937686346429927</v>
+      </c>
+      <c r="K21">
+        <v>-0.2842676218074806</v>
+      </c>
+      <c r="L21">
+        <v>0.4260244484285426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.1217161238900369</v>
+      </c>
+      <c r="J22">
+        <v>0.6698153575994166</v>
+      </c>
+      <c r="K22">
+        <v>0.1421338109037403</v>
+      </c>
+      <c r="L22">
+        <v>0.6952876854012655</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.2434322477800739</v>
+      </c>
+      <c r="J23">
+        <v>0.3937686346429927</v>
+      </c>
+      <c r="K23">
+        <v>0.2842676218074806</v>
+      </c>
+      <c r="L23">
+        <v>0.4260244484285426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.2434322477800739</v>
+      </c>
+      <c r="J24">
+        <v>0.3937686346429927</v>
+      </c>
+      <c r="K24">
+        <v>-0.2842676218074806</v>
+      </c>
+      <c r="L24">
+        <v>0.4260244484285426</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
         <v>16</v>
       </c>
-      <c r="F17">
+      <c r="F25">
         <v>0</v>
       </c>
-      <c r="G17">
+      <c r="G25">
         <v>0</v>
       </c>
-      <c r="H17">
+      <c r="H25">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18">
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
         <v>16</v>
       </c>
-      <c r="F18">
+      <c r="F28">
         <v>0</v>
       </c>
-      <c r="G18">
+      <c r="G28">
         <v>0</v>
       </c>
-      <c r="H18">
+      <c r="H28">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="E19">
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
         <v>16</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>0</v>
       </c>
-      <c r="G19">
+      <c r="G29">
         <v>0</v>
       </c>
-      <c r="H19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20">
-        <v>16</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21">
-        <v>16</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
+      <c r="H29">
         <v>16</v>
       </c>
     </row>
@@ -3591,7 +4816,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3657,10 +4882,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>23</v>
@@ -3695,10 +4920,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>23</v>
@@ -3733,10 +4958,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -3771,10 +4996,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -3809,10 +5034,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -3847,10 +5072,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -3885,10 +5110,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -3923,10 +5148,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -3961,10 +5186,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -3999,10 +5224,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -4037,10 +5262,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>50</v>
@@ -4071,341 +5296,645 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9</v>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.1306708482007147</v>
+        <v>0.04969039949999533</v>
       </c>
       <c r="J13">
-        <v>0.3581258439224645</v>
+        <v>0.8509806870320558</v>
       </c>
       <c r="K13">
-        <v>-0.2011840434130176</v>
+        <v>0.01262892050706804</v>
       </c>
       <c r="L13">
-        <v>0.2863985630278126</v>
+        <v>0.9723786419920799</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>0.08553337321327789</v>
+        <v>-0.149071198499986</v>
       </c>
       <c r="J14">
-        <v>0.5483178177462631</v>
+        <v>0.5730251193553904</v>
       </c>
       <c r="K14">
-        <v>0.1166847704091495</v>
+        <v>-0.1894338076060206</v>
       </c>
       <c r="L14">
-        <v>0.5391786637186142</v>
+        <v>0.6001664342511973</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>9</v>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>0.04028068704356932</v>
+        <v>-0.1256297269074015</v>
       </c>
       <c r="J15">
-        <v>0.7782565834710006</v>
+        <v>0.6374017405958849</v>
       </c>
       <c r="K15">
-        <v>0.06082851254261235</v>
+        <v>-0.152008377581442</v>
       </c>
       <c r="L15">
-        <v>0.7494911940114868</v>
+        <v>0.6750590889374006</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.2077674306436665</v>
+        <v>-0.298142396999972</v>
       </c>
       <c r="J16">
-        <v>0.1435729559776537</v>
+        <v>0.2596563563704499</v>
       </c>
       <c r="K16">
-        <v>-0.2975516272906987</v>
+        <v>-0.3788676152120412</v>
       </c>
       <c r="L16">
-        <v>0.1102840897457505</v>
+        <v>0.2802942824523375</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.2608745973749755</v>
+        <v>-0.1987615979999813</v>
       </c>
       <c r="J17">
-        <v>0.189459515366179</v>
+        <v>0.4523703606773608</v>
       </c>
       <c r="K17">
-        <v>-0.3941471994340144</v>
+        <v>-0.3409808536908371</v>
       </c>
       <c r="L17">
-        <v>0.1308813812945024</v>
+        <v>0.3349456951179903</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.3540440964374667</v>
+        <v>0.149071198499986</v>
       </c>
       <c r="J18">
-        <v>0.07494263177455186</v>
+        <v>0.5730251193553904</v>
       </c>
       <c r="K18">
-        <v>-0.4534975499279393</v>
+        <v>0.1641759665918845</v>
       </c>
       <c r="L18">
-        <v>0.07768807638224377</v>
+        <v>0.6503895621649565</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>0.14034022285596</v>
+        <v>0.07537783614444091</v>
       </c>
       <c r="J19">
-        <v>0.481699512487204</v>
+        <v>0.7773295263554205</v>
       </c>
       <c r="K19">
-        <v>0.1568611789958072</v>
+        <v>0.1076726007868547</v>
       </c>
       <c r="L19">
-        <v>0.5618076700772363</v>
+        <v>0.7671778789420547</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>0.03774256780481986</v>
+        <v>-0.09938079899999065</v>
       </c>
       <c r="J20">
-        <v>0.8508111952177798</v>
+        <v>0.7071142312899612</v>
       </c>
       <c r="K20">
-        <v>0.06715718224198458</v>
+        <v>-0.1262892050706804</v>
       </c>
       <c r="L20">
-        <v>0.8048182163992386</v>
+        <v>0.7281063840216824</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>-0.149071198499986</v>
+      </c>
+      <c r="J21">
+        <v>0.5730251193553904</v>
+      </c>
+      <c r="K21">
+        <v>-0.2399494896342928</v>
+      </c>
+      <c r="L21">
+        <v>0.5043017190353258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>26</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0.3975231959999626</v>
+      </c>
+      <c r="J22">
+        <v>0.1328549557310538</v>
+      </c>
+      <c r="K22">
+        <v>0.5304146612968577</v>
+      </c>
+      <c r="L22">
+        <v>0.1147392659290222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>26</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>0.298142396999972</v>
+      </c>
+      <c r="J23">
+        <v>0.2596563563704499</v>
+      </c>
+      <c r="K23">
+        <v>0.4041254562261773</v>
+      </c>
+      <c r="L23">
+        <v>0.2467547295422347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>26</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>-0.2484519974999766</v>
+      </c>
+      <c r="J24">
+        <v>0.347558036741169</v>
+      </c>
+      <c r="K24">
+        <v>-0.4293832972403134</v>
+      </c>
+      <c r="L24">
+        <v>0.2155824117700313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>30</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>-0.2608745973749755</v>
+      </c>
+      <c r="J25">
+        <v>0.189459515366179</v>
+      </c>
+      <c r="K25">
+        <v>-0.3941471994340144</v>
+      </c>
+      <c r="L25">
+        <v>0.1308813812945024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>14</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>-0.3540440964374667</v>
+      </c>
+      <c r="J26">
+        <v>0.07494263177455186</v>
+      </c>
+      <c r="K26">
+        <v>-0.4534975499279393</v>
+      </c>
+      <c r="L26">
+        <v>0.07768807638224377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>14</v>
+      </c>
+      <c r="G27">
+        <v>30</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.14034022285596</v>
+      </c>
+      <c r="J27">
+        <v>0.481699512487204</v>
+      </c>
+      <c r="K27">
+        <v>0.1568611789958072</v>
+      </c>
+      <c r="L27">
+        <v>0.5618076700772363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>0.03774256780481986</v>
+      </c>
+      <c r="J28">
+        <v>0.8508111952177798</v>
+      </c>
+      <c r="K28">
+        <v>0.06715718224198458</v>
+      </c>
+      <c r="L28">
+        <v>0.8048182163992386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="E21">
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>14</v>
       </c>
-      <c r="G21">
+      <c r="G29">
         <v>30</v>
       </c>
-      <c r="H21">
+      <c r="H29">
         <v>16</v>
       </c>
-      <c r="I21">
+      <c r="I29">
         <v>0.07453559924999299</v>
       </c>
-      <c r="J21">
+      <c r="J29">
         <v>0.7077285315990198</v>
       </c>
-      <c r="K21">
+      <c r="K29">
         <v>0.07913380065856659</v>
       </c>
-      <c r="L21">
+      <c r="L29">
         <v>0.770810224273788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corr results with infer no filter
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -874,7 +874,7 @@
         <v>48</v>
       </c>
       <c r="G10">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="H10">
         <v>50</v>
@@ -912,7 +912,7 @@
         <v>48</v>
       </c>
       <c r="G11">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="H11">
         <v>50</v>
@@ -950,7 +950,7 @@
         <v>48</v>
       </c>
       <c r="G12">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -1444,22 +1444,22 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1626978433639921</v>
+        <v>-0.1807753815155468</v>
       </c>
       <c r="J25">
-        <v>0.4043745903773081</v>
+        <v>0.3541954904764164</v>
       </c>
       <c r="K25">
-        <v>-0.2500726110965064</v>
+        <v>-0.2576049186596542</v>
       </c>
       <c r="L25">
-        <v>0.3502469232913418</v>
+        <v>0.3354345184285685</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1482,22 +1482,22 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1988529196671015</v>
+        <v>-0.1807753815155468</v>
       </c>
       <c r="J26">
-        <v>0.3081411014502622</v>
+        <v>0.3541954904764164</v>
       </c>
       <c r="K26">
-        <v>-0.2741759952985793</v>
+        <v>-0.2666436877354316</v>
       </c>
       <c r="L26">
-        <v>0.3041353554760347</v>
+        <v>0.3181414648703181</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1520,22 +1520,22 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3721433734379864</v>
+        <v>0.3539900381483285</v>
       </c>
       <c r="J27">
-        <v>0.05729901570416417</v>
+        <v>0.07056136851892029</v>
       </c>
       <c r="K27">
-        <v>0.443979491086295</v>
+        <v>0.4341802833034056</v>
       </c>
       <c r="L27">
-        <v>0.08493122100226924</v>
+        <v>0.09288178063084394</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H28">
         <v>16</v>
@@ -1570,10 +1570,10 @@
         <v>0.4027546538976249</v>
       </c>
       <c r="K28">
-        <v>-0.2341913484699036</v>
+        <v>-0.2493004677260264</v>
       </c>
       <c r="L28">
-        <v>0.3826574736700414</v>
+        <v>0.3517858440384553</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1596,7 +1596,7 @@
         <v>15</v>
       </c>
       <c r="G29">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H29">
         <v>16</v>
@@ -1608,10 +1608,10 @@
         <v>0.5166373798159882</v>
       </c>
       <c r="K29">
-        <v>-0.159684920338733</v>
+        <v>-0.1491396897503261</v>
       </c>
       <c r="L29">
-        <v>0.554695992273345</v>
+        <v>0.5814513259975999</v>
       </c>
     </row>
   </sheetData>
@@ -3847,7 +3847,7 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4126,25 +4126,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01796621933296706</v>
+        <v>-0.004001088444105332</v>
       </c>
       <c r="J10">
-        <v>0.8831428170689836</v>
+        <v>0.9739374982488735</v>
       </c>
       <c r="K10">
-        <v>-0.01941575076033076</v>
+        <v>-0.004014544573191041</v>
       </c>
       <c r="L10">
-        <v>0.8935368700981905</v>
+        <v>0.9779259755977681</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4164,25 +4164,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02073391231297599</v>
+        <v>-0.01888959038201153</v>
       </c>
       <c r="J11">
-        <v>0.8590316155348903</v>
+        <v>0.8717029852220165</v>
       </c>
       <c r="K11">
-        <v>-0.02339586347864377</v>
+        <v>-0.02206154843492711</v>
       </c>
       <c r="L11">
-        <v>0.8718796181740638</v>
+        <v>0.8791305588586364</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4202,25 +4202,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.248946277190559</v>
+        <v>-0.2476064162497625</v>
       </c>
       <c r="J12">
-        <v>0.03184335671615308</v>
+        <v>0.0331142128596994</v>
       </c>
       <c r="K12">
-        <v>-0.3107802994453792</v>
+        <v>-0.3099127537051835</v>
       </c>
       <c r="L12">
-        <v>0.02804344582260457</v>
+        <v>0.02850794708171081</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4696,13 +4696,25 @@
         <v>16</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>16</v>
+      </c>
+      <c r="I25">
+        <v>-0.3535533905932737</v>
+      </c>
+      <c r="J25">
+        <v>0.1037416782365415</v>
+      </c>
+      <c r="K25">
+        <v>-0.4200840252084029</v>
+      </c>
+      <c r="L25">
+        <v>0.105228057983522</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -4722,13 +4734,25 @@
         <v>16</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>16</v>
+      </c>
+      <c r="I26">
+        <v>-0.1649915822768611</v>
+      </c>
+      <c r="J26">
+        <v>0.4476990724652935</v>
+      </c>
+      <c r="K26">
+        <v>-0.1960392117639214</v>
+      </c>
+      <c r="L26">
+        <v>0.4668248490265503</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -4748,13 +4772,25 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.02366905341655754</v>
+      </c>
+      <c r="J27">
+        <v>0.9135633303377861</v>
+      </c>
+      <c r="K27">
+        <v>0.02802621677476181</v>
+      </c>
+      <c r="L27">
+        <v>0.9179387985999929</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -4774,13 +4810,25 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>16</v>
+      </c>
+      <c r="I28">
+        <v>-0.2625754538144587</v>
+      </c>
+      <c r="J28">
+        <v>0.2314460271038938</v>
+      </c>
+      <c r="K28">
+        <v>-0.3089716991054783</v>
+      </c>
+      <c r="L28">
+        <v>0.2442606266224961</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -4800,13 +4848,25 @@
         <v>16</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>16</v>
+      </c>
+      <c r="I29">
+        <v>0.2592724864350675</v>
+      </c>
+      <c r="J29">
+        <v>0.2328233516916538</v>
+      </c>
+      <c r="K29">
+        <v>0.3080616184861621</v>
+      </c>
+      <c r="L29">
+        <v>0.2457251662216493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made the main one be max
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -833,25 +833,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G9">
-        <v>441</v>
+        <v>1200</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.1982706498886916</v>
+        <v>-0.1679930849817192</v>
       </c>
       <c r="J9">
-        <v>0.00536937267196464</v>
+        <v>0.01571209940531982</v>
       </c>
       <c r="K9">
-        <v>-0.2886630924945615</v>
+        <v>-0.2581562594294852</v>
       </c>
       <c r="L9">
-        <v>0.003584220045792815</v>
+        <v>0.009508181415596517</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -874,22 +874,22 @@
         <v>48</v>
       </c>
       <c r="G10">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01391413642584883</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J10">
-        <v>0.9090032366864784</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K10">
-        <v>-0.01026612600739247</v>
+        <v>-0.01605248793883186</v>
       </c>
       <c r="L10">
-        <v>0.9435901857829745</v>
+        <v>0.9118983828429555</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -912,22 +912,22 @@
         <v>48</v>
       </c>
       <c r="G11">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-0.0319066731228802</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.7837672300250216</v>
       </c>
       <c r="K11">
-        <v>-0.0299893827986723</v>
+        <v>-0.03045075791865187</v>
       </c>
       <c r="L11">
-        <v>0.8362130272367809</v>
+        <v>0.8337285990222609</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -950,22 +950,22 @@
         <v>48</v>
       </c>
       <c r="G12">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.2441570787714312</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>0.03455416553919029</v>
       </c>
       <c r="K12">
-        <v>-0.3096184720415943</v>
+        <v>-0.3094340106343606</v>
       </c>
       <c r="L12">
-        <v>0.02866696147428332</v>
+        <v>0.02876701130235894</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5217,25 +5217,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="G9">
-        <v>49</v>
+        <v>808</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.02338955473951822</v>
+        <v>-0.1508932577851104</v>
       </c>
       <c r="J9">
-        <v>0.7695518235571096</v>
+        <v>0.03976539977998658</v>
       </c>
       <c r="K9">
-        <v>-0.02899175010168209</v>
+        <v>-0.2101007063448729</v>
       </c>
       <c r="L9">
-        <v>0.7746233072761167</v>
+        <v>0.03589890255176344</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5255,10 +5255,10 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>165</v>
+        <v>219</v>
       </c>
       <c r="H10">
         <v>50</v>
@@ -5293,10 +5293,10 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G11">
-        <v>165</v>
+        <v>219</v>
       </c>
       <c r="H11">
         <v>50</v>
@@ -5331,10 +5331,10 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>165</v>
+        <v>219</v>
       </c>
       <c r="H12">
         <v>50</v>

</xml_diff>

<commit_message>
updated stuff from replication-package branch
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -507,7 +507,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
@@ -833,25 +833,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G9">
-        <v>434</v>
+        <v>1200</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.1903363180248888</v>
+        <v>-0.1679930849817192</v>
       </c>
       <c r="J9">
-        <v>0.007575221566781355</v>
+        <v>0.01571209940531982</v>
       </c>
       <c r="K9">
-        <v>-0.2775832265508705</v>
+        <v>-0.2581562594294852</v>
       </c>
       <c r="L9">
-        <v>0.005172267323392988</v>
+        <v>0.009508181415596517</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -874,22 +874,22 @@
         <v>48</v>
       </c>
       <c r="G10">
-        <v>794</v>
+        <v>863</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01391413642584883</v>
+        <v>-0.01788960397609135</v>
       </c>
       <c r="J10">
-        <v>0.9090032366864784</v>
+        <v>0.8831700141519032</v>
       </c>
       <c r="K10">
-        <v>-0.01026612600739247</v>
+        <v>-0.01605248793883186</v>
       </c>
       <c r="L10">
-        <v>0.9435901857829745</v>
+        <v>0.9118983828429555</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -912,22 +912,22 @@
         <v>48</v>
       </c>
       <c r="G11">
-        <v>794</v>
+        <v>863</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-0.0319066731228802</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.7837672300250216</v>
       </c>
       <c r="K11">
-        <v>-0.0299893827986723</v>
+        <v>-0.03045075791865187</v>
       </c>
       <c r="L11">
-        <v>0.8362130272367809</v>
+        <v>0.8337285990222609</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -950,22 +950,22 @@
         <v>48</v>
       </c>
       <c r="G12">
-        <v>794</v>
+        <v>863</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.2441570787714312</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>0.03455416553919029</v>
       </c>
       <c r="K12">
-        <v>-0.3096184720415943</v>
+        <v>-0.3094340106343606</v>
       </c>
       <c r="L12">
-        <v>0.02866696147428332</v>
+        <v>0.02876701130235894</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5217,25 +5217,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="G9">
-        <v>42</v>
+        <v>808</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>0.02530070087153832</v>
+        <v>-0.1508932577851104</v>
       </c>
       <c r="J9">
-        <v>0.7524683996638825</v>
+        <v>0.03976539977998658</v>
       </c>
       <c r="K9">
-        <v>0.02951927871749955</v>
+        <v>-0.2101007063448729</v>
       </c>
       <c r="L9">
-        <v>0.770634516417006</v>
+        <v>0.03589890255176344</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5255,10 +5255,10 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="H10">
         <v>50</v>
@@ -5293,10 +5293,10 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="H11">
         <v>50</v>
@@ -5331,10 +5331,10 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="H12">
         <v>50</v>

</xml_diff>

<commit_message>
Removed meta data from excel files + new results
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0727E5DF-8310-4208-B60B-5DA5D706E670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -13,7 +14,7 @@
     <sheet name="infer" sheetId="4" r:id="rId4"/>
     <sheet name="openjml" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -140,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +205,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -250,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,9 +291,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,6 +343,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,12 +536,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -508,11 +553,10 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="11" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -576,19 +620,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.3377277477430254</v>
+        <v>-0.33772774774302539</v>
       </c>
       <c r="J2">
-        <v>0.03761941401427579</v>
+        <v>3.7619414014275793E-2</v>
       </c>
       <c r="K2">
-        <v>-0.3976802252851466</v>
+        <v>-0.39768022528514663</v>
       </c>
       <c r="L2">
-        <v>0.06021635626528627</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>6.0216356265286271E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -614,19 +658,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.4275482906928738</v>
+        <v>-0.42754829069287381</v>
       </c>
       <c r="J3">
-        <v>0.007641040482277836</v>
+        <v>7.6410404822778357E-3</v>
       </c>
       <c r="K3">
-        <v>-0.5452867412432369</v>
+        <v>-0.54528674124323695</v>
       </c>
       <c r="L3">
-        <v>0.007124393687845218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>7.124393687845218E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -652,19 +696,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.4111706600105638</v>
+        <v>0.41117066001056379</v>
       </c>
       <c r="J4">
-        <v>0.00982101261512518</v>
+        <v>9.8210126151251805E-3</v>
       </c>
       <c r="K4">
-        <v>0.5360003171861121</v>
+        <v>0.53600031718611207</v>
       </c>
       <c r="L4">
-        <v>0.008382091244079634</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>8.3820912440796345E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -690,19 +734,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.3133397807202561</v>
+        <v>-0.31333978072025609</v>
       </c>
       <c r="J5">
-        <v>0.1884699909010059</v>
+        <v>0.18846999090100591</v>
       </c>
       <c r="K5">
-        <v>-0.3178304128441319</v>
+        <v>-0.31783041284413188</v>
       </c>
       <c r="L5">
-        <v>0.3140610795011266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.31406107950112661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -728,19 +772,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.4526019054848143</v>
+        <v>-0.45260190548481433</v>
       </c>
       <c r="J6">
-        <v>0.05748353173133636</v>
+        <v>5.7483531731336357E-2</v>
       </c>
       <c r="K6">
-        <v>-0.4693542143163343</v>
+        <v>-0.46935421431633428</v>
       </c>
       <c r="L6">
-        <v>0.1237049815910057</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>0.12370498159100569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -766,19 +810,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.3829708431025352</v>
+        <v>-0.38297084310253521</v>
       </c>
       <c r="J7">
         <v>0.1079738014574666</v>
       </c>
       <c r="K7">
-        <v>-0.458267106891539</v>
+        <v>-0.45826710689153899</v>
       </c>
       <c r="L7">
-        <v>0.1340598783554668</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>0.13405987835546679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -804,19 +848,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.1392621247645583</v>
+        <v>0.13926212476455829</v>
       </c>
       <c r="J8">
         <v>0.5588858290416201</v>
       </c>
       <c r="K8">
-        <v>0.2032636361212471</v>
+        <v>0.20326363612124709</v>
       </c>
       <c r="L8">
-        <v>0.5263323724525723</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.52633237245257225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -842,19 +886,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.1679930849817192</v>
+        <v>-0.16799308498171919</v>
       </c>
       <c r="J9">
-        <v>0.01571209940531982</v>
+        <v>1.571209940531982E-2</v>
       </c>
       <c r="K9">
-        <v>-0.2581562594294852</v>
+        <v>-0.25815625942948522</v>
       </c>
       <c r="L9">
-        <v>0.009508181415596517</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>9.5081814155965165E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -880,19 +924,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-1.7889603976091351E-2</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.88317001415190322</v>
       </c>
       <c r="K10">
-        <v>-0.01605248793883186</v>
+        <v>-1.605248793883186E-2</v>
       </c>
       <c r="L10">
-        <v>0.9118983828429555</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.91189838284295555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -918,19 +962,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.0319066731228802</v>
+        <v>-3.1906673122880203E-2</v>
       </c>
       <c r="J11">
-        <v>0.7837672300250216</v>
+        <v>0.78376723002502158</v>
       </c>
       <c r="K11">
-        <v>-0.03045075791865187</v>
+        <v>-3.0450757918651868E-2</v>
       </c>
       <c r="L11">
-        <v>0.8337285990222609</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.83372859902226093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -959,16 +1003,16 @@
         <v>-0.2441570787714312</v>
       </c>
       <c r="J12">
-        <v>0.03455416553919029</v>
+        <v>3.4554165539190287E-2</v>
       </c>
       <c r="K12">
         <v>-0.3094340106343606</v>
       </c>
       <c r="L12">
-        <v>0.02876701130235894</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.8767011302358939E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -994,19 +1038,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4535394202249742</v>
+        <v>-0.45353942022497418</v>
       </c>
       <c r="J13">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K13">
-        <v>-0.5512130501182249</v>
+        <v>-0.55121305011822486</v>
       </c>
       <c r="L13">
-        <v>0.09862398123473154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>9.8623981234731539E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1032,19 +1076,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.02387049580131443</v>
+        <v>-2.387049580131443E-2</v>
       </c>
       <c r="J14">
-        <v>0.92675547372309</v>
+        <v>0.92675547372308997</v>
       </c>
       <c r="K14">
-        <v>-0.09290107586262218</v>
+        <v>-9.2901075862622182E-2</v>
       </c>
       <c r="L14">
-        <v>0.7985237548304135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.79852375483041349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1070,19 +1114,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.09656090991705352</v>
+        <v>9.6560909917053517E-2</v>
       </c>
       <c r="J15">
-        <v>0.7120793980044939</v>
+        <v>0.71207939800449394</v>
       </c>
       <c r="K15">
-        <v>0.1428819499477476</v>
+        <v>0.14288194994774761</v>
       </c>
       <c r="L15">
-        <v>0.6937488280957302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.69374882809573024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1108,19 +1152,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.7399853698407473</v>
+        <v>-0.73998536984074725</v>
       </c>
       <c r="J16">
-        <v>0.004375235749920733</v>
+        <v>4.375235749920733E-3</v>
       </c>
       <c r="K16">
-        <v>-0.8670767080511405</v>
+        <v>-0.86707670805114045</v>
       </c>
       <c r="L16">
-        <v>0.001159768265192443</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>1.1597682651924429E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1146,19 +1190,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.3103164454170876</v>
+        <v>-0.31031644541708758</v>
       </c>
       <c r="J17">
         <v>0.2320634889020341</v>
       </c>
       <c r="K17">
-        <v>-0.4149581388530457</v>
+        <v>-0.41495813885304572</v>
       </c>
       <c r="L17">
         <v>0.233093730241445</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1184,19 +1228,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.4535394202249742</v>
+        <v>0.45353942022497418</v>
       </c>
       <c r="J18">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K18">
-        <v>0.5635998602332413</v>
+        <v>0.56359986023324127</v>
       </c>
       <c r="L18">
-        <v>0.08974939558201678</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>8.9749395582016778E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1222,19 +1266,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.4828045495852675</v>
+        <v>0.48280454958526747</v>
       </c>
       <c r="J19">
-        <v>0.06499039472076076</v>
+        <v>6.4990394720760764E-2</v>
       </c>
       <c r="K19">
-        <v>0.5932707052178214</v>
+        <v>0.59327070521782144</v>
       </c>
       <c r="L19">
-        <v>0.0706202179291523</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>7.0620217929152296E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1260,19 +1304,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.3580574370197164</v>
+        <v>-0.35805743701971637</v>
       </c>
       <c r="J20">
-        <v>0.1679207532945924</v>
+        <v>0.16792075329459241</v>
       </c>
       <c r="K20">
-        <v>-0.4954724046006516</v>
+        <v>-0.49547240460065162</v>
       </c>
       <c r="L20">
-        <v>0.1453294522910624</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.14532945229106239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1298,19 +1342,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.4535394202249742</v>
+        <v>-0.45353942022497418</v>
       </c>
       <c r="J21">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K21">
-        <v>-0.6007602905782901</v>
+        <v>-0.60076029057829006</v>
       </c>
       <c r="L21">
-        <v>0.06625295074379814</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>6.6252950743798139E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1339,16 +1383,16 @@
         <v>0.1193524790065721</v>
       </c>
       <c r="J22">
-        <v>0.6457756768370824</v>
+        <v>0.64577567683708237</v>
       </c>
       <c r="K22">
-        <v>0.1486417213801955</v>
+        <v>0.14864172138019549</v>
       </c>
       <c r="L22">
-        <v>0.6819355638686473</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.68193556386864729</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1374,19 +1418,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.167093470609201</v>
+        <v>0.16709347060920099</v>
       </c>
       <c r="J23">
-        <v>0.5199036173455835</v>
+        <v>0.51990361734558355</v>
       </c>
       <c r="K23">
-        <v>0.2725098225303584</v>
+        <v>0.27250982253035838</v>
       </c>
       <c r="L23">
-        <v>0.446215643690079</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.44621564369007899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1412,19 +1456,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.3580574370197164</v>
+        <v>-0.35805743701971637</v>
       </c>
       <c r="J24">
-        <v>0.1679207532945924</v>
+        <v>0.16792075329459241</v>
       </c>
       <c r="K24">
-        <v>-0.4706987843706191</v>
+        <v>-0.47069878437061913</v>
       </c>
       <c r="L24">
         <v>0.1697475039817557</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1450,19 +1494,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1807753815155468</v>
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J25">
-        <v>0.3541954904764164</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K25">
-        <v>-0.2576049186596542</v>
+        <v>-0.25760491865965418</v>
       </c>
       <c r="L25">
-        <v>0.3354345184285685</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.33543451842856847</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1488,19 +1532,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1807753815155468</v>
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J26">
-        <v>0.3541954904764164</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K26">
-        <v>-0.2666436877354316</v>
+        <v>-0.26664368773543162</v>
       </c>
       <c r="L26">
-        <v>0.3181414648703181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.31814146487031808</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1526,19 +1570,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3539900381483285</v>
+        <v>0.35399003814832852</v>
       </c>
       <c r="J27">
-        <v>0.07056136851892029</v>
+        <v>7.0561368518920295E-2</v>
       </c>
       <c r="K27">
-        <v>0.4341802833034056</v>
+        <v>0.43418028330340558</v>
       </c>
       <c r="L27">
-        <v>0.09288178063084394</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>9.2881780630843944E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1567,16 +1611,16 @@
         <v>-0.1647705109143269</v>
       </c>
       <c r="J28">
-        <v>0.4027546538976249</v>
+        <v>0.40275465389762488</v>
       </c>
       <c r="K28">
         <v>-0.2493004677260264</v>
       </c>
       <c r="L28">
-        <v>0.3517858440384553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.35178584403845531</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1605,27 +1649,28 @@
         <v>-0.1265427670608828</v>
       </c>
       <c r="J29">
-        <v>0.5166373798159882</v>
+        <v>0.51663737981598823</v>
       </c>
       <c r="K29">
         <v>-0.1491396897503261</v>
       </c>
       <c r="L29">
-        <v>0.5814513259975999</v>
+        <v>0.58145132599759985</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1636,12 +1681,11 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="10" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1708,16 +1752,16 @@
         <v>-0.2277100170213244</v>
       </c>
       <c r="J2">
-        <v>0.2003280221869526</v>
+        <v>0.20032802218695259</v>
       </c>
       <c r="K2">
-        <v>-0.2719723502938716</v>
+        <v>-0.27197235029387162</v>
       </c>
       <c r="L2">
-        <v>0.2093250956596323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>0.20932509565963231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1743,19 +1787,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.263477777620917</v>
+        <v>-0.26347777762091701</v>
       </c>
       <c r="J3">
         <v>0.1329850671160174</v>
       </c>
       <c r="K3">
-        <v>-0.3201778730528596</v>
+        <v>-0.32017787305285961</v>
       </c>
       <c r="L3">
-        <v>0.1363764100850406</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>0.13637641008504059</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1784,16 +1828,16 @@
         <v>0.2297034206521828</v>
       </c>
       <c r="J4">
-        <v>0.187290841633909</v>
+        <v>0.18729084163390899</v>
       </c>
       <c r="K4">
-        <v>0.2809695424230301</v>
+        <v>0.28096954242303013</v>
       </c>
       <c r="L4">
-        <v>0.1940516726155841</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>0.19405167261558409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1819,7 +1863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1871,7 +1915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1897,7 +1941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1923,19 +1967,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2289041597670328</v>
+        <v>-0.22890415976703279</v>
       </c>
       <c r="J9">
-        <v>0.004154062204876697</v>
+        <v>4.1540622048766972E-3</v>
       </c>
       <c r="K9">
-        <v>-0.2872671746617843</v>
+        <v>-0.28726717466178431</v>
       </c>
       <c r="L9">
-        <v>0.003756720549751365</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3.7567205497513649E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1961,19 +2005,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-1.7889603976091351E-2</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.88317001415190322</v>
       </c>
       <c r="K10">
-        <v>-0.02174552145202223</v>
+        <v>-2.1745521452022229E-2</v>
       </c>
       <c r="L10">
-        <v>0.8808493755591094</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.88084937555910936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1999,19 +2043,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-2.439922062337898E-2</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.83378844789272755</v>
       </c>
       <c r="K11">
-        <v>-0.02805160729475809</v>
+        <v>-2.8051607294758089E-2</v>
       </c>
       <c r="L11">
-        <v>0.8466646412386398</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.84666464123863983</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2037,19 +2081,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.25161225674918491</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>2.940004335865699E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3118320089283974</v>
+        <v>-0.31183200892839741</v>
       </c>
       <c r="L12">
-        <v>0.02748882596687927</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.7488825966879269E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2075,19 +2119,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.3651483716701108</v>
+        <v>0.36514837167011083</v>
       </c>
       <c r="J13">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K13">
-        <v>0.4264014327112208</v>
+        <v>0.42640143271122077</v>
       </c>
       <c r="L13">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2113,19 +2157,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>0.7302967433402215</v>
+        <v>0.73029674334022154</v>
       </c>
       <c r="J14">
-        <v>0.01051524593585891</v>
+        <v>1.0515245935858911E-2</v>
       </c>
       <c r="K14">
-        <v>0.8528028654224417</v>
+        <v>0.85280286542244166</v>
       </c>
       <c r="L14">
-        <v>0.001712874149321468</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>1.712874149321468E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2151,19 +2195,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.7385489458759965</v>
+        <v>0.73854894587599651</v>
       </c>
       <c r="J15">
-        <v>0.01028204822194895</v>
+        <v>1.0282048221948951E-2</v>
       </c>
       <c r="K15">
-        <v>0.8553989227683017</v>
+        <v>0.85539892276830165</v>
       </c>
       <c r="L15">
-        <v>0.001600453316805279</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>1.600453316805279E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2192,16 +2236,16 @@
         <v>-0.1217161238900369</v>
       </c>
       <c r="J16">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K16">
         <v>-0.1421338109037403</v>
       </c>
       <c r="L16">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2227,19 +2271,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.5477225575051662</v>
+        <v>-0.54772255750516619</v>
       </c>
       <c r="J17">
-        <v>0.05500883362926572</v>
+        <v>5.5008833629265723E-2</v>
       </c>
       <c r="K17">
-        <v>-0.6396021490668313</v>
+        <v>-0.63960214906683133</v>
       </c>
       <c r="L17">
-        <v>0.04643461767158175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>4.6434617671581753E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2265,19 +2309,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.3651483716701108</v>
+        <v>-0.36514837167011083</v>
       </c>
       <c r="J18">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K18">
-        <v>-0.4264014327112208</v>
+        <v>-0.42640143271122077</v>
       </c>
       <c r="L18">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2303,19 +2347,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>-0.3077287274483319</v>
+        <v>-0.30772872744833191</v>
       </c>
       <c r="J19">
-        <v>0.2849576406684299</v>
+        <v>0.28495764066842988</v>
       </c>
       <c r="K19">
-        <v>-0.3564162178201257</v>
+        <v>-0.35641621782012572</v>
       </c>
       <c r="L19">
-        <v>0.312061132326838</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.31206113232683802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2344,16 +2388,16 @@
         <v>0.3042903097250923</v>
       </c>
       <c r="J20">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K20">
-        <v>0.3553345272593507</v>
+        <v>0.35533452725935072</v>
       </c>
       <c r="L20">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2379,19 +2423,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.3651483716701108</v>
+        <v>-0.36514837167011083</v>
       </c>
       <c r="J21">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K21">
-        <v>-0.4264014327112208</v>
+        <v>-0.42640143271122077</v>
       </c>
       <c r="L21">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2420,16 +2464,16 @@
         <v>0.3042903097250923</v>
       </c>
       <c r="J22">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K22">
-        <v>0.3553345272593507</v>
+        <v>0.35533452725935072</v>
       </c>
       <c r="L22">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2455,19 +2499,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.3651483716701108</v>
+        <v>0.36514837167011083</v>
       </c>
       <c r="J23">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K23">
-        <v>0.4264014327112208</v>
+        <v>0.42640143271122077</v>
       </c>
       <c r="L23">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2493,19 +2537,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.4260064336151292</v>
+        <v>-0.42600643361512919</v>
       </c>
       <c r="J24">
-        <v>0.1355930012663022</v>
+        <v>0.13559300126630219</v>
       </c>
       <c r="K24">
         <v>-0.497468338163091</v>
       </c>
       <c r="L24">
-        <v>0.1434614655950857</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.14346146559508571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2531,19 +2575,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1023234355858201</v>
+        <v>-0.10232343558582011</v>
       </c>
       <c r="J25">
-        <v>0.6377328900501884</v>
+        <v>0.63773289005018841</v>
       </c>
       <c r="K25">
-        <v>-0.1215783580010781</v>
+        <v>-0.12157835800107809</v>
       </c>
       <c r="L25">
-        <v>0.6537671093538482</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.65376710935384819</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2569,19 +2613,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.01461763365511715</v>
+        <v>-1.4617633655117149E-2</v>
       </c>
       <c r="J26">
-        <v>0.94636892512424</v>
+        <v>0.94636892512423998</v>
       </c>
       <c r="K26">
-        <v>-0.01736833685729687</v>
+        <v>-1.736833685729687E-2</v>
       </c>
       <c r="L26">
-        <v>0.949096032737041</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.94909603273704102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2607,19 +2651,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.2788995520575487</v>
+        <v>0.27889955205754868</v>
       </c>
       <c r="J27">
-        <v>0.2008903265397131</v>
+        <v>0.20089032653971309</v>
       </c>
       <c r="K27">
         <v>0.3302413141237342</v>
       </c>
       <c r="L27">
-        <v>0.2115824618683086</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.21158246186830859</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2645,19 +2689,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.1628423836175867</v>
+        <v>-0.16284238361758671</v>
       </c>
       <c r="J28">
-        <v>0.458010988385219</v>
+        <v>0.45801098838521898</v>
       </c>
       <c r="K28">
-        <v>-0.1916161134706239</v>
+        <v>-0.19161611347062391</v>
       </c>
       <c r="L28">
         <v>0.4771333722542902</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2683,30 +2727,31 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.2484997721369916</v>
+        <v>-0.24849977213699159</v>
       </c>
       <c r="J29">
-        <v>0.2528129010164081</v>
+        <v>0.25281290101640808</v>
       </c>
       <c r="K29">
-        <v>-0.2952617265740468</v>
+        <v>-0.29526172657404681</v>
       </c>
       <c r="L29">
-        <v>0.2669012522950682</v>
+        <v>0.26690125229506823</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -2722,7 +2767,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2760,7 +2805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2786,19 +2831,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.1707825127659933</v>
+        <v>-0.17078251276599329</v>
       </c>
       <c r="J2">
         <v>0.3368221511559395</v>
       </c>
       <c r="K2">
-        <v>-0.2206327958702234</v>
+        <v>-0.22063279587022341</v>
       </c>
       <c r="L2">
-        <v>0.3117066831945562</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>0.31170668319455619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2824,19 +2869,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.2155727271443866</v>
+        <v>-0.21557272714438661</v>
       </c>
       <c r="J3">
         <v>0.2189727791934982</v>
       </c>
       <c r="K3">
-        <v>-0.2830068271047704</v>
+        <v>-0.28300682710477038</v>
       </c>
       <c r="L3">
-        <v>0.1907013837125806</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>0.19070138371258061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2865,16 +2910,16 @@
         <v>0.182178575000007</v>
       </c>
       <c r="J4">
-        <v>0.2956465760209075</v>
+        <v>0.29564657602090749</v>
       </c>
       <c r="K4">
-        <v>0.2404694281998906</v>
+        <v>0.24046942819989059</v>
       </c>
       <c r="L4">
-        <v>0.2690489763203219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>0.26904897632032188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2900,19 +2945,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.1113404428537808</v>
+        <v>-0.11134044285378079</v>
       </c>
       <c r="J5">
-        <v>0.6639079018776488</v>
+        <v>0.66390790187764881</v>
       </c>
       <c r="K5">
-        <v>-0.131013944022344</v>
+        <v>-0.13101394402234401</v>
       </c>
       <c r="L5">
-        <v>0.6848487144273757</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.68484871442737572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2938,19 +2983,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.2597943666588219</v>
+        <v>-0.25979436665882188</v>
       </c>
       <c r="J6">
-        <v>0.3106354563374008</v>
+        <v>0.31063545633740081</v>
       </c>
       <c r="K6">
-        <v>-0.3056992027188027</v>
+        <v>-0.30569920271880269</v>
       </c>
       <c r="L6">
-        <v>0.3338931364506602</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>0.33389313645066021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2976,19 +3021,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.1113404428537808</v>
+        <v>0.11134044285378079</v>
       </c>
       <c r="J7">
-        <v>0.6639079018776488</v>
+        <v>0.66390790187764881</v>
       </c>
       <c r="K7">
-        <v>0.131013944022344</v>
+        <v>0.13101394402234401</v>
       </c>
       <c r="L7">
-        <v>0.6848487144273757</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>0.68484871442737572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3014,19 +3059,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.2597943666588219</v>
+        <v>-0.25979436665882188</v>
       </c>
       <c r="J8">
-        <v>0.3106354563374008</v>
+        <v>0.31063545633740081</v>
       </c>
       <c r="K8">
-        <v>-0.3056992027188027</v>
+        <v>-0.30569920271880269</v>
       </c>
       <c r="L8">
-        <v>0.3338931364506602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.33389313645066021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3052,19 +3097,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459341</v>
+        <v>-0.15625137459340999</v>
       </c>
       <c r="J9">
-        <v>0.0301286154880051</v>
+        <v>3.0128615488005099E-2</v>
       </c>
       <c r="K9">
         <v>-0.2203331090972887</v>
       </c>
       <c r="L9">
-        <v>0.0276105659239954</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>2.7610565923995401E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3090,19 +3135,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01391413642584883</v>
+        <v>-1.3914136425848831E-2</v>
       </c>
       <c r="J10">
-        <v>0.9090032366864784</v>
+        <v>0.90900323668647842</v>
       </c>
       <c r="K10">
-        <v>-0.01026612600739247</v>
+        <v>-1.0266126007392471E-2</v>
       </c>
       <c r="L10">
-        <v>0.9435901857829745</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.94359018578297449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3128,19 +3173,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-2.8152946873129591E-2</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.80868009561069343</v>
       </c>
       <c r="K11">
-        <v>-0.0299893827986723</v>
+        <v>-2.99893827986723E-2</v>
       </c>
       <c r="L11">
-        <v>0.8362130272367809</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.83621302723678093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3166,19 +3211,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.24788466776030799</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>3.1887928946905821E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3096184720415943</v>
+        <v>-0.30961847204159432</v>
       </c>
       <c r="L12">
-        <v>0.02866696147428332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.8666961474283319E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3204,19 +3249,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4787549991450212</v>
+        <v>-0.47875499914502118</v>
       </c>
       <c r="J13">
-        <v>0.07217560549492458</v>
+        <v>7.2175605494924577E-2</v>
       </c>
       <c r="K13">
-        <v>-0.6292853089020909</v>
+        <v>-0.62928530890209089</v>
       </c>
       <c r="L13">
-        <v>0.05124855216842294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>5.1248552168422938E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3242,19 +3287,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.2267786838055363</v>
+        <v>-0.22677868380553631</v>
       </c>
       <c r="J14">
-        <v>0.3943870594034554</v>
+        <v>0.39438705940345542</v>
       </c>
       <c r="K14">
-        <v>-0.2860387767736777</v>
+        <v>-0.28603877677367773</v>
       </c>
       <c r="L14">
-        <v>0.4230203924441358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.42302039244413581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3283,16 +3328,16 @@
         <v>-0.1019294382875251</v>
       </c>
       <c r="J15">
-        <v>0.7040542681897126</v>
+        <v>0.70405426818971262</v>
       </c>
       <c r="K15">
-        <v>-0.0765092055676006</v>
+        <v>-7.6509205567600602E-2</v>
       </c>
       <c r="L15">
         <v>0.8336123677972922</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3318,19 +3363,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.579545525280815</v>
+        <v>-0.57954552528081504</v>
       </c>
       <c r="J16">
-        <v>0.02951512807757192</v>
+        <v>2.9515128077571919E-2</v>
       </c>
       <c r="K16">
-        <v>-0.7119187333033755</v>
+        <v>-0.71191873330337552</v>
       </c>
       <c r="L16">
-        <v>0.02091481468718881</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>2.091481468718881E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3356,19 +3401,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1259881576697424</v>
+        <v>-0.12598815766974239</v>
       </c>
       <c r="J17">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K17">
-        <v>-0.1906925178491184</v>
+        <v>-0.19069251784911839</v>
       </c>
       <c r="L17">
         <v>0.5977007516614028</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3394,19 +3439,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.579545525280815</v>
+        <v>0.57954552528081504</v>
       </c>
       <c r="J18">
-        <v>0.02951512807757192</v>
+        <v>2.9515128077571919E-2</v>
       </c>
       <c r="K18">
-        <v>0.7437008196115621</v>
+        <v>0.74370081961156209</v>
       </c>
       <c r="L18">
-        <v>0.01366958411527145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>1.3669584115271451E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -3432,19 +3477,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.560611910581388</v>
+        <v>0.56061191058138804</v>
       </c>
       <c r="J19">
-        <v>0.0366903087793031</v>
+        <v>3.6690308779303099E-2</v>
       </c>
       <c r="K19">
-        <v>0.7172738021962557</v>
+        <v>0.71727380219625569</v>
       </c>
       <c r="L19">
-        <v>0.01954204435368506</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>1.9542044353685058E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -3470,19 +3515,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.4787549991450212</v>
+        <v>-0.47875499914502118</v>
       </c>
       <c r="J20">
-        <v>0.07217560549492458</v>
+        <v>7.2175605494924577E-2</v>
       </c>
       <c r="K20">
-        <v>-0.6419981434253655</v>
+        <v>-0.64199814342536554</v>
       </c>
       <c r="L20">
-        <v>0.04536158917864154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>4.536158917864154E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3508,19 +3553,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2771739468734333</v>
+        <v>-0.27717394687343327</v>
       </c>
       <c r="J21">
-        <v>0.2978975979923409</v>
+        <v>0.29789759799234089</v>
       </c>
       <c r="K21">
-        <v>-0.3750286184365996</v>
+        <v>-0.37502861843659963</v>
       </c>
       <c r="L21">
-        <v>0.2855969029688312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.28559690296883122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3546,19 +3591,19 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.1259881576697424</v>
+        <v>0.12598815766974239</v>
       </c>
       <c r="J22">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K22">
         <v>0.1461975970176575</v>
       </c>
       <c r="L22">
-        <v>0.6869410188538527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.68694101885385273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3584,19 +3629,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.1259881576697424</v>
+        <v>0.12598815766974239</v>
       </c>
       <c r="J23">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K23">
-        <v>0.2161181868956676</v>
+        <v>0.21611818689566761</v>
       </c>
       <c r="L23">
-        <v>0.5487107060733141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.54871070607331407</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3622,19 +3667,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2267786838055363</v>
+        <v>-0.22677868380553631</v>
       </c>
       <c r="J24">
-        <v>0.3943870594034554</v>
+        <v>0.39438705940345542</v>
       </c>
       <c r="K24">
-        <v>-0.3114644458202268</v>
+        <v>-0.31146444582022681</v>
       </c>
       <c r="L24">
-        <v>0.3810089567050594</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.38100895670505941</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3660,19 +3705,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>0.08475793795260131</v>
+        <v>8.4757937952601309E-2</v>
       </c>
       <c r="J25">
-        <v>0.6923284900281212</v>
+        <v>0.69232849002812125</v>
       </c>
       <c r="K25">
         <v>0.1099316484014564</v>
       </c>
       <c r="L25">
-        <v>0.685265005536689</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.68526500553668901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -3698,19 +3743,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>0.08475793795260131</v>
+        <v>8.4757937952601309E-2</v>
       </c>
       <c r="J26">
-        <v>0.6923284900281212</v>
+        <v>0.69232849002812125</v>
       </c>
       <c r="K26">
         <v>0.1099316484014564</v>
       </c>
       <c r="L26">
-        <v>0.685265005536689</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.68526500553668901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3736,19 +3781,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3404532748240978</v>
+        <v>0.34045327482409782</v>
       </c>
       <c r="J27">
         <v>0.1131965364706231</v>
       </c>
       <c r="K27">
-        <v>0.4029530171380015</v>
+        <v>0.40295301713800152</v>
       </c>
       <c r="L27">
         <v>0.1217337691688223</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3774,19 +3819,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.4978586625371179</v>
+        <v>-0.49785866253711791</v>
       </c>
       <c r="J28">
-        <v>0.02133732054563453</v>
+        <v>2.1337320545634531E-2</v>
       </c>
       <c r="K28">
-        <v>-0.5769230769230769</v>
+        <v>-0.57692307692307687</v>
       </c>
       <c r="L28">
-        <v>0.01929785020805572</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>1.929785020805572E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -3812,30 +3857,31 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.01695158759052026</v>
+        <v>-1.6951587590520258E-2</v>
       </c>
       <c r="J29">
-        <v>0.9369217280976989</v>
+        <v>0.93692172809769891</v>
       </c>
       <c r="K29">
-        <v>-0.03834824944236852</v>
+        <v>-3.8348249442368518E-2</v>
       </c>
       <c r="L29">
-        <v>0.8878693028318899</v>
+        <v>0.88786930283188992</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -3851,7 +3897,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3889,7 +3935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3915,7 +3961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3941,7 +3987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3967,7 +4013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3993,7 +4039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4019,7 +4065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4045,7 +4091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -4071,7 +4117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4100,16 +4146,16 @@
         <v>-0.1325530043077417</v>
       </c>
       <c r="J9">
-        <v>0.1086826442074059</v>
+        <v>0.10868264420740591</v>
       </c>
       <c r="K9">
-        <v>-0.1612223880273475</v>
+        <v>-0.16122238802734751</v>
       </c>
       <c r="L9">
         <v>0.1090548020620709</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -4135,19 +4181,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.004001088444105332</v>
+        <v>-4.0010884441053322E-3</v>
       </c>
       <c r="J10">
-        <v>0.9739374982488735</v>
+        <v>0.97393749824887355</v>
       </c>
       <c r="K10">
-        <v>-0.004014544573191041</v>
+        <v>-4.0145445731910407E-3</v>
       </c>
       <c r="L10">
-        <v>0.9779259755977681</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.97792597559776806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -4173,19 +4219,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.01888959038201153</v>
+        <v>-1.8889590382011531E-2</v>
       </c>
       <c r="J11">
         <v>0.8717029852220165</v>
       </c>
       <c r="K11">
-        <v>-0.02206154843492711</v>
+        <v>-2.2061548434927108E-2</v>
       </c>
       <c r="L11">
-        <v>0.8791305588586364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.87913055885863645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4211,19 +4257,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2476064162497625</v>
+        <v>-0.24760641624976251</v>
       </c>
       <c r="J12">
-        <v>0.0331142128596994</v>
+        <v>3.3114212859699399E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3099127537051835</v>
+        <v>-0.30991275370518351</v>
       </c>
       <c r="L12">
-        <v>0.02850794708171081</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.850794708171081E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -4261,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4290,16 +4336,16 @@
         <v>0.6085806194501846</v>
       </c>
       <c r="J14">
-        <v>0.03300625766123251</v>
+        <v>3.300625766123251E-2</v>
       </c>
       <c r="K14">
-        <v>0.7106690545187014</v>
+        <v>0.71066905451870144</v>
       </c>
       <c r="L14">
-        <v>0.02124449212877441</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>2.1244492128774412E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -4325,19 +4371,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.6770032003863301</v>
+        <v>0.67700320038633011</v>
       </c>
       <c r="J15">
-        <v>0.01865536081150319</v>
+        <v>1.865536081150319E-2</v>
       </c>
       <c r="K15">
-        <v>0.7841156792042765</v>
+        <v>0.78411567920427649</v>
       </c>
       <c r="L15">
-        <v>0.007255789526699558</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>7.2557895266995576E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -4366,16 +4412,16 @@
         <v>-0.1217161238900369</v>
       </c>
       <c r="J16">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K16">
         <v>-0.1421338109037403</v>
       </c>
       <c r="L16">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4404,16 +4450,16 @@
         <v>-0.3042903097250923</v>
       </c>
       <c r="J17">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K17">
-        <v>-0.3553345272593507</v>
+        <v>-0.35533452725935072</v>
       </c>
       <c r="L17">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4439,19 +4485,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.06085806194501846</v>
+        <v>6.0858061945018457E-2</v>
       </c>
       <c r="J18">
-        <v>0.8311704095417624</v>
+        <v>0.83117040954176236</v>
       </c>
       <c r="K18">
-        <v>0.07106690545187015</v>
+        <v>7.1066905451870152E-2</v>
       </c>
       <c r="L18">
-        <v>0.8453239136912953</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.84532391369129534</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4477,19 +4523,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.09231861823449956</v>
+        <v>9.2318618234499564E-2</v>
       </c>
       <c r="J19">
-        <v>0.7483812122920345</v>
+        <v>0.74838121229203447</v>
       </c>
       <c r="K19">
-        <v>0.1069248653460377</v>
+        <v>0.10692486534603771</v>
       </c>
       <c r="L19">
-        <v>0.7687577033932652</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.76875770339326521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4515,19 +4561,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.06085806194501846</v>
+        <v>-6.0858061945018457E-2</v>
       </c>
       <c r="J20">
-        <v>0.8311704095417624</v>
+        <v>0.83117040954176236</v>
       </c>
       <c r="K20">
-        <v>-0.07106690545187015</v>
+        <v>-7.1066905451870152E-2</v>
       </c>
       <c r="L20">
-        <v>0.8453239136912953</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.84532391369129534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -4553,19 +4599,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2434322477800739</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J21">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K21">
-        <v>-0.2842676218074806</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L21">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -4594,16 +4640,16 @@
         <v>0.1217161238900369</v>
       </c>
       <c r="J22">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K22">
         <v>0.1421338109037403</v>
       </c>
       <c r="L22">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4629,19 +4675,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.2434322477800739</v>
+        <v>0.24343224778007391</v>
       </c>
       <c r="J23">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K23">
-        <v>0.2842676218074806</v>
+        <v>0.28426762180748061</v>
       </c>
       <c r="L23">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -4667,19 +4713,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2434322477800739</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J24">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K24">
-        <v>-0.2842676218074806</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L24">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -4705,19 +4751,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.3535533905932737</v>
+        <v>-0.35355339059327368</v>
       </c>
       <c r="J25">
         <v>0.1037416782365415</v>
       </c>
       <c r="K25">
-        <v>-0.4200840252084029</v>
+        <v>-0.42008402520840288</v>
       </c>
       <c r="L25">
         <v>0.105228057983522</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -4743,19 +4789,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1649915822768611</v>
+        <v>-0.16499158227686109</v>
       </c>
       <c r="J26">
         <v>0.4476990724652935</v>
       </c>
       <c r="K26">
-        <v>-0.1960392117639214</v>
+        <v>-0.19603921176392139</v>
       </c>
       <c r="L26">
         <v>0.4668248490265503</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -4781,19 +4827,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.02366905341655754</v>
+        <v>2.3669053416557541E-2</v>
       </c>
       <c r="J27">
-        <v>0.9135633303377861</v>
+        <v>0.91356333033778614</v>
       </c>
       <c r="K27">
-        <v>0.02802621677476181</v>
+        <v>2.802621677476181E-2</v>
       </c>
       <c r="L27">
-        <v>0.9179387985999929</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.91793879859999294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -4819,19 +4865,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.2625754538144587</v>
+        <v>-0.26257545381445868</v>
       </c>
       <c r="J28">
-        <v>0.2314460271038938</v>
+        <v>0.23144602710389381</v>
       </c>
       <c r="K28">
-        <v>-0.3089716991054783</v>
+        <v>-0.30897169910547828</v>
       </c>
       <c r="L28">
-        <v>0.2442606266224961</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.24426062662249609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -4857,13 +4903,13 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.2592724864350675</v>
+        <v>0.25927248643506751</v>
       </c>
       <c r="J29">
         <v>0.2328233516916538</v>
       </c>
       <c r="K29">
-        <v>0.3080616184861621</v>
+        <v>0.30806161848616209</v>
       </c>
       <c r="L29">
         <v>0.2457251662216493</v>
@@ -4871,16 +4917,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -4896,7 +4943,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4934,7 +4981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4960,7 +5007,7 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.2588600915717736</v>
+        <v>-0.25886009157177359</v>
       </c>
       <c r="J2">
         <v>0.1185826134820492</v>
@@ -4972,7 +5019,7 @@
         <v>0.157096814687567</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5001,16 +5048,16 @@
         <v>-0.3630554894720564</v>
       </c>
       <c r="J3">
-        <v>0.02649782086730554</v>
+        <v>2.6497820867305542E-2</v>
       </c>
       <c r="K3">
-        <v>-0.4471228632493155</v>
+        <v>-0.44712286324931549</v>
       </c>
       <c r="L3">
-        <v>0.03242678547292783</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>3.2426785472927828E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -5036,19 +5083,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.3826849293392768</v>
+        <v>0.38268492933927678</v>
       </c>
       <c r="J4">
-        <v>0.01856470797931634</v>
+        <v>1.856470797931634E-2</v>
       </c>
       <c r="K4">
-        <v>0.4532739558663172</v>
+        <v>0.45327395586631719</v>
       </c>
       <c r="L4">
-        <v>0.0298421137496698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>2.9842113749669798E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5077,16 +5124,16 @@
         <v>-0.2018433569398328</v>
       </c>
       <c r="J5">
-        <v>0.4065712940338708</v>
+        <v>0.40657129403387082</v>
       </c>
       <c r="K5">
         <v>-0.2056848110006326</v>
       </c>
       <c r="L5">
-        <v>0.521309719682044</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.52130971968204398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5112,10 +5159,10 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.2385421491107114</v>
+        <v>-0.23854214911071139</v>
       </c>
       <c r="J6">
-        <v>0.326671088638757</v>
+        <v>0.32667108863875699</v>
       </c>
       <c r="K6">
         <v>-0.2437745908155646</v>
@@ -5124,7 +5171,7 @@
         <v>0.4451488240391529</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -5150,19 +5197,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.4954336943068622</v>
+        <v>-0.49543369430686218</v>
       </c>
       <c r="J7">
-        <v>0.0416368567827736</v>
+        <v>4.1636856782773603E-2</v>
       </c>
       <c r="K7">
-        <v>-0.5561107852980067</v>
+        <v>-0.55611078529800673</v>
       </c>
       <c r="L7">
-        <v>0.06043495620092659</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>6.0434956200926593E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5188,19 +5235,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.3486385256233475</v>
+        <v>0.34863852562334752</v>
       </c>
       <c r="J8">
-        <v>0.1517044197305971</v>
+        <v>0.15170441973059709</v>
       </c>
       <c r="K8">
-        <v>0.4037516660382788</v>
+        <v>0.40375166603827878</v>
       </c>
       <c r="L8">
-        <v>0.1930534976448194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.19305349764481941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5229,16 +5276,16 @@
         <v>-0.1508932577851104</v>
       </c>
       <c r="J9">
-        <v>0.03976539977998658</v>
+        <v>3.9765399779986582E-2</v>
       </c>
       <c r="K9">
-        <v>-0.2101007063448729</v>
+        <v>-0.21010070634487291</v>
       </c>
       <c r="L9">
-        <v>0.03589890255176344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3.5898902551763437E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -5264,19 +5311,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.02584053907657639</v>
+        <v>-2.584053907657639E-2</v>
       </c>
       <c r="J10">
-        <v>0.8319012317886401</v>
+        <v>0.83190123178864006</v>
       </c>
       <c r="K10">
-        <v>-0.02491868767248899</v>
+        <v>-2.491868767248899E-2</v>
       </c>
       <c r="L10">
-        <v>0.8636170341288709</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.86361703412887092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -5302,19 +5349,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-2.439922062337898E-2</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.83378844789272755</v>
       </c>
       <c r="K11">
-        <v>-0.02888208251072132</v>
+        <v>-2.8882082510721319E-2</v>
       </c>
       <c r="L11">
-        <v>0.8421820698041393</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.84218206980413934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5340,19 +5387,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.25161225674918491</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>2.940004335865699E-2</v>
       </c>
       <c r="K12">
-        <v>-0.311094163299463</v>
+        <v>-0.31109416329946299</v>
       </c>
       <c r="L12">
-        <v>0.02787696039183273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.7876960391832729E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -5378,19 +5425,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.04969039949999533</v>
+        <v>4.9690399499995333E-2</v>
       </c>
       <c r="J13">
-        <v>0.8509806870320558</v>
+        <v>0.85098068703205576</v>
       </c>
       <c r="K13">
-        <v>0.01262892050706804</v>
+        <v>1.262892050706804E-2</v>
       </c>
       <c r="L13">
-        <v>0.9723786419920799</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>0.97237864199207991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -5416,19 +5463,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.149071198499986</v>
+        <v>-0.14907119849998601</v>
       </c>
       <c r="J14">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K14">
         <v>-0.1894338076060206</v>
       </c>
       <c r="L14">
-        <v>0.6001664342511973</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.60016643425119731</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5454,19 +5501,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.1256297269074015</v>
+        <v>-0.12562972690740151</v>
       </c>
       <c r="J15">
-        <v>0.6374017405958849</v>
+        <v>0.63740174059588495</v>
       </c>
       <c r="K15">
-        <v>-0.152008377581442</v>
+        <v>-0.15200837758144201</v>
       </c>
       <c r="L15">
-        <v>0.6750590889374006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.67505908893740063</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -5492,19 +5539,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.298142396999972</v>
+        <v>-0.29814239699997203</v>
       </c>
       <c r="J16">
-        <v>0.2596563563704499</v>
+        <v>0.25965635637044993</v>
       </c>
       <c r="K16">
-        <v>-0.3788676152120412</v>
+        <v>-0.37886761521204121</v>
       </c>
       <c r="L16">
-        <v>0.2802942824523375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.28029428245233751</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -5533,16 +5580,16 @@
         <v>-0.1987615979999813</v>
       </c>
       <c r="J17">
-        <v>0.4523703606773608</v>
+        <v>0.45237036067736081</v>
       </c>
       <c r="K17">
-        <v>-0.3409808536908371</v>
+        <v>-0.34098085369083708</v>
       </c>
       <c r="L17">
-        <v>0.3349456951179903</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>0.33494569511799033</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -5568,19 +5615,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.149071198499986</v>
+        <v>0.14907119849998601</v>
       </c>
       <c r="J18">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K18">
-        <v>0.1641759665918845</v>
+        <v>0.16417596659188449</v>
       </c>
       <c r="L18">
-        <v>0.6503895621649565</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.65038956216495647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -5606,19 +5653,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.07537783614444091</v>
+        <v>7.5377836144440907E-2</v>
       </c>
       <c r="J19">
-        <v>0.7773295263554205</v>
+        <v>0.77732952635542052</v>
       </c>
       <c r="K19">
         <v>0.1076726007868547</v>
       </c>
       <c r="L19">
-        <v>0.7671778789420547</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.76717787894205469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -5644,19 +5691,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.09938079899999065</v>
+        <v>-9.9380798999990652E-2</v>
       </c>
       <c r="J20">
         <v>0.7071142312899612</v>
       </c>
       <c r="K20">
-        <v>-0.1262892050706804</v>
+        <v>-0.12628920507068039</v>
       </c>
       <c r="L20">
-        <v>0.7281063840216824</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.72810638402168237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -5682,19 +5729,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.149071198499986</v>
+        <v>-0.14907119849998601</v>
       </c>
       <c r="J21">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K21">
         <v>-0.2399494896342928</v>
       </c>
       <c r="L21">
-        <v>0.5043017190353258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.50430171903532583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -5720,19 +5767,19 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.3975231959999626</v>
+        <v>0.39752319599996261</v>
       </c>
       <c r="J22">
         <v>0.1328549557310538</v>
       </c>
       <c r="K22">
-        <v>0.5304146612968577</v>
+        <v>0.53041466129685766</v>
       </c>
       <c r="L22">
         <v>0.1147392659290222</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -5758,19 +5805,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.298142396999972</v>
+        <v>0.29814239699997203</v>
       </c>
       <c r="J23">
-        <v>0.2596563563704499</v>
+        <v>0.25965635637044993</v>
       </c>
       <c r="K23">
-        <v>0.4041254562261773</v>
+        <v>0.40412545622617729</v>
       </c>
       <c r="L23">
-        <v>0.2467547295422347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.24675472954223471</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -5799,16 +5846,16 @@
         <v>-0.2484519974999766</v>
       </c>
       <c r="J24">
-        <v>0.347558036741169</v>
+        <v>0.34755803674116897</v>
       </c>
       <c r="K24">
-        <v>-0.4293832972403134</v>
+        <v>-0.42938329724031338</v>
       </c>
       <c r="L24">
-        <v>0.2155824117700313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.21558241177003129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -5834,7 +5881,7 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.31352722326441</v>
+        <v>-0.31352722326441002</v>
       </c>
       <c r="J25">
         <v>0.1131685336545776</v>
@@ -5843,10 +5890,10 @@
         <v>-0.4479914656638877</v>
       </c>
       <c r="L25">
-        <v>0.08182143505121871</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>8.1821435051218708E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -5875,16 +5922,16 @@
         <v>-0.3872983346207417</v>
       </c>
       <c r="J26">
-        <v>0.05036597579032801</v>
+        <v>5.0365975790328012E-2</v>
       </c>
       <c r="K26">
-        <v>-0.5070173682344674</v>
+        <v>-0.50701736823446741</v>
       </c>
       <c r="L26">
-        <v>0.04501930875693567</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>4.5019308756935668E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -5910,19 +5957,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.08334047874242113</v>
+        <v>8.3340478742421134E-2</v>
       </c>
       <c r="J27">
         <v>0.6747078413451294</v>
       </c>
       <c r="K27">
-        <v>0.08027373462987823</v>
+        <v>8.0273734629878232E-2</v>
       </c>
       <c r="L27">
-        <v>0.7675926515511813</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.76759265155118128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -5948,19 +5995,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>0.09338863578008762</v>
+        <v>9.3388635780087617E-2</v>
       </c>
       <c r="J28">
-        <v>0.6401498414586226</v>
+        <v>0.64014984145862264</v>
       </c>
       <c r="K28">
         <v>0.1305442024324843</v>
       </c>
       <c r="L28">
-        <v>0.6298840619248964</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.62988406192489643</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -5986,19 +6033,20 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.1290994448735805</v>
+        <v>0.12909944487358049</v>
       </c>
       <c r="J29">
-        <v>0.5142199988155506</v>
+        <v>0.51421999881555058</v>
       </c>
       <c r="K29">
-        <v>0.1619428608987702</v>
+        <v>0.16194286089877019</v>
       </c>
       <c r="L29">
-        <v>0.5490376092324329</v>
+        <v>0.54903760923243294</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix issue with DS 6 results
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -508,7 +508,7 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -880,16 +880,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-0.004414751593059719</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.9661430518463994</v>
       </c>
       <c r="K10">
-        <v>-0.01605248793883186</v>
+        <v>0.01233315619210278</v>
       </c>
       <c r="L10">
-        <v>0.9118983828429555</v>
+        <v>0.932256616388448</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -918,16 +918,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.0319066731228802</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.7837672300250216</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>-0.03045075791865187</v>
+        <v>0.01007744778718968</v>
       </c>
       <c r="L11">
-        <v>0.8337285990222609</v>
+        <v>0.9446252971798705</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -956,16 +956,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2441570787714312</v>
+        <v>0.04719010357797921</v>
       </c>
       <c r="J12">
-        <v>0.03455416553919029</v>
+        <v>0.632959082865391</v>
       </c>
       <c r="K12">
-        <v>-0.3094340106343606</v>
+        <v>0.07620564634846749</v>
       </c>
       <c r="L12">
-        <v>0.02876701130235894</v>
+        <v>0.5988937623118764</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1961,16 +1961,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-0.2741939043543897</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.01523742906785629</v>
       </c>
       <c r="K10">
-        <v>-0.02174552145202223</v>
+        <v>-0.3438060590640694</v>
       </c>
       <c r="L10">
-        <v>0.8808493755591094</v>
+        <v>0.0145005762354219</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1999,16 +1999,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-0.2885159533670518</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.007534224862278689</v>
       </c>
       <c r="K11">
-        <v>-0.02805160729475809</v>
+        <v>-0.3916527812158478</v>
       </c>
       <c r="L11">
-        <v>0.8466646412386398</v>
+        <v>0.004913052567611288</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2037,16 +2037,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>0.1527404930393114</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>0.1545006958890939</v>
       </c>
       <c r="K12">
-        <v>-0.3118320089283974</v>
+        <v>0.1874148805812322</v>
       </c>
       <c r="L12">
-        <v>0.02748882596687927</v>
+        <v>0.192476549579598</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2716,9 +2716,9 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3090,16 +3090,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01391413642584883</v>
+        <v>0.03324642499485375</v>
       </c>
       <c r="J10">
-        <v>0.9090032366864784</v>
+        <v>0.7524695495544889</v>
       </c>
       <c r="K10">
-        <v>-0.01026612600739247</v>
+        <v>0.05369692827151148</v>
       </c>
       <c r="L10">
-        <v>0.9435901857829745</v>
+        <v>0.7111154281850389</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3128,16 +3128,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>0.02630142666529713</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.7941029996140164</v>
       </c>
       <c r="K11">
-        <v>-0.0299893827986723</v>
+        <v>0.0345247475921612</v>
       </c>
       <c r="L11">
-        <v>0.8362130272367809</v>
+        <v>0.8118632018166435</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3166,16 +3166,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>0.02696081483975262</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>0.7877495099042957</v>
       </c>
       <c r="K12">
-        <v>-0.3096184720415943</v>
+        <v>0.03904490288887924</v>
       </c>
       <c r="L12">
-        <v>0.02866696147428332</v>
+        <v>0.7877690834629696</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3847,7 +3847,7 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4135,16 +4135,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.004001088444105332</v>
+        <v>-0.1454025530693833</v>
       </c>
       <c r="J10">
-        <v>0.9739374982488735</v>
+        <v>0.2372373518450496</v>
       </c>
       <c r="K10">
-        <v>-0.004014544573191041</v>
+        <v>-0.17271903862684</v>
       </c>
       <c r="L10">
-        <v>0.9779259755977681</v>
+        <v>0.2303502122764337</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4173,16 +4173,16 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.01888959038201153</v>
+        <v>-0.1395616700784287</v>
       </c>
       <c r="J11">
-        <v>0.8717029852220165</v>
+        <v>0.2348980869048207</v>
       </c>
       <c r="K11">
-        <v>-0.02206154843492711</v>
+        <v>-0.1674579385094694</v>
       </c>
       <c r="L11">
-        <v>0.8791305588586364</v>
+        <v>0.2450782275649824</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4211,16 +4211,16 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2476064162497625</v>
+        <v>0.02140819589682411</v>
       </c>
       <c r="J12">
-        <v>0.0331142128596994</v>
+        <v>0.8544862615484419</v>
       </c>
       <c r="K12">
-        <v>-0.3099127537051835</v>
+        <v>0.02708713119452734</v>
       </c>
       <c r="L12">
-        <v>0.02850794708171081</v>
+        <v>0.8518765230635053</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5264,16 +5264,16 @@
         <v>49</v>
       </c>
       <c r="I10">
-        <v>0.03422036410971387</v>
+        <v>-0.1679543721361666</v>
       </c>
       <c r="J10">
-        <v>0.7818977362007468</v>
+        <v>0.1236240407674998</v>
       </c>
       <c r="K10">
-        <v>0.04252367998412877</v>
+        <v>-0.1891736836680379</v>
       </c>
       <c r="L10">
-        <v>0.7717300425982628</v>
+        <v>0.1929773116581186</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5302,16 +5302,16 @@
         <v>49</v>
       </c>
       <c r="I11">
-        <v>0.01076426888425463</v>
+        <v>-0.1257020377320922</v>
       </c>
       <c r="J11">
-        <v>0.9273329987305904</v>
+        <v>0.2278618094667795</v>
       </c>
       <c r="K11">
-        <v>0.008061812533558553</v>
+        <v>-0.1630362203611797</v>
       </c>
       <c r="L11">
-        <v>0.9561570140240785</v>
+        <v>0.2630118256866814</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5340,16 +5340,16 @@
         <v>49</v>
       </c>
       <c r="I12">
-        <v>-0.2437500527506231</v>
+        <v>0.09860866138702759</v>
       </c>
       <c r="J12">
-        <v>0.03767751829147191</v>
+        <v>0.3411530572805948</v>
       </c>
       <c r="K12">
-        <v>-0.290944056466156</v>
+        <v>0.1348255148415411</v>
       </c>
       <c r="L12">
-        <v>0.04254594694787119</v>
+        <v>0.3556729989431554</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>

<commit_message>
updated results with infer-no-filter
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -874,22 +874,22 @@
         <v>48</v>
       </c>
       <c r="G10">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.07151897580756746</v>
+        <v>-0.07157910106056362</v>
       </c>
       <c r="J10">
-        <v>0.4917488054518981</v>
+        <v>0.4916600219100405</v>
       </c>
       <c r="K10">
-        <v>-0.08931126357943785</v>
+        <v>-0.08830673038161191</v>
       </c>
       <c r="L10">
-        <v>0.5373749382690856</v>
+        <v>0.5419792899048017</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -912,22 +912,22 @@
         <v>48</v>
       </c>
       <c r="G11">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.05168950124013011</v>
+        <v>-0.05507056613029693</v>
       </c>
       <c r="J11">
-        <v>0.6032567277221177</v>
+        <v>0.5800104076897017</v>
       </c>
       <c r="K11">
-        <v>-0.07214314607514075</v>
+        <v>-0.07444201065306216</v>
       </c>
       <c r="L11">
-        <v>0.6185714228997314</v>
+        <v>0.6074026216973724</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -950,22 +950,22 @@
         <v>48</v>
       </c>
       <c r="G12">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1067986554659529</v>
+        <v>0.1102028102074909</v>
       </c>
       <c r="J12">
-        <v>0.2798502856543867</v>
+        <v>0.265108023071319</v>
       </c>
       <c r="K12">
-        <v>0.163493994752763</v>
+        <v>0.1660257192865707</v>
       </c>
       <c r="L12">
-        <v>0.2565888686910258</v>
+        <v>0.2491959671429019</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1444,22 +1444,22 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1626978433639921</v>
+        <v>-0.1807753815155468</v>
       </c>
       <c r="J25">
-        <v>0.4043745903773081</v>
+        <v>0.3541954904764164</v>
       </c>
       <c r="K25">
-        <v>-0.2500726110965064</v>
+        <v>-0.2576049186596542</v>
       </c>
       <c r="L25">
-        <v>0.3502469232913418</v>
+        <v>0.3354345184285685</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1482,22 +1482,22 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1988529196671015</v>
+        <v>-0.1807753815155468</v>
       </c>
       <c r="J26">
-        <v>0.3081411014502622</v>
+        <v>0.3541954904764164</v>
       </c>
       <c r="K26">
-        <v>-0.2741759952985793</v>
+        <v>-0.2666436877354316</v>
       </c>
       <c r="L26">
-        <v>0.3041353554760347</v>
+        <v>0.3181414648703181</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1520,22 +1520,22 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3721433734379864</v>
+        <v>0.3539900381483285</v>
       </c>
       <c r="J27">
-        <v>0.05729901570416417</v>
+        <v>0.07056136851892029</v>
       </c>
       <c r="K27">
-        <v>0.443979491086295</v>
+        <v>0.4341802833034056</v>
       </c>
       <c r="L27">
-        <v>0.08493122100226924</v>
+        <v>0.09288178063084394</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H28">
         <v>16</v>
@@ -1570,10 +1570,10 @@
         <v>0.4027546538976249</v>
       </c>
       <c r="K28">
-        <v>-0.2341913484699036</v>
+        <v>-0.2493004677260264</v>
       </c>
       <c r="L28">
-        <v>0.3826574736700414</v>
+        <v>0.3517858440384553</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1596,7 +1596,7 @@
         <v>15</v>
       </c>
       <c r="G29">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H29">
         <v>16</v>
@@ -1608,10 +1608,10 @@
         <v>0.5166373798159882</v>
       </c>
       <c r="K29">
-        <v>-0.159684920338733</v>
+        <v>-0.1491396897503261</v>
       </c>
       <c r="L29">
-        <v>0.554695992273345</v>
+        <v>0.5814513259975999</v>
       </c>
     </row>
   </sheetData>
@@ -4126,25 +4126,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.1913882186302207</v>
+        <v>-0.1454025530693833</v>
       </c>
       <c r="J10">
-        <v>0.1232008006808224</v>
+        <v>0.2372373518450496</v>
       </c>
       <c r="K10">
-        <v>-0.2202109622728743</v>
+        <v>-0.17271903862684</v>
       </c>
       <c r="L10">
-        <v>0.1243730565524269</v>
+        <v>0.2303502122764337</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4164,25 +4164,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.1807130786720777</v>
+        <v>-0.1395616700784287</v>
       </c>
       <c r="J11">
-        <v>0.1274891908063156</v>
+        <v>0.2348980869048207</v>
       </c>
       <c r="K11">
-        <v>-0.2177254496446563</v>
+        <v>-0.1674579385094694</v>
       </c>
       <c r="L11">
-        <v>0.1287880141876493</v>
+        <v>0.2450782275649824</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4202,25 +4202,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.04052204492365539</v>
+        <v>0.02140819589682411</v>
       </c>
       <c r="J12">
-        <v>0.7308602875071768</v>
+        <v>0.8544862615484419</v>
       </c>
       <c r="K12">
-        <v>-0.04914019746654562</v>
+        <v>0.02708713119452734</v>
       </c>
       <c r="L12">
-        <v>0.7346926691344551</v>
+        <v>0.8518765230635053</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4696,13 +4696,25 @@
         <v>16</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>16</v>
+      </c>
+      <c r="I25">
+        <v>-0.3535533905932737</v>
+      </c>
+      <c r="J25">
+        <v>0.1037416782365415</v>
+      </c>
+      <c r="K25">
+        <v>-0.4200840252084029</v>
+      </c>
+      <c r="L25">
+        <v>0.105228057983522</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -4722,13 +4734,25 @@
         <v>16</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>16</v>
+      </c>
+      <c r="I26">
+        <v>-0.1649915822768611</v>
+      </c>
+      <c r="J26">
+        <v>0.4476990724652935</v>
+      </c>
+      <c r="K26">
+        <v>-0.1960392117639214</v>
+      </c>
+      <c r="L26">
+        <v>0.4668248490265503</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -4748,13 +4772,25 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>16</v>
+      </c>
+      <c r="I27">
+        <v>0.02366905341655754</v>
+      </c>
+      <c r="J27">
+        <v>0.9135633303377861</v>
+      </c>
+      <c r="K27">
+        <v>0.02802621677476181</v>
+      </c>
+      <c r="L27">
+        <v>0.9179387985999929</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -4774,13 +4810,25 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>16</v>
+      </c>
+      <c r="I28">
+        <v>-0.2625754538144587</v>
+      </c>
+      <c r="J28">
+        <v>0.2314460271038938</v>
+      </c>
+      <c r="K28">
+        <v>-0.3089716991054783</v>
+      </c>
+      <c r="L28">
+        <v>0.2442606266224961</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -4800,13 +4848,25 @@
         <v>16</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>16</v>
+      </c>
+      <c r="I29">
+        <v>0.2592724864350675</v>
+      </c>
+      <c r="J29">
+        <v>0.2328233516916538</v>
+      </c>
+      <c r="K29">
+        <v>0.3080616184861621</v>
+      </c>
+      <c r="L29">
+        <v>0.2457251662216493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results w/ openjml handling fixed
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -506,8 +506,8 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
@@ -836,22 +836,22 @@
         <v>94</v>
       </c>
       <c r="G9">
-        <v>498</v>
+        <v>1143</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2267615580201486</v>
+        <v>-0.166102596545867</v>
       </c>
       <c r="J9">
-        <v>0.001375395213558095</v>
+        <v>0.01727604806480851</v>
       </c>
       <c r="K9">
-        <v>-0.3306847132478023</v>
+        <v>-0.2527623213330977</v>
       </c>
       <c r="L9">
-        <v>0.000778487901037674</v>
+        <v>0.01117475265921138</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -874,22 +874,22 @@
         <v>48</v>
       </c>
       <c r="G10">
-        <v>813</v>
+        <v>859</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.07157910106056362</v>
+        <v>-0.004414751593059719</v>
       </c>
       <c r="J10">
-        <v>0.4916600219100405</v>
+        <v>0.9661430518463994</v>
       </c>
       <c r="K10">
-        <v>-0.08830673038161191</v>
+        <v>0.01233315619210278</v>
       </c>
       <c r="L10">
-        <v>0.5419792899048017</v>
+        <v>0.932256616388448</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -912,22 +912,22 @@
         <v>48</v>
       </c>
       <c r="G11">
-        <v>813</v>
+        <v>859</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.05507056613029693</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.5800104076897017</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>-0.07444201065306216</v>
+        <v>0.01007744778718968</v>
       </c>
       <c r="L11">
-        <v>0.6074026216973724</v>
+        <v>0.9446252971798705</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -950,22 +950,22 @@
         <v>48</v>
       </c>
       <c r="G12">
-        <v>813</v>
+        <v>859</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1102028102074909</v>
+        <v>0.04719010357797921</v>
       </c>
       <c r="J12">
-        <v>0.265108023071319</v>
+        <v>0.632959082865391</v>
       </c>
       <c r="K12">
-        <v>0.1660257192865707</v>
+        <v>0.07620564634846749</v>
       </c>
       <c r="L12">
-        <v>0.2491959671429019</v>
+        <v>0.5988937623118764</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4891,7 +4891,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
@@ -5220,22 +5220,22 @@
         <v>69</v>
       </c>
       <c r="G9">
-        <v>106</v>
+        <v>751</v>
       </c>
       <c r="H9">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.1004064600277419</v>
+        <v>-0.1230941982211943</v>
       </c>
       <c r="J9">
-        <v>0.3197996198904468</v>
+        <v>0.107046316578524</v>
       </c>
       <c r="K9">
-        <v>-0.1258658290311623</v>
+        <v>-0.1671214681732231</v>
       </c>
       <c r="L9">
-        <v>0.3337653039608836</v>
+        <v>0.09653017580355105</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5258,22 +5258,22 @@
         <v>41</v>
       </c>
       <c r="G10">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="H10">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.2134569412305524</v>
+        <v>-0.1410673005708742</v>
       </c>
       <c r="J10">
-        <v>0.05383248704028133</v>
+        <v>0.1918480862059539</v>
       </c>
       <c r="K10">
-        <v>-0.254689962010721</v>
+        <v>-0.1594915550278049</v>
       </c>
       <c r="L10">
-        <v>0.08064290874044987</v>
+        <v>0.2685745446816231</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5296,22 +5296,22 @@
         <v>41</v>
       </c>
       <c r="G11">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="H11">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.1499545016214044</v>
+        <v>-0.1104149035826812</v>
       </c>
       <c r="J11">
-        <v>0.1564334829386408</v>
+        <v>0.285180706372306</v>
       </c>
       <c r="K11">
-        <v>-0.2015245812013276</v>
+        <v>-0.1439811999024739</v>
       </c>
       <c r="L11">
-        <v>0.1695848710732239</v>
+        <v>0.318492693335327</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5334,22 +5334,22 @@
         <v>41</v>
       </c>
       <c r="G12">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="H12">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1670554193005554</v>
+        <v>0.1113864967082373</v>
       </c>
       <c r="J12">
-        <v>0.1123317103170471</v>
+        <v>0.2778961820094916</v>
       </c>
       <c r="K12">
-        <v>0.2349915639777836</v>
+        <v>0.1553560043181458</v>
       </c>
       <c r="L12">
-        <v>0.1078882378308313</v>
+        <v>0.2813439520692285</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>

<commit_message>
fixed removing snippets with timeouts
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -4891,7 +4891,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
@@ -5223,19 +5223,19 @@
         <v>751</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="I9">
-        <v>-0.1230941982211943</v>
+        <v>-0.1004064600277419</v>
       </c>
       <c r="J9">
-        <v>0.107046316578524</v>
+        <v>0.3197996198904468</v>
       </c>
       <c r="K9">
-        <v>-0.1671214681732231</v>
+        <v>-0.1258658290311623</v>
       </c>
       <c r="L9">
-        <v>0.09653017580355105</v>
+        <v>0.3337653039608836</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5261,19 +5261,19 @@
         <v>215</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10">
-        <v>-0.1410673005708742</v>
+        <v>-0.2134569412305524</v>
       </c>
       <c r="J10">
-        <v>0.1918480862059539</v>
+        <v>0.05383248704028133</v>
       </c>
       <c r="K10">
-        <v>-0.1594915550278049</v>
+        <v>-0.254689962010721</v>
       </c>
       <c r="L10">
-        <v>0.2685745446816231</v>
+        <v>0.08064290874044987</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5299,19 +5299,19 @@
         <v>215</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11">
-        <v>-0.1104149035826812</v>
+        <v>-0.1499545016214044</v>
       </c>
       <c r="J11">
-        <v>0.285180706372306</v>
+        <v>0.1564334829386408</v>
       </c>
       <c r="K11">
-        <v>-0.1439811999024739</v>
+        <v>-0.2015245812013276</v>
       </c>
       <c r="L11">
-        <v>0.318492693335327</v>
+        <v>0.1695848710732239</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5337,19 +5337,19 @@
         <v>215</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12">
-        <v>0.1113864967082373</v>
+        <v>0.1670554193005554</v>
       </c>
       <c r="J12">
-        <v>0.2778961820094916</v>
+        <v>0.1123317103170471</v>
       </c>
       <c r="K12">
-        <v>0.1553560043181458</v>
+        <v>0.2349915639777836</v>
       </c>
       <c r="L12">
-        <v>0.2813439520692285</v>
+        <v>0.1078882378308313</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>

<commit_message>
running pipeline on new warning sets
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -506,10 +506,10 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -699,7 +699,7 @@
         <v>-0.3178304128441319</v>
       </c>
       <c r="L5">
-        <v>0.3140610795011266</v>
+        <v>0.3140610795011265</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -833,25 +833,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2267615580201486</v>
+        <v>-0.2232481170885827</v>
       </c>
       <c r="J9">
-        <v>0.001375395213558095</v>
+        <v>0.001636069376151588</v>
       </c>
       <c r="K9">
-        <v>-0.3306847132478023</v>
+        <v>-0.3234519555354279</v>
       </c>
       <c r="L9">
-        <v>0.000778487901037674</v>
+        <v>0.001028681640569814</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -871,25 +871,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10">
-        <v>813</v>
+        <v>794</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.07157910106056362</v>
+        <v>-0.05768310136706124</v>
       </c>
       <c r="J10">
-        <v>0.4916600219100405</v>
+        <v>0.5808166089173682</v>
       </c>
       <c r="K10">
-        <v>-0.08830673038161191</v>
+        <v>-0.06873895440322977</v>
       </c>
       <c r="L10">
-        <v>0.5419792899048017</v>
+        <v>0.635267646345926</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -909,25 +909,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11">
-        <v>813</v>
+        <v>794</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.05507056613029693</v>
+        <v>-0.03854494781179903</v>
       </c>
       <c r="J11">
-        <v>0.5800104076897017</v>
+        <v>0.6995394491817443</v>
       </c>
       <c r="K11">
-        <v>-0.07444201065306216</v>
+        <v>-0.04832503745113209</v>
       </c>
       <c r="L11">
-        <v>0.6074026216973724</v>
+        <v>0.7389368221688255</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -947,25 +947,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G12">
-        <v>813</v>
+        <v>794</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1102028102074909</v>
+        <v>0.1156617751198898</v>
       </c>
       <c r="J12">
-        <v>0.265108023071319</v>
+        <v>0.2438312496350385</v>
       </c>
       <c r="K12">
-        <v>0.1660257192865707</v>
+        <v>0.1718948469712283</v>
       </c>
       <c r="L12">
-        <v>0.2491959671429019</v>
+        <v>0.2326162766495191</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -988,22 +988,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4535394202249742</v>
+        <v>-0.3373495424699933</v>
       </c>
       <c r="J13">
-        <v>0.08070214265077501</v>
+        <v>0.2074202127647988</v>
       </c>
       <c r="K13">
-        <v>-0.5512130501182249</v>
+        <v>-0.4296689244236597</v>
       </c>
       <c r="L13">
-        <v>0.09862398123473154</v>
+        <v>0.215243543278886</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1026,22 +1026,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.02387049580131443</v>
+        <v>-0.1816497536376887</v>
       </c>
       <c r="J14">
-        <v>0.92675547372309</v>
+        <v>0.4972433060612282</v>
       </c>
       <c r="K14">
-        <v>-0.09290107586262218</v>
+        <v>-0.2669155439601523</v>
       </c>
       <c r="L14">
-        <v>0.7985237548304135</v>
+        <v>0.4559719917038285</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1064,22 +1064,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.09656090991705352</v>
+        <v>-0.0524863881081478</v>
       </c>
       <c r="J15">
-        <v>0.7120793980044939</v>
+        <v>0.8456867367859529</v>
       </c>
       <c r="K15">
-        <v>0.1428819499477476</v>
+        <v>-0.06856450678985078</v>
       </c>
       <c r="L15">
-        <v>0.6937488280957302</v>
+        <v>0.8507182473580949</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1102,22 +1102,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.7399853698407473</v>
+        <v>-0.7525489793561388</v>
       </c>
       <c r="J16">
-        <v>0.004375235749920733</v>
+        <v>0.004918698145511134</v>
       </c>
       <c r="K16">
-        <v>-0.8670767080511405</v>
+        <v>-0.8788682545029405</v>
       </c>
       <c r="L16">
-        <v>0.001159768265192443</v>
+        <v>0.000811787483996615</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1140,22 +1140,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.3103164454170876</v>
+        <v>-0.1816497536376887</v>
       </c>
       <c r="J17">
-        <v>0.2320634889020341</v>
+        <v>0.4972433060612282</v>
       </c>
       <c r="K17">
-        <v>-0.4149581388530457</v>
+        <v>-0.260405408741612</v>
       </c>
       <c r="L17">
-        <v>0.233093730241445</v>
+        <v>0.4674445466605421</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1178,22 +1178,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.4535394202249742</v>
+        <v>0.4411494016915297</v>
       </c>
       <c r="J18">
-        <v>0.08070214265077501</v>
+        <v>0.09923045565594253</v>
       </c>
       <c r="K18">
-        <v>0.5635998602332413</v>
+        <v>0.5143006822646836</v>
       </c>
       <c r="L18">
-        <v>0.08974939558201678</v>
+        <v>0.1282920587230653</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1216,22 +1216,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.4828045495852675</v>
+        <v>0.4198911048651824</v>
       </c>
       <c r="J19">
-        <v>0.06499039472076076</v>
+        <v>0.1194709867717007</v>
       </c>
       <c r="K19">
-        <v>0.5932707052178214</v>
+        <v>0.5060713596393749</v>
       </c>
       <c r="L19">
-        <v>0.0706202179291523</v>
+        <v>0.1355782583455031</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1254,22 +1254,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.3580574370197164</v>
+        <v>-0.3892494720807615</v>
       </c>
       <c r="J20">
-        <v>0.1679207532945924</v>
+        <v>0.1457680056362324</v>
       </c>
       <c r="K20">
-        <v>-0.4954724046006516</v>
+        <v>-0.5077905470461433</v>
       </c>
       <c r="L20">
-        <v>0.1453294522910624</v>
+        <v>0.1340355823255553</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1292,22 +1292,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.4535394202249742</v>
+        <v>-0.3373495424699933</v>
       </c>
       <c r="J21">
-        <v>0.08070214265077501</v>
+        <v>0.2074202127647988</v>
       </c>
       <c r="K21">
-        <v>-0.6007602905782901</v>
+        <v>-0.4687297357349016</v>
       </c>
       <c r="L21">
-        <v>0.06625295074379814</v>
+        <v>0.1717865787289185</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1330,22 +1330,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.1193524790065721</v>
+        <v>0.0778498944161523</v>
       </c>
       <c r="J22">
-        <v>0.6457756768370824</v>
+        <v>0.7711058640185235</v>
       </c>
       <c r="K22">
-        <v>0.1486417213801955</v>
+        <v>0.09765202827810447</v>
       </c>
       <c r="L22">
-        <v>0.6819355638686473</v>
+        <v>0.788411563708648</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1368,22 +1368,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.167093470609201</v>
+        <v>0.1297498240269205</v>
       </c>
       <c r="J23">
-        <v>0.5199036173455835</v>
+        <v>0.6277606629910362</v>
       </c>
       <c r="K23">
-        <v>0.2725098225303584</v>
+        <v>0.2083243269932896</v>
       </c>
       <c r="L23">
-        <v>0.446215643690079</v>
+        <v>0.5635582121900502</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1406,22 +1406,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.3580574370197164</v>
+        <v>-0.2335496832484569</v>
       </c>
       <c r="J24">
-        <v>0.1679207532945924</v>
+        <v>0.3827797056047885</v>
       </c>
       <c r="K24">
-        <v>-0.4706987843706191</v>
+        <v>-0.3320168961455552</v>
       </c>
       <c r="L24">
-        <v>0.1697475039817557</v>
+        <v>0.3486190102393061</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1914,25 +1914,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2289041597670328</v>
+        <v>-0.2419880147043038</v>
       </c>
       <c r="J9">
-        <v>0.004154062204876697</v>
+        <v>0.002471409738675847</v>
       </c>
       <c r="K9">
-        <v>-0.2872671746617843</v>
+        <v>-0.303489343721962</v>
       </c>
       <c r="L9">
-        <v>0.003756720549751365</v>
+        <v>0.002144343888314521</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2008,7 +2008,7 @@
         <v>-0.3916527812158478</v>
       </c>
       <c r="L11">
-        <v>0.004913052567611288</v>
+        <v>0.00491305256761129</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3251,7 +3251,7 @@
         <v>-0.2860387767736777</v>
       </c>
       <c r="L14">
-        <v>0.4230203924441358</v>
+        <v>0.4230203924441357</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3848,7 +3848,7 @@
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4088,25 +4088,13 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>100</v>
-      </c>
-      <c r="I9">
-        <v>-0.1325530043077417</v>
-      </c>
-      <c r="J9">
-        <v>0.1086826442074059</v>
-      </c>
-      <c r="K9">
-        <v>-0.1612223880273475</v>
-      </c>
-      <c r="L9">
-        <v>0.1090548020620709</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4126,25 +4114,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.1454025530693833</v>
+        <v>0.01421997815784012</v>
       </c>
       <c r="J10">
-        <v>0.2372373518450496</v>
+        <v>0.9088173646349219</v>
       </c>
       <c r="K10">
-        <v>-0.17271903862684</v>
+        <v>0.01636148293791983</v>
       </c>
       <c r="L10">
-        <v>0.2303502122764337</v>
+        <v>0.9102093962355748</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4164,25 +4152,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.1395616700784287</v>
+        <v>0.001918117792161453</v>
       </c>
       <c r="J11">
-        <v>0.2348980869048207</v>
+        <v>0.9870933347767511</v>
       </c>
       <c r="K11">
-        <v>-0.1674579385094694</v>
+        <v>0.002310973073108823</v>
       </c>
       <c r="L11">
-        <v>0.2450782275649824</v>
+        <v>0.9872920353883015</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4202,25 +4190,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.02140819589682411</v>
+        <v>0.2419047619047619</v>
       </c>
       <c r="J12">
-        <v>0.8544862615484419</v>
+        <v>0.04002718189621234</v>
       </c>
       <c r="K12">
-        <v>0.02708713119452734</v>
+        <v>0.2933526131391836</v>
       </c>
       <c r="L12">
-        <v>0.8518765230635053</v>
+        <v>0.03867934687031337</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4240,25 +4228,13 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>10</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -4278,25 +4254,13 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>10</v>
-      </c>
-      <c r="I14">
-        <v>0.6085806194501846</v>
-      </c>
-      <c r="J14">
-        <v>0.03300625766123251</v>
-      </c>
-      <c r="K14">
-        <v>0.7106690545187014</v>
-      </c>
-      <c r="L14">
-        <v>0.02124449212877441</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4316,25 +4280,13 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>10</v>
-      </c>
-      <c r="I15">
-        <v>0.6770032003863301</v>
-      </c>
-      <c r="J15">
-        <v>0.01865536081150319</v>
-      </c>
-      <c r="K15">
-        <v>0.7841156792042765</v>
-      </c>
-      <c r="L15">
-        <v>0.007255789526699558</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4354,25 +4306,13 @@
         <v>10</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>10</v>
-      </c>
-      <c r="I16">
-        <v>-0.1217161238900369</v>
-      </c>
-      <c r="J16">
-        <v>0.6698153575994166</v>
-      </c>
-      <c r="K16">
-        <v>-0.1421338109037403</v>
-      </c>
-      <c r="L16">
-        <v>0.6952876854012655</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -4392,25 +4332,13 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>10</v>
-      </c>
-      <c r="I17">
-        <v>-0.3042903097250923</v>
-      </c>
-      <c r="J17">
-        <v>0.2864220227778588</v>
-      </c>
-      <c r="K17">
-        <v>-0.3553345272593507</v>
-      </c>
-      <c r="L17">
-        <v>0.3136373640754537</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -4430,25 +4358,13 @@
         <v>10</v>
       </c>
       <c r="F18">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>10</v>
-      </c>
-      <c r="I18">
-        <v>0.06085806194501846</v>
-      </c>
-      <c r="J18">
-        <v>0.8311704095417624</v>
-      </c>
-      <c r="K18">
-        <v>0.07106690545187015</v>
-      </c>
-      <c r="L18">
-        <v>0.8453239136912953</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -4468,25 +4384,13 @@
         <v>10</v>
       </c>
       <c r="F19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>10</v>
-      </c>
-      <c r="I19">
-        <v>0.09231861823449956</v>
-      </c>
-      <c r="J19">
-        <v>0.7483812122920345</v>
-      </c>
-      <c r="K19">
-        <v>0.1069248653460377</v>
-      </c>
-      <c r="L19">
-        <v>0.7687577033932652</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -4506,25 +4410,13 @@
         <v>10</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>10</v>
-      </c>
-      <c r="I20">
-        <v>-0.06085806194501846</v>
-      </c>
-      <c r="J20">
-        <v>0.8311704095417624</v>
-      </c>
-      <c r="K20">
-        <v>-0.07106690545187015</v>
-      </c>
-      <c r="L20">
-        <v>0.8453239136912953</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -4544,25 +4436,13 @@
         <v>10</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>10</v>
-      </c>
-      <c r="I21">
-        <v>-0.2434322477800739</v>
-      </c>
-      <c r="J21">
-        <v>0.3937686346429927</v>
-      </c>
-      <c r="K21">
-        <v>-0.2842676218074806</v>
-      </c>
-      <c r="L21">
-        <v>0.4260244484285426</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -4582,25 +4462,13 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <v>10</v>
-      </c>
-      <c r="I22">
-        <v>0.1217161238900369</v>
-      </c>
-      <c r="J22">
-        <v>0.6698153575994166</v>
-      </c>
-      <c r="K22">
-        <v>0.1421338109037403</v>
-      </c>
-      <c r="L22">
-        <v>0.6952876854012655</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -4620,25 +4488,13 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>10</v>
-      </c>
-      <c r="I23">
-        <v>0.2434322477800739</v>
-      </c>
-      <c r="J23">
-        <v>0.3937686346429927</v>
-      </c>
-      <c r="K23">
-        <v>0.2842676218074806</v>
-      </c>
-      <c r="L23">
-        <v>0.4260244484285426</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -4658,25 +4514,13 @@
         <v>10</v>
       </c>
       <c r="F24">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>10</v>
-      </c>
-      <c r="I24">
-        <v>-0.2434322477800739</v>
-      </c>
-      <c r="J24">
-        <v>0.3937686346429927</v>
-      </c>
-      <c r="K24">
-        <v>-0.2842676218074806</v>
-      </c>
-      <c r="L24">
-        <v>0.4260244484285426</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5159,7 +5003,7 @@
         <v>-0.5561107852980067</v>
       </c>
       <c r="L7">
-        <v>0.06043495620092659</v>
+        <v>0.0604349562009266</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5273,7 +5117,7 @@
         <v>-0.2757884146130811</v>
       </c>
       <c r="L10">
-        <v>0.0525532974249969</v>
+        <v>0.05255329742499692</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5311,7 +5155,7 @@
         <v>-0.2382169979796553</v>
       </c>
       <c r="L11">
-        <v>0.09572883636182701</v>
+        <v>0.095728836361827</v>
       </c>
     </row>
     <row r="12" spans="1:12">

</xml_diff>

<commit_message>
Generated all data again
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -699,7 +699,7 @@
         <v>-0.3178304128441319</v>
       </c>
       <c r="L5">
-        <v>0.3140610795011265</v>
+        <v>0.3140610795011266</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -836,22 +836,22 @@
         <v>92</v>
       </c>
       <c r="G9">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2232481170885827</v>
+        <v>-0.2138929578962992</v>
       </c>
       <c r="J9">
-        <v>0.001636069376151588</v>
+        <v>0.002549332151279517</v>
       </c>
       <c r="K9">
-        <v>-0.3234519555354279</v>
+        <v>-0.3104211061218942</v>
       </c>
       <c r="L9">
-        <v>0.001028681640569814</v>
+        <v>0.001671025456360345</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1444,22 +1444,22 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1807753815155468</v>
+        <v>-0.2089183206099184</v>
       </c>
       <c r="J25">
-        <v>0.3541954904764164</v>
+        <v>0.2858071051160878</v>
       </c>
       <c r="K25">
-        <v>-0.2576049186596542</v>
+        <v>-0.2761088800464458</v>
       </c>
       <c r="L25">
-        <v>0.3354345184285685</v>
+        <v>0.3006008438154604</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1482,22 +1482,22 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1807753815155468</v>
+        <v>-0.1907515101220994</v>
       </c>
       <c r="J26">
-        <v>0.3541954904764164</v>
+        <v>0.3297832606788835</v>
       </c>
       <c r="K26">
-        <v>-0.2666436877354316</v>
+        <v>-0.2791264634349316</v>
       </c>
       <c r="L26">
-        <v>0.3181414648703181</v>
+        <v>0.2951316609645892</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1520,22 +1520,22 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3539900381483285</v>
+        <v>0.3648596387010686</v>
       </c>
       <c r="J27">
-        <v>0.07056136851892029</v>
+        <v>0.06317307481323101</v>
       </c>
       <c r="K27">
-        <v>0.4341802833034056</v>
+        <v>0.4446662347157511</v>
       </c>
       <c r="L27">
-        <v>0.09288178063084394</v>
+        <v>0.08439298705280707</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1558,22 +1558,22 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H28">
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.1647705109143269</v>
+        <v>-0.1563850753205831</v>
       </c>
       <c r="J28">
-        <v>0.4027546538976249</v>
+        <v>0.4285752941987943</v>
       </c>
       <c r="K28">
-        <v>-0.2493004677260264</v>
+        <v>-0.2133681077431026</v>
       </c>
       <c r="L28">
-        <v>0.3517858440384553</v>
+        <v>0.4275202599269713</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1596,22 +1596,22 @@
         <v>15</v>
       </c>
       <c r="G29">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H29">
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.1265427670608828</v>
+        <v>-0.1725846996342804</v>
       </c>
       <c r="J29">
-        <v>0.5166373798159882</v>
+        <v>0.377919481405675</v>
       </c>
       <c r="K29">
-        <v>-0.1491396897503261</v>
+        <v>-0.1931253368630878</v>
       </c>
       <c r="L29">
-        <v>0.5814513259975999</v>
+        <v>0.4736035833560223</v>
       </c>
     </row>
   </sheetData>
@@ -1914,25 +1914,25 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2419880147043038</v>
+        <v>-0.2260489959509954</v>
       </c>
       <c r="J9">
-        <v>0.002471409738675847</v>
+        <v>0.004741931174898608</v>
       </c>
       <c r="K9">
-        <v>-0.303489343721962</v>
+        <v>-0.2832375756589699</v>
       </c>
       <c r="L9">
-        <v>0.002144343888314521</v>
+        <v>0.004297109542258244</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2008,7 +2008,7 @@
         <v>-0.3916527812158478</v>
       </c>
       <c r="L11">
-        <v>0.00491305256761129</v>
+        <v>0.004913052567611288</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3046,22 +3046,22 @@
         <v>88</v>
       </c>
       <c r="G9">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459341</v>
+        <v>-0.1509654696395568</v>
       </c>
       <c r="J9">
-        <v>0.0301286154880051</v>
+        <v>0.03611918064522761</v>
       </c>
       <c r="K9">
-        <v>-0.2203331090972887</v>
+        <v>-0.2132165514106953</v>
       </c>
       <c r="L9">
-        <v>0.0276105659239954</v>
+        <v>0.0331785702669911</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3251,7 +3251,7 @@
         <v>-0.2860387767736777</v>
       </c>
       <c r="L14">
-        <v>0.4230203924441357</v>
+        <v>0.4230203924441358</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4208,7 +4208,7 @@
         <v>0.2933526131391836</v>
       </c>
       <c r="L12">
-        <v>0.03867934687031337</v>
+        <v>0.03867934687031339</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5003,7 +5003,7 @@
         <v>-0.5561107852980067</v>
       </c>
       <c r="L7">
-        <v>0.0604349562009266</v>
+        <v>0.06043495620092659</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5117,7 +5117,7 @@
         <v>-0.2757884146130811</v>
       </c>
       <c r="L10">
-        <v>0.05255329742499692</v>
+        <v>0.0525532974249969</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5155,7 +5155,7 @@
         <v>-0.2382169979796553</v>
       </c>
       <c r="L11">
-        <v>0.095728836361827</v>
+        <v>0.09572883636182701</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5669,25 +5669,25 @@
         <v>16</v>
       </c>
       <c r="F25">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G25">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.31352722326441</v>
+        <v>-0.3244079990200284</v>
       </c>
       <c r="J25">
-        <v>0.1131685336545776</v>
+        <v>0.1020809611324846</v>
       </c>
       <c r="K25">
-        <v>-0.4479914656638877</v>
+        <v>-0.4824165900576836</v>
       </c>
       <c r="L25">
-        <v>0.08182143505121871</v>
+        <v>0.05842088299110668</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -5707,25 +5707,25 @@
         <v>16</v>
       </c>
       <c r="F26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.3872983346207417</v>
+        <v>-0.4170959987400364</v>
       </c>
       <c r="J26">
-        <v>0.05036597579032801</v>
+        <v>0.03555790569992093</v>
       </c>
       <c r="K26">
-        <v>-0.5070173682344674</v>
+        <v>-0.5355127556300702</v>
       </c>
       <c r="L26">
-        <v>0.04501930875693567</v>
+        <v>0.03253137976639191</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -5745,25 +5745,25 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.08334047874242113</v>
+        <v>0.2047685867790963</v>
       </c>
       <c r="J27">
-        <v>0.6747078413451294</v>
+        <v>0.3037024766857317</v>
       </c>
       <c r="K27">
-        <v>0.08027373462987823</v>
+        <v>0.2170954499333818</v>
       </c>
       <c r="L27">
-        <v>0.7675926515511813</v>
+        <v>0.4192967698838219</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -5783,25 +5783,25 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G28">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H28">
         <v>16</v>
       </c>
       <c r="I28">
-        <v>0.09338863578008762</v>
+        <v>0.08448190755542286</v>
       </c>
       <c r="J28">
-        <v>0.6401498414586226</v>
+        <v>0.6731676659685988</v>
       </c>
       <c r="K28">
-        <v>0.1305442024324843</v>
+        <v>0.1201996807657877</v>
       </c>
       <c r="L28">
-        <v>0.6298840619248964</v>
+        <v>0.6574684200274921</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -5821,25 +5821,25 @@
         <v>16</v>
       </c>
       <c r="F29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G29">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H29">
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.1290994448735805</v>
+        <v>0.009268799972000809</v>
       </c>
       <c r="J29">
-        <v>0.5142199988155506</v>
+        <v>0.9627444106905073</v>
       </c>
       <c r="K29">
-        <v>0.1619428608987702</v>
+        <v>0.01365329971861369</v>
       </c>
       <c r="L29">
-        <v>0.5490376092324329</v>
+        <v>0.9599750222894384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated all data from last main commit
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -506,10 +506,10 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -699,7 +699,7 @@
         <v>-0.3178304128441319</v>
       </c>
       <c r="L5">
-        <v>0.3140610795011265</v>
+        <v>0.3140610795011266</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -874,22 +874,22 @@
         <v>46</v>
       </c>
       <c r="G10">
-        <v>794</v>
+        <v>767</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.05768310136706124</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0.5808166089173682</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>-0.06873895440322977</v>
+        <v>0.01048869174464198</v>
       </c>
       <c r="L10">
-        <v>0.635267646345926</v>
+        <v>0.9423692820963127</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -912,22 +912,22 @@
         <v>46</v>
       </c>
       <c r="G11">
-        <v>794</v>
+        <v>767</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.03854494781179903</v>
+        <v>0.01087930486403344</v>
       </c>
       <c r="J11">
-        <v>0.6995394491817443</v>
+        <v>0.9131676455849755</v>
       </c>
       <c r="K11">
-        <v>-0.04832503745113209</v>
+        <v>0.0205721853235722</v>
       </c>
       <c r="L11">
-        <v>0.7389368221688255</v>
+        <v>0.8872356454282179</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -950,22 +950,22 @@
         <v>46</v>
       </c>
       <c r="G12">
-        <v>794</v>
+        <v>767</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1156617751198898</v>
+        <v>0.1529118139971709</v>
       </c>
       <c r="J12">
-        <v>0.2438312496350385</v>
+        <v>0.1229781371552088</v>
       </c>
       <c r="K12">
-        <v>0.1718948469712283</v>
+        <v>0.2338571315807966</v>
       </c>
       <c r="L12">
-        <v>0.2326162766495191</v>
+        <v>0.1021436762030583</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -988,22 +988,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.3373495424699933</v>
+        <v>-0.5284193913361779</v>
       </c>
       <c r="J13">
-        <v>0.2074202127647988</v>
+        <v>0.05682819683984795</v>
       </c>
       <c r="K13">
-        <v>-0.4296689244236597</v>
+        <v>-0.6292532049656926</v>
       </c>
       <c r="L13">
-        <v>0.215243543278886</v>
+        <v>0.05126402824042627</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1026,22 +1026,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.1816497536376887</v>
+        <v>-0.4662524041201569</v>
       </c>
       <c r="J14">
-        <v>0.4972433060612282</v>
+        <v>0.09284922807157968</v>
       </c>
       <c r="K14">
-        <v>-0.2669155439601523</v>
+        <v>-0.5618332187193684</v>
       </c>
       <c r="L14">
-        <v>0.4559719917038285</v>
+        <v>0.090982576216914</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1064,22 +1064,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.0524863881081478</v>
+        <v>-0.3143473067309657</v>
       </c>
       <c r="J15">
-        <v>0.8456867367859529</v>
+        <v>0.2610207247026572</v>
       </c>
       <c r="K15">
-        <v>-0.06856450678985078</v>
+        <v>-0.3719387243003159</v>
       </c>
       <c r="L15">
-        <v>0.8507182473580949</v>
+        <v>0.2899037448075479</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1102,22 +1102,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.7525489793561388</v>
+        <v>-0.5905863785521988</v>
       </c>
       <c r="J16">
-        <v>0.004918698145511134</v>
+        <v>0.03327875704510121</v>
       </c>
       <c r="K16">
-        <v>-0.8788682545029405</v>
+        <v>-0.6741998624632421</v>
       </c>
       <c r="L16">
-        <v>0.000811787483996615</v>
+        <v>0.03251559932021606</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1140,22 +1140,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1816497536376887</v>
+        <v>0.03108349360801046</v>
       </c>
       <c r="J17">
-        <v>0.4972433060612282</v>
+        <v>0.9107940274245708</v>
       </c>
       <c r="K17">
-        <v>-0.260405408741612</v>
+        <v>0.02247332874877474</v>
       </c>
       <c r="L17">
-        <v>0.4674445466605421</v>
+        <v>0.9508644143273767</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1178,22 +1178,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.4411494016915297</v>
+        <v>0.404085416904136</v>
       </c>
       <c r="J18">
-        <v>0.09923045565594253</v>
+        <v>0.1452595077432854</v>
       </c>
       <c r="K18">
-        <v>0.5143006822646836</v>
+        <v>0.4944132324730443</v>
       </c>
       <c r="L18">
-        <v>0.1282920587230653</v>
+        <v>0.1463267160789159</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1216,22 +1216,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.4198911048651824</v>
+        <v>0.4400862294233521</v>
       </c>
       <c r="J19">
-        <v>0.1194709867717007</v>
+        <v>0.1155858306979473</v>
       </c>
       <c r="K19">
-        <v>0.5060713596393749</v>
+        <v>0.5297309103671165</v>
       </c>
       <c r="L19">
-        <v>0.1355782583455031</v>
+        <v>0.1152952650343875</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1254,22 +1254,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.3892494720807615</v>
+        <v>-0.404085416904136</v>
       </c>
       <c r="J20">
-        <v>0.1457680056362324</v>
+        <v>0.1452595077432854</v>
       </c>
       <c r="K20">
-        <v>-0.5077905470461433</v>
+        <v>-0.4494665749754947</v>
       </c>
       <c r="L20">
-        <v>0.1340355823255553</v>
+        <v>0.1925017251163437</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1292,22 +1292,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.3373495424699933</v>
+        <v>-0.2175844552560732</v>
       </c>
       <c r="J21">
-        <v>0.2074202127647988</v>
+        <v>0.4328879340133424</v>
       </c>
       <c r="K21">
-        <v>-0.4687297357349016</v>
+        <v>-0.3146266024828463</v>
       </c>
       <c r="L21">
-        <v>0.1717865787289185</v>
+        <v>0.3759325783116143</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1330,22 +1330,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.0778498944161523</v>
+        <v>-0.2175844552560732</v>
       </c>
       <c r="J22">
-        <v>0.7711058640185235</v>
+        <v>0.4328879340133424</v>
       </c>
       <c r="K22">
-        <v>0.09765202827810447</v>
+        <v>-0.2696799449852968</v>
       </c>
       <c r="L22">
-        <v>0.788411563708648</v>
+        <v>0.4511390079856625</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1368,22 +1368,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.1297498240269205</v>
+        <v>-0.1554174680400523</v>
       </c>
       <c r="J23">
-        <v>0.6277606629910362</v>
+        <v>0.5753530764008791</v>
       </c>
       <c r="K23">
-        <v>0.2083243269932896</v>
+        <v>-0.1573133012414231</v>
       </c>
       <c r="L23">
-        <v>0.5635582121900502</v>
+        <v>0.6642676178335104</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1406,22 +1406,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2335496832484569</v>
+        <v>-0.03108349360801046</v>
       </c>
       <c r="J24">
-        <v>0.3827797056047885</v>
+        <v>0.9107940274245708</v>
       </c>
       <c r="K24">
-        <v>-0.3320168961455552</v>
+        <v>-0.04494665749754947</v>
       </c>
       <c r="L24">
-        <v>0.3486190102393061</v>
+        <v>0.9018775739844269</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1444,22 +1444,22 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1807753815155468</v>
+        <v>-0.2089183206099184</v>
       </c>
       <c r="J25">
-        <v>0.3541954904764164</v>
+        <v>0.2858071051160878</v>
       </c>
       <c r="K25">
-        <v>-0.2576049186596542</v>
+        <v>-0.2761088800464458</v>
       </c>
       <c r="L25">
-        <v>0.3354345184285685</v>
+        <v>0.3006008438154604</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1482,22 +1482,22 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1807753815155468</v>
+        <v>-0.1907515101220994</v>
       </c>
       <c r="J26">
-        <v>0.3541954904764164</v>
+        <v>0.3297832606788835</v>
       </c>
       <c r="K26">
-        <v>-0.2666436877354316</v>
+        <v>-0.2791264634349316</v>
       </c>
       <c r="L26">
-        <v>0.3181414648703181</v>
+        <v>0.2951316609645892</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1520,22 +1520,22 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3539900381483285</v>
+        <v>0.3648596387010686</v>
       </c>
       <c r="J27">
-        <v>0.07056136851892029</v>
+        <v>0.06317307481323101</v>
       </c>
       <c r="K27">
-        <v>0.4341802833034056</v>
+        <v>0.4446662347157511</v>
       </c>
       <c r="L27">
-        <v>0.09288178063084394</v>
+        <v>0.08439298705280707</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1558,22 +1558,22 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H28">
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.1647705109143269</v>
+        <v>-0.1563850753205831</v>
       </c>
       <c r="J28">
-        <v>0.4027546538976249</v>
+        <v>0.4285752941987943</v>
       </c>
       <c r="K28">
-        <v>-0.2493004677260264</v>
+        <v>-0.2133681077431026</v>
       </c>
       <c r="L28">
-        <v>0.3517858440384553</v>
+        <v>0.4275202599269713</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1596,22 +1596,22 @@
         <v>15</v>
       </c>
       <c r="G29">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H29">
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.1265427670608828</v>
+        <v>-0.1725846996342804</v>
       </c>
       <c r="J29">
-        <v>0.5166373798159882</v>
+        <v>0.377919481405675</v>
       </c>
       <c r="K29">
-        <v>-0.1491396897503261</v>
+        <v>-0.1931253368630878</v>
       </c>
       <c r="L29">
-        <v>0.5814513259975999</v>
+        <v>0.4736035833560223</v>
       </c>
     </row>
   </sheetData>
@@ -1952,25 +1952,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.2741939043543897</v>
+        <v>-0.1719856383383667</v>
       </c>
       <c r="J10">
-        <v>0.01523742906785629</v>
+        <v>0.1316238040142544</v>
       </c>
       <c r="K10">
-        <v>-0.3438060590640694</v>
+        <v>-0.2170916607282444</v>
       </c>
       <c r="L10">
-        <v>0.0145005762354219</v>
+        <v>0.1299324388039652</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1990,25 +1990,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.2885159533670518</v>
+        <v>-0.2220671589132321</v>
       </c>
       <c r="J11">
-        <v>0.007534224862278689</v>
+        <v>0.0416011054294208</v>
       </c>
       <c r="K11">
-        <v>-0.3916527812158478</v>
+        <v>-0.3044028033210576</v>
       </c>
       <c r="L11">
-        <v>0.00491305256761129</v>
+        <v>0.03161022555609473</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2028,25 +2028,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1527404930393114</v>
+        <v>0.2554933792020658</v>
       </c>
       <c r="J12">
-        <v>0.1545006958890939</v>
+        <v>0.01830915752272128</v>
       </c>
       <c r="K12">
-        <v>0.1874148805812322</v>
+        <v>0.3206647291565351</v>
       </c>
       <c r="L12">
-        <v>0.192476549579598</v>
+        <v>0.02318249883445114</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2066,25 +2066,25 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.3651483716701108</v>
+        <v>0.07453559924999299</v>
       </c>
       <c r="J13">
-        <v>0.2008251226951454</v>
+        <v>0.794002680192762</v>
       </c>
       <c r="K13">
-        <v>0.4264014327112208</v>
+        <v>0.08703882797784893</v>
       </c>
       <c r="L13">
-        <v>0.2191383605228726</v>
+        <v>0.8110384240587123</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2104,25 +2104,25 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>0.7302967433402215</v>
+        <v>0.3726779962499649</v>
       </c>
       <c r="J14">
-        <v>0.01051524593585891</v>
+        <v>0.191694602051888</v>
       </c>
       <c r="K14">
-        <v>0.8528028654224417</v>
+        <v>0.4351941398892446</v>
       </c>
       <c r="L14">
-        <v>0.001712874149321468</v>
+        <v>0.2087486300875882</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2142,25 +2142,25 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.7385489458759965</v>
+        <v>0.3768891807222045</v>
       </c>
       <c r="J15">
-        <v>0.01028204822194895</v>
+        <v>0.1903458092612167</v>
       </c>
       <c r="K15">
-        <v>0.8553989227683017</v>
+        <v>0.4365189348559864</v>
       </c>
       <c r="L15">
-        <v>0.001600453316805279</v>
+        <v>0.2072083540976897</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2180,25 +2180,25 @@
         <v>10</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.1217161238900369</v>
+        <v>0.149071198499986</v>
       </c>
       <c r="J16">
-        <v>0.6698153575994166</v>
+        <v>0.6015081344405899</v>
       </c>
       <c r="K16">
-        <v>-0.1421338109037403</v>
+        <v>0.1740776559556979</v>
       </c>
       <c r="L16">
-        <v>0.6952876854012655</v>
+        <v>0.6305360755569764</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2218,25 +2218,25 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.5477225575051662</v>
+        <v>-0.223606797749979</v>
       </c>
       <c r="J17">
-        <v>0.05500883362926572</v>
+        <v>0.4334219309560737</v>
       </c>
       <c r="K17">
-        <v>-0.6396021490668313</v>
+        <v>-0.2611164839335468</v>
       </c>
       <c r="L17">
-        <v>0.04643461767158175</v>
+        <v>0.4661852835040308</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2256,25 +2256,25 @@
         <v>10</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.3651483716701108</v>
+        <v>-0.4472135954999579</v>
       </c>
       <c r="J18">
-        <v>0.2008251226951454</v>
+        <v>0.117185087198138</v>
       </c>
       <c r="K18">
-        <v>-0.4264014327112208</v>
+        <v>-0.5222329678670935</v>
       </c>
       <c r="L18">
-        <v>0.2191383605228726</v>
+        <v>0.1215029188171132</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2294,25 +2294,25 @@
         <v>10</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>-0.3077287274483319</v>
+        <v>-0.3015113445777636</v>
       </c>
       <c r="J19">
-        <v>0.2849576406684299</v>
+        <v>0.2948019919337048</v>
       </c>
       <c r="K19">
-        <v>-0.3564162178201257</v>
+        <v>-0.3492151478847891</v>
       </c>
       <c r="L19">
-        <v>0.312061132326838</v>
+        <v>0.3226327672991101</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2332,25 +2332,25 @@
         <v>10</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>0.3042903097250923</v>
+        <v>0.4472135954999579</v>
       </c>
       <c r="J20">
-        <v>0.2864220227778588</v>
+        <v>0.117185087198138</v>
       </c>
       <c r="K20">
-        <v>0.3553345272593507</v>
+        <v>0.5222329678670935</v>
       </c>
       <c r="L20">
-        <v>0.3136373640754537</v>
+        <v>0.1215029188171132</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2370,25 +2370,25 @@
         <v>10</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.3651483716701108</v>
+        <v>-0.223606797749979</v>
       </c>
       <c r="J21">
-        <v>0.2008251226951454</v>
+        <v>0.4334219309560737</v>
       </c>
       <c r="K21">
-        <v>-0.4264014327112208</v>
+        <v>-0.2611164839335468</v>
       </c>
       <c r="L21">
-        <v>0.2191383605228726</v>
+        <v>0.4661852835040308</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2408,25 +2408,25 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.3042903097250923</v>
+        <v>-0.223606797749979</v>
       </c>
       <c r="J22">
-        <v>0.2864220227778588</v>
+        <v>0.4334219309560737</v>
       </c>
       <c r="K22">
-        <v>0.3553345272593507</v>
+        <v>-0.2611164839335468</v>
       </c>
       <c r="L22">
-        <v>0.3136373640754537</v>
+        <v>0.4661852835040308</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2446,25 +2446,25 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.3651483716701108</v>
+        <v>-0.149071198499986</v>
       </c>
       <c r="J23">
-        <v>0.2008251226951454</v>
+        <v>0.6015081344405899</v>
       </c>
       <c r="K23">
-        <v>0.4264014327112208</v>
+        <v>-0.1740776559556979</v>
       </c>
       <c r="L23">
-        <v>0.2191383605228726</v>
+        <v>0.6305360755569764</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2484,25 +2484,25 @@
         <v>10</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.4260064336151292</v>
+        <v>-0.07453559924999299</v>
       </c>
       <c r="J24">
-        <v>0.1355930012663022</v>
+        <v>0.794002680192762</v>
       </c>
       <c r="K24">
-        <v>-0.497468338163091</v>
+        <v>-0.08703882797784893</v>
       </c>
       <c r="L24">
-        <v>0.1434614655950857</v>
+        <v>0.8110384240587123</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2716,9 +2716,9 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3084,22 +3084,22 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>0.03324642499485375</v>
+        <v>0.08712167584961492</v>
       </c>
       <c r="J10">
-        <v>0.7524695495544889</v>
+        <v>0.4083766752312095</v>
       </c>
       <c r="K10">
-        <v>0.05369692827151148</v>
+        <v>0.1227687641955272</v>
       </c>
       <c r="L10">
-        <v>0.7111154281850389</v>
+        <v>0.3956759834281137</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3122,22 +3122,22 @@
         <v>40</v>
       </c>
       <c r="G11">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>0.02630142666529713</v>
+        <v>0.07462967377124524</v>
       </c>
       <c r="J11">
-        <v>0.7941029996140164</v>
+        <v>0.4588124610579571</v>
       </c>
       <c r="K11">
-        <v>0.0345247475921612</v>
+        <v>0.09255821810809323</v>
       </c>
       <c r="L11">
-        <v>0.8118632018166435</v>
+        <v>0.5226237277667096</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3160,22 +3160,22 @@
         <v>40</v>
       </c>
       <c r="G12">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.02696081483975262</v>
+        <v>0.0648462728029752</v>
       </c>
       <c r="J12">
-        <v>0.7877495099042957</v>
+        <v>0.5171200381290717</v>
       </c>
       <c r="K12">
-        <v>0.03904490288887924</v>
+        <v>0.08638478532010939</v>
       </c>
       <c r="L12">
-        <v>0.7877690834629696</v>
+        <v>0.5508414269428876</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3198,22 +3198,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4787549991450212</v>
+        <v>-0.6366820122120065</v>
       </c>
       <c r="J13">
-        <v>0.07217560549492458</v>
+        <v>0.01869720062275651</v>
       </c>
       <c r="K13">
-        <v>-0.6292853089020909</v>
+        <v>-0.8019532181238483</v>
       </c>
       <c r="L13">
-        <v>0.05124855216842294</v>
+        <v>0.005259237421010194</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3236,22 +3236,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.2267786838055363</v>
+        <v>-0.4705910525045265</v>
       </c>
       <c r="J14">
-        <v>0.3943870594034554</v>
+        <v>0.08219753762575091</v>
       </c>
       <c r="K14">
-        <v>-0.2860387767736777</v>
+        <v>-0.5414897797588377</v>
       </c>
       <c r="L14">
-        <v>0.4230203924441357</v>
+        <v>0.1059666504898876</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3274,22 +3274,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.1019294382875251</v>
+        <v>-0.3359355065735126</v>
       </c>
       <c r="J15">
-        <v>0.7040542681897126</v>
+        <v>0.218311625181403</v>
       </c>
       <c r="K15">
-        <v>-0.0765092055676006</v>
+        <v>-0.3506334920077187</v>
       </c>
       <c r="L15">
-        <v>0.8336123677972922</v>
+        <v>0.3205360031284263</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3312,22 +3312,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.579545525280815</v>
+        <v>-0.3598637460328732</v>
       </c>
       <c r="J16">
-        <v>0.02951512807757192</v>
+        <v>0.1838095557893692</v>
       </c>
       <c r="K16">
-        <v>-0.7119187333033755</v>
+        <v>-0.4592381676435712</v>
       </c>
       <c r="L16">
-        <v>0.02091481468718881</v>
+        <v>0.1818195500051732</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3350,22 +3350,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1259881576697424</v>
+        <v>0.08304547985373997</v>
       </c>
       <c r="J17">
-        <v>0.6360988735986226</v>
+        <v>0.7590571299004958</v>
       </c>
       <c r="K17">
-        <v>-0.1906925178491184</v>
+        <v>0.08910591312487204</v>
       </c>
       <c r="L17">
-        <v>0.5977007516614028</v>
+        <v>0.8066210879575378</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3388,22 +3388,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.579545525280815</v>
+        <v>0.5259547057403532</v>
       </c>
       <c r="J18">
-        <v>0.02951512807757192</v>
+        <v>0.05206997227535645</v>
       </c>
       <c r="K18">
-        <v>0.7437008196115621</v>
+        <v>0.7128473049989763</v>
       </c>
       <c r="L18">
-        <v>0.01366958411527145</v>
+        <v>0.02067214786469852</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -3426,22 +3426,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.560611910581388</v>
+        <v>0.5598925109558542</v>
       </c>
       <c r="J19">
-        <v>0.0366903087793031</v>
+        <v>0.04019719781553128</v>
       </c>
       <c r="K19">
-        <v>0.7172738021962557</v>
+        <v>0.7253300668002809</v>
       </c>
       <c r="L19">
-        <v>0.01954204435368506</v>
+        <v>0.01759621904480188</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3464,22 +3464,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.4787549991450212</v>
+        <v>-0.4705910525045265</v>
       </c>
       <c r="J20">
-        <v>0.07217560549492458</v>
+        <v>0.08219753762575091</v>
       </c>
       <c r="K20">
-        <v>-0.6419981434253655</v>
+        <v>-0.5689069837972599</v>
       </c>
       <c r="L20">
-        <v>0.04536158917864154</v>
+        <v>0.08610936073892451</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3502,22 +3502,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2771739468734333</v>
+        <v>-0.1384091330895666</v>
       </c>
       <c r="J21">
-        <v>0.2978975979923409</v>
+        <v>0.6092119761915052</v>
       </c>
       <c r="K21">
-        <v>-0.3750286184365996</v>
+        <v>-0.1987747292785607</v>
       </c>
       <c r="L21">
-        <v>0.2855969029688312</v>
+        <v>0.5819571528087297</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -3540,22 +3540,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.1259881576697424</v>
+        <v>-0.1384091330895666</v>
       </c>
       <c r="J22">
-        <v>0.6360988735986226</v>
+        <v>0.6092119761915052</v>
       </c>
       <c r="K22">
-        <v>0.1461975970176575</v>
+        <v>-0.1919204282689551</v>
       </c>
       <c r="L22">
-        <v>0.6869410188538527</v>
+        <v>0.595298950736874</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3578,22 +3578,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.1259881576697424</v>
+        <v>-0.1384091330895666</v>
       </c>
       <c r="J23">
-        <v>0.6360988735986226</v>
+        <v>0.6092119761915052</v>
       </c>
       <c r="K23">
-        <v>0.2161181868956676</v>
+        <v>-0.1302317191825053</v>
       </c>
       <c r="L23">
-        <v>0.5487107060733141</v>
+        <v>0.7199008272052645</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3616,22 +3616,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2267786838055363</v>
+        <v>-0.02768182661791332</v>
       </c>
       <c r="J24">
-        <v>0.3943870594034554</v>
+        <v>0.9185663957730847</v>
       </c>
       <c r="K24">
-        <v>-0.3114644458202268</v>
+        <v>-0.02741720403842217</v>
       </c>
       <c r="L24">
-        <v>0.3810089567050594</v>
+        <v>0.9400699293286143</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -4208,7 +4208,7 @@
         <v>0.2933526131391836</v>
       </c>
       <c r="L12">
-        <v>0.03867934687031337</v>
+        <v>0.03867934687031339</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5003,7 +5003,7 @@
         <v>-0.5561107852980067</v>
       </c>
       <c r="L7">
-        <v>0.0604349562009266</v>
+        <v>0.06043495620092659</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5117,7 +5117,7 @@
         <v>-0.2757884146130811</v>
       </c>
       <c r="L10">
-        <v>0.05255329742499692</v>
+        <v>0.0525532974249969</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5155,7 +5155,7 @@
         <v>-0.2382169979796553</v>
       </c>
       <c r="L11">
-        <v>0.095728836361827</v>
+        <v>0.09572883636182701</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5216,22 +5216,22 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.04969039949999533</v>
+        <v>0.05270462766947299</v>
       </c>
       <c r="J13">
-        <v>0.8509806870320558</v>
+        <v>0.8464505968765906</v>
       </c>
       <c r="K13">
-        <v>0.01262892050706804</v>
+        <v>0.0259499648053841</v>
       </c>
       <c r="L13">
-        <v>0.9723786419920799</v>
+        <v>0.9432726625041241</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -5254,22 +5254,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.149071198499986</v>
+        <v>-0.2635231383473649</v>
       </c>
       <c r="J14">
-        <v>0.5730251193553904</v>
+        <v>0.3329216080655659</v>
       </c>
       <c r="K14">
-        <v>-0.1894338076060206</v>
+        <v>-0.3503245248726853</v>
       </c>
       <c r="L14">
-        <v>0.6001664342511973</v>
+        <v>0.3209921486658833</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -5292,22 +5292,22 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.1256297269074015</v>
+        <v>-0.2398508059000617</v>
       </c>
       <c r="J15">
-        <v>0.6374017405958849</v>
+        <v>0.3819327979196356</v>
       </c>
       <c r="K15">
-        <v>-0.152008377581442</v>
+        <v>-0.3448837241706717</v>
       </c>
       <c r="L15">
-        <v>0.6750590889374006</v>
+        <v>0.3290799383310438</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -5330,22 +5330,22 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.298142396999972</v>
+        <v>-0.210818510677892</v>
       </c>
       <c r="J16">
-        <v>0.2596563563704499</v>
+        <v>0.4385780260809998</v>
       </c>
       <c r="K16">
-        <v>-0.3788676152120412</v>
+        <v>-0.259499648053841</v>
       </c>
       <c r="L16">
-        <v>0.2802942824523375</v>
+        <v>0.4690507582155354</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -5368,22 +5368,22 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1987615979999813</v>
+        <v>-0.105409255338946</v>
       </c>
       <c r="J17">
-        <v>0.4523703606773608</v>
+        <v>0.6985353583033387</v>
       </c>
       <c r="K17">
-        <v>-0.3409808536908371</v>
+        <v>-0.1686747712349966</v>
       </c>
       <c r="L17">
-        <v>0.3349456951179903</v>
+        <v>0.6413437507268416</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -5406,22 +5406,22 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.149071198499986</v>
+        <v>0.105409255338946</v>
       </c>
       <c r="J18">
-        <v>0.5730251193553904</v>
+        <v>0.6985353583033387</v>
       </c>
       <c r="K18">
-        <v>0.1641759665918845</v>
+        <v>0.1037998592215364</v>
       </c>
       <c r="L18">
-        <v>0.6503895621649565</v>
+        <v>0.7753684943458543</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -5444,22 +5444,22 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.07537783614444091</v>
+        <v>0.0266500895444513</v>
       </c>
       <c r="J19">
-        <v>0.7773295263554205</v>
+        <v>0.9226081041997291</v>
       </c>
       <c r="K19">
-        <v>0.1076726007868547</v>
+        <v>0.04555068055084343</v>
       </c>
       <c r="L19">
-        <v>0.7671778789420547</v>
+        <v>0.9005643729271482</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5482,22 +5482,22 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.09938079899999065</v>
+        <v>-0.105409255338946</v>
       </c>
       <c r="J20">
-        <v>0.7071142312899612</v>
+        <v>0.6985353583033387</v>
       </c>
       <c r="K20">
-        <v>-0.1262892050706804</v>
+        <v>-0.07784989441615228</v>
       </c>
       <c r="L20">
-        <v>0.7281063840216824</v>
+        <v>0.8307317091592451</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5520,22 +5520,22 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.149071198499986</v>
+        <v>-0.05270462766947299</v>
       </c>
       <c r="J21">
-        <v>0.5730251193553904</v>
+        <v>0.8464505968765906</v>
       </c>
       <c r="K21">
-        <v>-0.2399494896342928</v>
+        <v>-0.1037998592215364</v>
       </c>
       <c r="L21">
-        <v>0.5043017190353258</v>
+        <v>0.7753684943458543</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -5558,22 +5558,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.3975231959999626</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="J22">
-        <v>0.1328549557310538</v>
+        <v>0.2452781168067728</v>
       </c>
       <c r="K22">
-        <v>0.5304146612968577</v>
+        <v>0.3892494720807614</v>
       </c>
       <c r="L22">
-        <v>0.1147392659290222</v>
+        <v>0.2662240730692272</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -5596,22 +5596,22 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.298142396999972</v>
+        <v>0.210818510677892</v>
       </c>
       <c r="J23">
-        <v>0.2596563563704499</v>
+        <v>0.4385780260809998</v>
       </c>
       <c r="K23">
-        <v>0.4041254562261773</v>
+        <v>0.2465246656511489</v>
       </c>
       <c r="L23">
-        <v>0.2467547295422347</v>
+        <v>0.492323476312569</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -5634,22 +5634,22 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2484519974999766</v>
+        <v>-0.1581138830084189</v>
       </c>
       <c r="J24">
-        <v>0.347558036741169</v>
+        <v>0.5612758361345778</v>
       </c>
       <c r="K24">
-        <v>-0.4293832972403134</v>
+        <v>-0.259499648053841</v>
       </c>
       <c r="L24">
-        <v>0.2155824117700313</v>
+        <v>0.4690507582155354</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -5669,25 +5669,25 @@
         <v>16</v>
       </c>
       <c r="F25">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G25">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.31352722326441</v>
+        <v>-0.3244079990200284</v>
       </c>
       <c r="J25">
-        <v>0.1131685336545776</v>
+        <v>0.1020809611324846</v>
       </c>
       <c r="K25">
-        <v>-0.4479914656638877</v>
+        <v>-0.4824165900576836</v>
       </c>
       <c r="L25">
-        <v>0.08182143505121871</v>
+        <v>0.05842088299110668</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -5707,25 +5707,25 @@
         <v>16</v>
       </c>
       <c r="F26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H26">
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.3872983346207417</v>
+        <v>-0.4170959987400364</v>
       </c>
       <c r="J26">
-        <v>0.05036597579032801</v>
+        <v>0.03555790569992093</v>
       </c>
       <c r="K26">
-        <v>-0.5070173682344674</v>
+        <v>-0.5355127556300702</v>
       </c>
       <c r="L26">
-        <v>0.04501930875693567</v>
+        <v>0.03253137976639191</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -5745,25 +5745,25 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H27">
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.08334047874242113</v>
+        <v>0.2047685867790963</v>
       </c>
       <c r="J27">
-        <v>0.6747078413451294</v>
+        <v>0.3037024766857317</v>
       </c>
       <c r="K27">
-        <v>0.08027373462987823</v>
+        <v>0.2170954499333818</v>
       </c>
       <c r="L27">
-        <v>0.7675926515511813</v>
+        <v>0.4192967698838219</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -5783,25 +5783,25 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G28">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H28">
         <v>16</v>
       </c>
       <c r="I28">
-        <v>0.09338863578008762</v>
+        <v>0.08448190755542286</v>
       </c>
       <c r="J28">
-        <v>0.6401498414586226</v>
+        <v>0.6731676659685988</v>
       </c>
       <c r="K28">
-        <v>0.1305442024324843</v>
+        <v>0.1201996807657877</v>
       </c>
       <c r="L28">
-        <v>0.6298840619248964</v>
+        <v>0.6574684200274921</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -5821,25 +5821,25 @@
         <v>16</v>
       </c>
       <c r="F29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G29">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H29">
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.1290994448735805</v>
+        <v>0.009268799972000809</v>
       </c>
       <c r="J29">
-        <v>0.5142199988155506</v>
+        <v>0.9627444106905073</v>
       </c>
       <c r="K29">
-        <v>0.1619428608987702</v>
+        <v>0.01365329971861369</v>
       </c>
       <c r="L29">
-        <v>0.5490376092324329</v>
+        <v>0.9599750222894384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regenerated data from tools
</commit_message>
<xml_diff>
--- a/data/correlation_analysis.xlsx
+++ b/data/correlation_analysis.xlsx
@@ -871,25 +871,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G10">
-        <v>767</v>
+        <v>756</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.03273795352998621</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0.7533555144995171</v>
       </c>
       <c r="K10">
-        <v>0.01048869174464198</v>
+        <v>0.05803647837149319</v>
       </c>
       <c r="L10">
-        <v>0.9423692820963127</v>
+        <v>0.6889076329830681</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -909,25 +909,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G11">
-        <v>767</v>
+        <v>756</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>0.01087930486403344</v>
+        <v>0.03425374379645424</v>
       </c>
       <c r="J11">
-        <v>0.9131676455849755</v>
+        <v>0.7309454575964469</v>
       </c>
       <c r="K11">
-        <v>0.0205721853235722</v>
+        <v>0.0541093585155186</v>
       </c>
       <c r="L11">
-        <v>0.8872356454282179</v>
+        <v>0.70899421576776</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -947,25 +947,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G12">
-        <v>767</v>
+        <v>756</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1529118139971709</v>
+        <v>0.1808614901461585</v>
       </c>
       <c r="J12">
-        <v>0.1229781371552088</v>
+        <v>0.06767175514664597</v>
       </c>
       <c r="K12">
-        <v>0.2338571315807966</v>
+        <v>0.2775590260055978</v>
       </c>
       <c r="L12">
-        <v>0.1021436762030583</v>
+        <v>0.05099390517033404</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1952,25 +1952,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.1719856383383667</v>
+        <v>-0.1127953217534384</v>
       </c>
       <c r="J10">
-        <v>0.1316238040142544</v>
+        <v>0.3246303816462205</v>
       </c>
       <c r="K10">
-        <v>-0.2170916607282444</v>
+        <v>-0.141785465198251</v>
       </c>
       <c r="L10">
-        <v>0.1299324388039652</v>
+        <v>0.3260061663372782</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1990,25 +1990,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.2220671589132321</v>
+        <v>-0.1657843576414015</v>
       </c>
       <c r="J11">
-        <v>0.0416011054294208</v>
+        <v>0.1297187088392248</v>
       </c>
       <c r="K11">
-        <v>-0.3044028033210576</v>
+        <v>-0.228149078380763</v>
       </c>
       <c r="L11">
-        <v>0.03161022555609473</v>
+        <v>0.1110368177920856</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2028,25 +2028,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.2554933792020658</v>
+        <v>0.2135201189924139</v>
       </c>
       <c r="J12">
-        <v>0.01830915752272128</v>
+        <v>0.04951827186158275</v>
       </c>
       <c r="K12">
-        <v>0.3206647291565351</v>
+        <v>0.2585375793536707</v>
       </c>
       <c r="L12">
-        <v>0.02318249883445114</v>
+        <v>0.06985387930445178</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3084,22 +3084,22 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>0.08712167584961492</v>
+        <v>0.08993343971074573</v>
       </c>
       <c r="J10">
-        <v>0.4083766752312095</v>
+        <v>0.3939555332313259</v>
       </c>
       <c r="K10">
-        <v>0.1227687641955272</v>
+        <v>0.1261078291007821</v>
       </c>
       <c r="L10">
-        <v>0.3956759834281137</v>
+        <v>0.3828516225378101</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3122,22 +3122,22 @@
         <v>40</v>
       </c>
       <c r="G11">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>0.07462967377124524</v>
+        <v>0.07727463833790227</v>
       </c>
       <c r="J11">
-        <v>0.4588124610579571</v>
+        <v>0.4435614692500816</v>
       </c>
       <c r="K11">
-        <v>0.09255821810809323</v>
+        <v>0.09527592158164427</v>
       </c>
       <c r="L11">
-        <v>0.5226237277667096</v>
+        <v>0.5104337983014946</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3160,22 +3160,22 @@
         <v>40</v>
       </c>
       <c r="G12">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.0648462728029752</v>
+        <v>0.06408768791953229</v>
       </c>
       <c r="J12">
-        <v>0.5171200381290717</v>
+        <v>0.5225032783206667</v>
       </c>
       <c r="K12">
-        <v>0.08638478532010939</v>
+        <v>0.08576989054836207</v>
       </c>
       <c r="L12">
-        <v>0.5508414269428876</v>
+        <v>0.5536912247004897</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3846,8 +3846,8 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4114,25 +4114,25 @@
         <v>50</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>0.01421997815784012</v>
+        <v>-0.07463933708620761</v>
       </c>
       <c r="J10">
-        <v>0.9088173646349219</v>
+        <v>0.547733910068501</v>
       </c>
       <c r="K10">
-        <v>0.01636148293791983</v>
+        <v>-0.08587989564247843</v>
       </c>
       <c r="L10">
-        <v>0.9102093962355748</v>
+        <v>0.5531808807861933</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4152,25 +4152,25 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>0.001918117792161453</v>
+        <v>-0.02642855544759036</v>
       </c>
       <c r="J11">
-        <v>0.9870933347767511</v>
+        <v>0.8236209225496525</v>
       </c>
       <c r="K11">
-        <v>0.002310973073108823</v>
+        <v>-0.03184146471615851</v>
       </c>
       <c r="L11">
-        <v>0.9872920353883015</v>
+        <v>0.8262496889100787</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4190,25 +4190,25 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.2419047619047619</v>
+        <v>0.2391168558431198</v>
       </c>
       <c r="J12">
-        <v>0.04002718189621234</v>
+        <v>0.04237662250330112</v>
       </c>
       <c r="K12">
-        <v>0.2933526131391836</v>
+        <v>0.2899717804431688</v>
       </c>
       <c r="L12">
-        <v>0.03867934687031339</v>
+        <v>0.04108542769241475</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4736,7 +4736,7 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5102,22 +5102,22 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.2254320318923924</v>
+        <v>-0.05307283274919742</v>
       </c>
       <c r="J10">
-        <v>0.03750206210014283</v>
+        <v>0.6242364838392908</v>
       </c>
       <c r="K10">
-        <v>-0.2757884146130811</v>
+        <v>-0.07261500585855338</v>
       </c>
       <c r="L10">
-        <v>0.0525532974249969</v>
+        <v>0.6162718579812509</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5140,22 +5140,22 @@
         <v>40</v>
       </c>
       <c r="G11">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.1794340300657417</v>
+        <v>-0.01582502127477728</v>
       </c>
       <c r="J11">
-        <v>0.08321105252268295</v>
+        <v>0.8785433534210723</v>
       </c>
       <c r="K11">
-        <v>-0.2382169979796553</v>
+        <v>-0.02058248424779236</v>
       </c>
       <c r="L11">
-        <v>0.09572883636182701</v>
+        <v>0.8871795586689608</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5178,22 +5178,22 @@
         <v>40</v>
       </c>
       <c r="G12">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12">
-        <v>0.1869191683862415</v>
+        <v>0.2453259787285023</v>
       </c>
       <c r="J12">
-        <v>0.06934431565042681</v>
+        <v>0.01711709386488932</v>
       </c>
       <c r="K12">
-        <v>0.2610882725528407</v>
+        <v>0.340250349648349</v>
       </c>
       <c r="L12">
-        <v>0.06704286140152567</v>
+        <v>0.01561890085779964</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>